<commit_message>
Implemented choice- and level-dependent condition durations Implemented effects that change spell and activity condition durations Implemented activity spellcasts with pre-defined choice
</commit_message>
<xml_diff>
--- a/work assets/activities.xlsx
+++ b/work assets/activities.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23801"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23901"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/eb76e5660c890129/Personal/Projects/Design/Patherpoint/patherpoint/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/eb76e5660c890129/Personal/Projects/Design/PECS/PECS/work assets/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="617" documentId="13_ncr:40009_{E3EB266C-7612-416D-8781-7A2BED99FA57}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{AED4E7A3-AA7A-4967-AB5B-EDB7452BC0EC}"/>
+  <xr:revisionPtr revIDLastSave="619" documentId="13_ncr:40009_{E3EB266C-7612-416D-8781-7A2BED99FA57}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{4004FD57-9FFF-47DB-A752-68EC7A4EF4F2}"/>
   <bookViews>
-    <workbookView xWindow="368" yWindow="968" windowWidth="19050" windowHeight="11512" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="77040" windowHeight="21240" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="activities" sheetId="1" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2707" uniqueCount="1161">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5289" uniqueCount="1161">
   <si>
     <t>name</t>
   </si>
@@ -3458,9 +3458,6 @@
 &lt;strong&gt;White&lt;/strong&gt; 30-foot cone, 10d6 cold.</t>
   </si>
   <si>
-    <t>After using the breath weapon, roll 1d4 and change the duration of the cooldown condition to the result.</t>
-  </si>
-  <si>
     <t>Shroud of Flame</t>
   </si>
   <si>
@@ -3643,6 +3640,9 @@
   </si>
   <si>
     <t>gainConditions/0/value</t>
+  </si>
+  <si>
+    <t>Roll 1d4 and choose the appropriate duration for the cooldown condition.</t>
   </si>
 </sst>
 </file>
@@ -4556,9 +4556,9 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:93" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:93" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -4839,15 +4839,15 @@
         <v>45</v>
       </c>
     </row>
-    <row r="2" spans="1:93" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:93" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>1139</v>
+        <v>1138</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>71</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>1142</v>
+        <v>1141</v>
       </c>
       <c r="D2" s="2" t="s">
         <v>696</v>
@@ -4861,7 +4861,7 @@
       <c r="I2" s="2"/>
       <c r="J2" s="2"/>
       <c r="K2" s="1" t="s">
-        <v>1141</v>
+        <v>1140</v>
       </c>
       <c r="L2" s="1" t="s">
         <v>697</v>
@@ -4875,7 +4875,7 @@
       <c r="S2" s="1"/>
       <c r="T2" s="1"/>
       <c r="U2" s="1" t="s">
-        <v>1140</v>
+        <v>1139</v>
       </c>
       <c r="V2" s="1"/>
       <c r="W2" s="3"/>
@@ -4950,15 +4950,15 @@
       <c r="CN2" s="1"/>
       <c r="CO2" s="1"/>
     </row>
-    <row r="3" spans="1:93" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:93" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>1144</v>
+        <v>1143</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>51</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>1146</v>
+        <v>1145</v>
       </c>
       <c r="D3" s="2" t="s">
         <v>343</v>
@@ -4982,7 +4982,7 @@
       <c r="S3" s="1"/>
       <c r="T3" s="1"/>
       <c r="U3" s="1" t="s">
-        <v>1145</v>
+        <v>1144</v>
       </c>
       <c r="V3" s="1"/>
       <c r="W3" s="3"/>
@@ -5057,9 +5057,9 @@
       <c r="CN3" s="1"/>
       <c r="CO3" s="1"/>
     </row>
-    <row r="4" spans="1:93" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:93" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>1147</v>
+        <v>1146</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>51</v>
@@ -5091,7 +5091,7 @@
       <c r="S4" s="1"/>
       <c r="T4" s="1"/>
       <c r="U4" s="1" t="s">
-        <v>1148</v>
+        <v>1147</v>
       </c>
       <c r="V4" s="1"/>
       <c r="W4" s="3"/>
@@ -5106,10 +5106,10 @@
         <v>1</v>
       </c>
       <c r="AF4" s="4" t="s">
-        <v>1147</v>
+        <v>1146</v>
       </c>
       <c r="AG4" s="4" t="s">
-        <v>1147</v>
+        <v>1146</v>
       </c>
       <c r="AH4" s="7"/>
       <c r="AI4" s="4"/>
@@ -5172,15 +5172,15 @@
       <c r="CN4" s="1"/>
       <c r="CO4" s="1"/>
     </row>
-    <row r="5" spans="1:93" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:93" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>1149</v>
+        <v>1148</v>
       </c>
       <c r="B5" s="1" t="s">
         <v>130</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>1152</v>
+        <v>1151</v>
       </c>
       <c r="D5" s="2" t="s">
         <v>195</v>
@@ -5195,7 +5195,7 @@
       <c r="J5" s="2"/>
       <c r="K5" s="1"/>
       <c r="L5" s="1" t="s">
-        <v>1150</v>
+        <v>1149</v>
       </c>
       <c r="M5" s="1"/>
       <c r="N5" s="1"/>
@@ -5210,7 +5210,7 @@
       <c r="S5" s="1"/>
       <c r="T5" s="1"/>
       <c r="U5" s="1" t="s">
-        <v>1151</v>
+        <v>1150</v>
       </c>
       <c r="V5" s="1"/>
       <c r="W5" s="3"/>
@@ -5225,10 +5225,10 @@
         <v>1</v>
       </c>
       <c r="AF5" s="4" t="s">
-        <v>1147</v>
+        <v>1146</v>
       </c>
       <c r="AG5" s="4" t="s">
-        <v>1147</v>
+        <v>1146</v>
       </c>
       <c r="AH5" s="7"/>
       <c r="AI5" s="4"/>
@@ -5307,20 +5307,20 @@
   <dimension ref="A1:MG94"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="ME2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="LM2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="MG17" sqref="MG17"/>
+      <selection pane="bottomRight" activeCell="LY3" sqref="LY3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.1328125" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="37.59765625" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="345" width="27.3984375" style="1" customWidth="1"/>
-    <col min="346" max="16384" width="9.1328125" style="1"/>
+    <col min="1" max="1" width="37.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="345" width="27.42578125" style="1" customWidth="1"/>
+    <col min="346" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:345" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:345" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -5988,7 +5988,7 @@
         <v>698</v>
       </c>
       <c r="HO1" t="s">
-        <v>1154</v>
+        <v>1153</v>
       </c>
       <c r="HP1" t="s">
         <v>701</v>
@@ -6303,61 +6303,61 @@
         <v>1099</v>
       </c>
       <c r="LP1" t="s">
-        <v>1106</v>
+        <v>1105</v>
       </c>
       <c r="LQ1" t="s">
-        <v>1103</v>
+        <v>1102</v>
       </c>
       <c r="LR1" t="s">
-        <v>1105</v>
+        <v>1104</v>
       </c>
       <c r="LS1" t="s">
-        <v>1113</v>
+        <v>1112</v>
       </c>
       <c r="LT1" t="s">
-        <v>1115</v>
+        <v>1114</v>
       </c>
       <c r="LU1" t="s">
-        <v>1117</v>
+        <v>1116</v>
       </c>
       <c r="LV1" t="s">
+        <v>1120</v>
+      </c>
+      <c r="LW1" t="s">
         <v>1121</v>
       </c>
-      <c r="LW1" t="s">
-        <v>1122</v>
-      </c>
       <c r="LX1" t="s">
+        <v>1123</v>
+      </c>
+      <c r="LY1" t="s">
         <v>1124</v>
       </c>
-      <c r="LY1" t="s">
+      <c r="LZ1" t="s">
+        <v>1126</v>
+      </c>
+      <c r="MA1" t="s">
         <v>1125</v>
       </c>
-      <c r="LZ1" t="s">
-        <v>1127</v>
-      </c>
-      <c r="MA1" t="s">
-        <v>1126</v>
-      </c>
       <c r="MB1" t="s">
-        <v>1135</v>
+        <v>1134</v>
       </c>
       <c r="MC1" t="s">
-        <v>1139</v>
+        <v>1138</v>
       </c>
       <c r="MD1" t="s">
-        <v>1144</v>
+        <v>1143</v>
       </c>
       <c r="ME1" t="s">
-        <v>1147</v>
+        <v>1146</v>
       </c>
       <c r="MF1" t="s">
-        <v>1149</v>
+        <v>1148</v>
       </c>
       <c r="MG1" t="s">
-        <v>1156</v>
+        <v>1155</v>
       </c>
     </row>
-    <row r="2" spans="1:345" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:345" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
@@ -7382,7 +7382,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="3" spans="1:345" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:345" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>20</v>
       </c>
@@ -7531,7 +7531,7 @@
         <v>618</v>
       </c>
       <c r="HM3" s="1" t="s">
-        <v>1143</v>
+        <v>1142</v>
       </c>
       <c r="HQ3" s="1" t="s">
         <v>706</v>
@@ -7570,28 +7570,28 @@
         <v>1084</v>
       </c>
       <c r="LH3" s="1" t="s">
-        <v>1102</v>
+        <v>1160</v>
       </c>
       <c r="LM3" s="1" t="s">
         <v>1077</v>
       </c>
       <c r="LT3" s="1" t="s">
-        <v>1138</v>
+        <v>1137</v>
       </c>
       <c r="LY3" s="1" t="s">
-        <v>1133</v>
+        <v>1132</v>
       </c>
       <c r="MC3" s="1" t="s">
-        <v>1142</v>
+        <v>1141</v>
       </c>
       <c r="MD3" s="1" t="s">
-        <v>1146</v>
+        <v>1145</v>
       </c>
       <c r="MF3" s="1" t="s">
-        <v>1152</v>
+        <v>1151</v>
       </c>
     </row>
-    <row r="4" spans="1:345" s="2" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:345" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>3</v>
       </c>
@@ -8523,7 +8523,7 @@
         <v>342</v>
       </c>
       <c r="LQ4" s="2" t="s">
-        <v>1104</v>
+        <v>1103</v>
       </c>
       <c r="LR4" s="2" t="s">
         <v>625</v>
@@ -8568,7 +8568,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="5" spans="1:345" s="2" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:345" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>4</v>
       </c>
@@ -9239,7 +9239,7 @@
         <v>344</v>
       </c>
     </row>
-    <row r="6" spans="1:345" s="2" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:345" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>11</v>
       </c>
@@ -9604,7 +9604,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="7" spans="1:345" s="2" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:345" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>12</v>
       </c>
@@ -9855,7 +9855,7 @@
         <v>343</v>
       </c>
     </row>
-    <row r="8" spans="1:345" s="2" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:345" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
         <v>13</v>
       </c>
@@ -10001,7 +10001,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="9" spans="1:345" s="2" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:345" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
         <v>34</v>
       </c>
@@ -10027,7 +10027,7 @@
         <v>315</v>
       </c>
     </row>
-    <row r="10" spans="1:345" s="2" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:345" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
         <v>37</v>
       </c>
@@ -10041,7 +10041,7 @@
         <v>992</v>
       </c>
     </row>
-    <row r="11" spans="1:345" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:345" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>6</v>
       </c>
@@ -10259,7 +10259,7 @@
         <v>683</v>
       </c>
       <c r="HO11" s="1" t="s">
-        <v>1155</v>
+        <v>1154</v>
       </c>
       <c r="HQ11" s="1" t="s">
         <v>705</v>
@@ -10334,16 +10334,16 @@
         <v>1014</v>
       </c>
       <c r="LP11" s="1" t="s">
-        <v>1108</v>
+        <v>1107</v>
       </c>
       <c r="LU11" s="1" t="s">
-        <v>1118</v>
+        <v>1117</v>
       </c>
       <c r="MC11" s="1" t="s">
-        <v>1141</v>
+        <v>1140</v>
       </c>
     </row>
-    <row r="12" spans="1:345" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:345" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>10</v>
       </c>
@@ -10552,16 +10552,16 @@
         <v>1023</v>
       </c>
       <c r="LP12" s="1" t="s">
-        <v>1107</v>
+        <v>1106</v>
       </c>
       <c r="MC12" s="1" t="s">
         <v>697</v>
       </c>
       <c r="MF12" s="1" t="s">
-        <v>1150</v>
+        <v>1149</v>
       </c>
     </row>
-    <row r="13" spans="1:345" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:345" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>5</v>
       </c>
@@ -10740,7 +10740,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:345" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:345" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>1085</v>
       </c>
@@ -10748,7 +10748,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:345" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:345" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>48</v>
       </c>
@@ -10759,7 +10759,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:345" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:345" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
         <v>35</v>
       </c>
@@ -10767,7 +10767,7 @@
         <v>310</v>
       </c>
     </row>
-    <row r="17" spans="1:345" x14ac:dyDescent="0.45">
+    <row r="17" spans="1:345" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
         <v>18</v>
       </c>
@@ -10881,7 +10881,7 @@
         <v>809</v>
       </c>
     </row>
-    <row r="18" spans="1:345" x14ac:dyDescent="0.45">
+    <row r="18" spans="1:345" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
         <v>19</v>
       </c>
@@ -11003,7 +11003,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="19" spans="1:345" x14ac:dyDescent="0.45">
+    <row r="19" spans="1:345" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
         <v>36</v>
       </c>
@@ -11014,7 +11014,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="20" spans="1:345" x14ac:dyDescent="0.45">
+    <row r="20" spans="1:345" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
         <v>21</v>
       </c>
@@ -11061,7 +11061,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="21" spans="1:345" x14ac:dyDescent="0.45">
+    <row r="21" spans="1:345" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
         <v>2</v>
       </c>
@@ -11729,7 +11729,7 @@
         <v>699</v>
       </c>
       <c r="HO21" s="1" t="s">
-        <v>1153</v>
+        <v>1152</v>
       </c>
       <c r="HP21" s="1" t="s">
         <v>702</v>
@@ -12044,61 +12044,61 @@
         <v>1100</v>
       </c>
       <c r="LP21" s="1" t="s">
-        <v>1109</v>
+        <v>1108</v>
       </c>
       <c r="LQ21" s="1" t="s">
+        <v>1110</v>
+      </c>
+      <c r="LR21" s="1" t="s">
         <v>1111</v>
       </c>
-      <c r="LR21" s="1" t="s">
-        <v>1112</v>
-      </c>
       <c r="LS21" s="1" t="s">
-        <v>1114</v>
+        <v>1113</v>
       </c>
       <c r="LT21" s="1" t="s">
-        <v>1116</v>
+        <v>1115</v>
       </c>
       <c r="LU21" s="1" t="s">
-        <v>1137</v>
+        <v>1136</v>
       </c>
       <c r="LV21" s="1" t="s">
-        <v>1119</v>
+        <v>1118</v>
       </c>
       <c r="LW21" s="1" t="s">
-        <v>1123</v>
+        <v>1122</v>
       </c>
       <c r="LX21" s="1" t="s">
-        <v>1134</v>
+        <v>1133</v>
       </c>
       <c r="LY21" s="1" t="s">
+        <v>1127</v>
+      </c>
+      <c r="LZ21" s="1" t="s">
         <v>1128</v>
       </c>
-      <c r="LZ21" s="1" t="s">
-        <v>1129</v>
-      </c>
       <c r="MA21" s="1" t="s">
-        <v>1132</v>
+        <v>1131</v>
       </c>
       <c r="MB21" s="1" t="s">
-        <v>1136</v>
+        <v>1135</v>
       </c>
       <c r="MC21" s="1" t="s">
-        <v>1140</v>
+        <v>1139</v>
       </c>
       <c r="MD21" s="1" t="s">
-        <v>1145</v>
+        <v>1144</v>
       </c>
       <c r="ME21" s="1" t="s">
-        <v>1148</v>
+        <v>1147</v>
       </c>
       <c r="MF21" s="1" t="s">
-        <v>1151</v>
+        <v>1150</v>
       </c>
       <c r="MG21" s="1" t="s">
-        <v>1157</v>
+        <v>1156</v>
       </c>
     </row>
-    <row r="22" spans="1:345" x14ac:dyDescent="0.45">
+    <row r="22" spans="1:345" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
         <v>38</v>
       </c>
@@ -12115,7 +12115,7 @@
         <v>789</v>
       </c>
     </row>
-    <row r="23" spans="1:345" s="3" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="23" spans="1:345" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A23" s="3" t="s">
         <v>14</v>
       </c>
@@ -12174,7 +12174,7 @@
         <v>854</v>
       </c>
     </row>
-    <row r="24" spans="1:345" s="3" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="24" spans="1:345" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A24" s="3" t="s">
         <v>15</v>
       </c>
@@ -12242,7 +12242,7 @@
         <v>855</v>
       </c>
     </row>
-    <row r="25" spans="1:345" s="3" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="25" spans="1:345" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A25" s="3" t="s">
         <v>16</v>
       </c>
@@ -12316,7 +12316,7 @@
         <v>772</v>
       </c>
     </row>
-    <row r="26" spans="1:345" s="3" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="26" spans="1:345" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A26" s="3" t="s">
         <v>17</v>
       </c>
@@ -12375,7 +12375,7 @@
         <v>856</v>
       </c>
     </row>
-    <row r="27" spans="1:345" s="7" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="27" spans="1:345" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A27" s="7" t="s">
         <v>25</v>
       </c>
@@ -12392,7 +12392,7 @@
         <v>1082</v>
       </c>
     </row>
-    <row r="28" spans="1:345" s="4" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="28" spans="1:345" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A28" s="4" t="s">
         <v>22</v>
       </c>
@@ -12403,7 +12403,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="29" spans="1:345" s="4" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="29" spans="1:345" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A29" s="4" t="s">
         <v>1034</v>
       </c>
@@ -12411,7 +12411,7 @@
         <v>1025</v>
       </c>
     </row>
-    <row r="30" spans="1:345" s="4" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="30" spans="1:345" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A30" s="4" t="s">
         <v>1086</v>
       </c>
@@ -12419,7 +12419,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="31" spans="1:345" s="4" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="31" spans="1:345" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A31" s="4" t="s">
         <v>7</v>
       </c>
@@ -12703,7 +12703,7 @@
         <v>100</v>
       </c>
       <c r="LH31" s="4">
-        <v>40</v>
+        <v>-5</v>
       </c>
       <c r="LI31" s="4">
         <v>-1</v>
@@ -12736,7 +12736,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="32" spans="1:345" s="4" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="32" spans="1:345" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A32" s="4" t="s">
         <v>8</v>
       </c>
@@ -12918,7 +12918,7 @@
         <v>666</v>
       </c>
       <c r="HO32" s="4" t="s">
-        <v>1154</v>
+        <v>1153</v>
       </c>
       <c r="HQ32" s="4" t="s">
         <v>703</v>
@@ -13053,31 +13053,31 @@
         <v>1099</v>
       </c>
       <c r="LQ32" s="4" t="s">
-        <v>1103</v>
+        <v>1102</v>
       </c>
       <c r="LU32" s="4" t="s">
-        <v>1117</v>
+        <v>1116</v>
       </c>
       <c r="LV32" s="4" t="s">
-        <v>1120</v>
+        <v>1119</v>
       </c>
       <c r="LX32" s="4" t="s">
-        <v>1124</v>
+        <v>1123</v>
       </c>
       <c r="LZ32" s="4" t="s">
-        <v>1131</v>
+        <v>1130</v>
       </c>
       <c r="MA32" s="4" t="s">
-        <v>1126</v>
+        <v>1125</v>
       </c>
       <c r="ME32" s="4" t="s">
-        <v>1147</v>
+        <v>1146</v>
       </c>
       <c r="MG32" s="4" t="s">
-        <v>1158</v>
+        <v>1157</v>
       </c>
     </row>
-    <row r="33" spans="1:345" s="4" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="33" spans="1:345" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A33" s="4" t="s">
         <v>9</v>
       </c>
@@ -13253,7 +13253,7 @@
         <v>666</v>
       </c>
       <c r="HO33" s="4" t="s">
-        <v>1154</v>
+        <v>1153</v>
       </c>
       <c r="HQ33" s="4" t="s">
         <v>703</v>
@@ -13388,39 +13388,39 @@
         <v>1099</v>
       </c>
       <c r="LQ33" s="4" t="s">
-        <v>1103</v>
+        <v>1102</v>
       </c>
       <c r="LU33" s="4" t="s">
-        <v>1117</v>
+        <v>1116</v>
       </c>
       <c r="LV33" s="4" t="s">
-        <v>1121</v>
+        <v>1120</v>
       </c>
       <c r="LX33" s="4" t="s">
+        <v>1123</v>
+      </c>
+      <c r="LZ33" s="4" t="s">
         <v>1124</v>
       </c>
-      <c r="LZ33" s="4" t="s">
+      <c r="MA33" s="4" t="s">
         <v>1125</v>
       </c>
-      <c r="MA33" s="4" t="s">
-        <v>1126</v>
-      </c>
       <c r="ME33" s="4" t="s">
-        <v>1147</v>
+        <v>1146</v>
       </c>
       <c r="MG33" s="4" t="s">
+        <v>1158</v>
+      </c>
+    </row>
+    <row r="34" spans="1:345" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A34" s="4" t="s">
         <v>1159</v>
-      </c>
-    </row>
-    <row r="34" spans="1:345" s="4" customFormat="1" x14ac:dyDescent="0.45">
-      <c r="A34" s="4" t="s">
-        <v>1160</v>
       </c>
       <c r="MG34" s="4">
         <v>1</v>
       </c>
     </row>
-    <row r="35" spans="1:345" s="7" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="35" spans="1:345" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A35" s="7" t="s">
         <v>29</v>
       </c>
@@ -13431,7 +13431,7 @@
         <v>1037</v>
       </c>
     </row>
-    <row r="36" spans="1:345" s="4" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="36" spans="1:345" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A36" s="4" t="s">
         <v>1035</v>
       </c>
@@ -13439,7 +13439,7 @@
         <v>1026</v>
       </c>
     </row>
-    <row r="37" spans="1:345" s="4" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="37" spans="1:345" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A37" s="4" t="s">
         <v>1094</v>
       </c>
@@ -13447,7 +13447,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="38" spans="1:345" s="4" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="38" spans="1:345" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A38" s="4" t="s">
         <v>26</v>
       </c>
@@ -13455,7 +13455,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="39" spans="1:345" s="4" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="39" spans="1:345" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A39" s="4" t="s">
         <v>27</v>
       </c>
@@ -13472,7 +13472,7 @@
         <v>945</v>
       </c>
     </row>
-    <row r="40" spans="1:345" s="4" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="40" spans="1:345" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A40" s="4" t="s">
         <v>28</v>
       </c>
@@ -13489,7 +13489,7 @@
         <v>945</v>
       </c>
     </row>
-    <row r="41" spans="1:345" s="4" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="41" spans="1:345" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A41" s="4" t="s">
         <v>47</v>
       </c>
@@ -13497,7 +13497,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="42" spans="1:345" s="7" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="42" spans="1:345" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A42" s="7" t="s">
         <v>33</v>
       </c>
@@ -13508,7 +13508,7 @@
         <v>1036</v>
       </c>
     </row>
-    <row r="43" spans="1:345" s="4" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="43" spans="1:345" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A43" s="4" t="s">
         <v>1039</v>
       </c>
@@ -13516,7 +13516,7 @@
         <v>1027</v>
       </c>
     </row>
-    <row r="44" spans="1:345" s="4" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="44" spans="1:345" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A44" s="4" t="s">
         <v>1093</v>
       </c>
@@ -13524,7 +13524,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="45" spans="1:345" s="4" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="45" spans="1:345" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A45" s="4" t="s">
         <v>30</v>
       </c>
@@ -13532,7 +13532,7 @@
         <v>500</v>
       </c>
     </row>
-    <row r="46" spans="1:345" s="4" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="46" spans="1:345" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A46" s="4" t="s">
         <v>31</v>
       </c>
@@ -13543,7 +13543,7 @@
         <v>945</v>
       </c>
     </row>
-    <row r="47" spans="1:345" s="4" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="47" spans="1:345" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A47" s="4" t="s">
         <v>32</v>
       </c>
@@ -13554,7 +13554,7 @@
         <v>945</v>
       </c>
     </row>
-    <row r="48" spans="1:345" s="7" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="48" spans="1:345" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A48" s="7" t="s">
         <v>1040</v>
       </c>
@@ -13562,7 +13562,7 @@
         <v>1070</v>
       </c>
     </row>
-    <row r="49" spans="1:305" s="4" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="49" spans="1:305" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A49" s="4" t="s">
         <v>1041</v>
       </c>
@@ -13570,7 +13570,7 @@
         <v>1029</v>
       </c>
     </row>
-    <row r="50" spans="1:305" s="4" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="50" spans="1:305" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A50" s="4" t="s">
         <v>1092</v>
       </c>
@@ -13578,12 +13578,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="51" spans="1:305" s="4" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="51" spans="1:305" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A51" s="4" t="s">
         <v>1042</v>
       </c>
     </row>
-    <row r="52" spans="1:305" s="4" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="52" spans="1:305" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A52" s="4" t="s">
         <v>1043</v>
       </c>
@@ -13591,7 +13591,7 @@
         <v>945</v>
       </c>
     </row>
-    <row r="53" spans="1:305" s="4" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="53" spans="1:305" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A53" s="4" t="s">
         <v>1044</v>
       </c>
@@ -13599,7 +13599,7 @@
         <v>945</v>
       </c>
     </row>
-    <row r="54" spans="1:305" s="7" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="54" spans="1:305" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A54" s="7" t="s">
         <v>1045</v>
       </c>
@@ -13607,7 +13607,7 @@
         <v>1071</v>
       </c>
     </row>
-    <row r="55" spans="1:305" s="4" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="55" spans="1:305" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A55" s="4" t="s">
         <v>1046</v>
       </c>
@@ -13615,7 +13615,7 @@
         <v>1030</v>
       </c>
     </row>
-    <row r="56" spans="1:305" s="4" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="56" spans="1:305" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A56" s="4" t="s">
         <v>1091</v>
       </c>
@@ -13623,12 +13623,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="57" spans="1:305" s="4" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="57" spans="1:305" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A57" s="4" t="s">
         <v>1047</v>
       </c>
     </row>
-    <row r="58" spans="1:305" s="4" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="58" spans="1:305" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A58" s="4" t="s">
         <v>1048</v>
       </c>
@@ -13636,7 +13636,7 @@
         <v>945</v>
       </c>
     </row>
-    <row r="59" spans="1:305" s="4" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="59" spans="1:305" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A59" s="4" t="s">
         <v>1049</v>
       </c>
@@ -13644,7 +13644,7 @@
         <v>945</v>
       </c>
     </row>
-    <row r="60" spans="1:305" s="7" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="60" spans="1:305" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A60" s="7" t="s">
         <v>1050</v>
       </c>
@@ -13652,7 +13652,7 @@
         <v>1072</v>
       </c>
     </row>
-    <row r="61" spans="1:305" s="4" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="61" spans="1:305" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A61" s="4" t="s">
         <v>1051</v>
       </c>
@@ -13660,7 +13660,7 @@
         <v>1031</v>
       </c>
     </row>
-    <row r="62" spans="1:305" s="4" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="62" spans="1:305" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A62" s="4" t="s">
         <v>1090</v>
       </c>
@@ -13668,12 +13668,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="63" spans="1:305" s="4" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="63" spans="1:305" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A63" s="4" t="s">
         <v>1052</v>
       </c>
     </row>
-    <row r="64" spans="1:305" s="4" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="64" spans="1:305" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A64" s="4" t="s">
         <v>1053</v>
       </c>
@@ -13681,7 +13681,7 @@
         <v>945</v>
       </c>
     </row>
-    <row r="65" spans="1:305" s="4" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="65" spans="1:305" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A65" s="4" t="s">
         <v>1054</v>
       </c>
@@ -13689,7 +13689,7 @@
         <v>945</v>
       </c>
     </row>
-    <row r="66" spans="1:305" s="7" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="66" spans="1:305" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A66" s="7" t="s">
         <v>1055</v>
       </c>
@@ -13697,7 +13697,7 @@
         <v>1073</v>
       </c>
     </row>
-    <row r="67" spans="1:305" s="4" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="67" spans="1:305" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A67" s="4" t="s">
         <v>1056</v>
       </c>
@@ -13705,7 +13705,7 @@
         <v>1032</v>
       </c>
     </row>
-    <row r="68" spans="1:305" s="4" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="68" spans="1:305" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A68" s="4" t="s">
         <v>1089</v>
       </c>
@@ -13713,12 +13713,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="69" spans="1:305" s="4" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="69" spans="1:305" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A69" s="4" t="s">
         <v>1057</v>
       </c>
     </row>
-    <row r="70" spans="1:305" s="4" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="70" spans="1:305" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A70" s="4" t="s">
         <v>1058</v>
       </c>
@@ -13726,7 +13726,7 @@
         <v>945</v>
       </c>
     </row>
-    <row r="71" spans="1:305" s="4" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="71" spans="1:305" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A71" s="4" t="s">
         <v>1059</v>
       </c>
@@ -13734,7 +13734,7 @@
         <v>945</v>
       </c>
     </row>
-    <row r="72" spans="1:305" s="7" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="72" spans="1:305" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A72" s="7" t="s">
         <v>1060</v>
       </c>
@@ -13742,7 +13742,7 @@
         <v>1074</v>
       </c>
     </row>
-    <row r="73" spans="1:305" s="4" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="73" spans="1:305" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A73" s="4" t="s">
         <v>1061</v>
       </c>
@@ -13750,7 +13750,7 @@
         <v>1033</v>
       </c>
     </row>
-    <row r="74" spans="1:305" s="4" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="74" spans="1:305" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A74" s="4" t="s">
         <v>1088</v>
       </c>
@@ -13758,12 +13758,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="75" spans="1:305" s="4" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="75" spans="1:305" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A75" s="4" t="s">
         <v>1062</v>
       </c>
     </row>
-    <row r="76" spans="1:305" s="4" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="76" spans="1:305" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A76" s="4" t="s">
         <v>1063</v>
       </c>
@@ -13771,7 +13771,7 @@
         <v>945</v>
       </c>
     </row>
-    <row r="77" spans="1:305" s="4" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="77" spans="1:305" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A77" s="4" t="s">
         <v>1064</v>
       </c>
@@ -13779,7 +13779,7 @@
         <v>945</v>
       </c>
     </row>
-    <row r="78" spans="1:305" s="7" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="78" spans="1:305" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A78" s="7" t="s">
         <v>1065</v>
       </c>
@@ -13787,7 +13787,7 @@
         <v>1075</v>
       </c>
     </row>
-    <row r="79" spans="1:305" s="4" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="79" spans="1:305" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A79" s="4" t="s">
         <v>1066</v>
       </c>
@@ -13795,7 +13795,7 @@
         <v>1028</v>
       </c>
     </row>
-    <row r="80" spans="1:305" s="4" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="80" spans="1:305" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A80" s="4" t="s">
         <v>1087</v>
       </c>
@@ -13803,12 +13803,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="81" spans="1:338" s="4" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="81" spans="1:338" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A81" s="4" t="s">
         <v>1067</v>
       </c>
     </row>
-    <row r="82" spans="1:338" s="4" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="82" spans="1:338" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A82" s="4" t="s">
         <v>1068</v>
       </c>
@@ -13816,7 +13816,7 @@
         <v>945</v>
       </c>
     </row>
-    <row r="83" spans="1:338" s="4" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="83" spans="1:338" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A83" s="4" t="s">
         <v>1069</v>
       </c>
@@ -13824,7 +13824,7 @@
         <v>945</v>
       </c>
     </row>
-    <row r="84" spans="1:338" s="5" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="84" spans="1:338" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A84" s="5" t="s">
         <v>23</v>
       </c>
@@ -13853,7 +13853,7 @@
         <v>289</v>
       </c>
     </row>
-    <row r="85" spans="1:338" s="5" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="85" spans="1:338" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A85" s="5" t="s">
         <v>24</v>
       </c>
@@ -13882,7 +13882,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="86" spans="1:338" s="8" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="86" spans="1:338" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A86" s="8" t="s">
         <v>41</v>
       </c>
@@ -13899,7 +13899,7 @@
         <v>718</v>
       </c>
     </row>
-    <row r="87" spans="1:338" s="6" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="87" spans="1:338" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A87" s="6" t="s">
         <v>40</v>
       </c>
@@ -13916,7 +13916,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="88" spans="1:338" s="6" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="88" spans="1:338" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A88" s="6" t="s">
         <v>39</v>
       </c>
@@ -13930,10 +13930,10 @@
         <v>1022</v>
       </c>
       <c r="LP88" s="6" t="s">
-        <v>1110</v>
+        <v>1109</v>
       </c>
     </row>
-    <row r="89" spans="1:338" s="8" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="89" spans="1:338" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A89" s="8" t="s">
         <v>44</v>
       </c>
@@ -13941,7 +13941,7 @@
         <v>718</v>
       </c>
     </row>
-    <row r="90" spans="1:338" s="6" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="90" spans="1:338" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A90" s="6" t="s">
         <v>43</v>
       </c>
@@ -13949,7 +13949,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="91" spans="1:338" s="6" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="91" spans="1:338" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A91" s="6" t="s">
         <v>42</v>
       </c>
@@ -13957,7 +13957,7 @@
         <v>717</v>
       </c>
     </row>
-    <row r="92" spans="1:338" x14ac:dyDescent="0.45">
+    <row r="92" spans="1:338" x14ac:dyDescent="0.25">
       <c r="A92" s="1" t="s">
         <v>49</v>
       </c>
@@ -13965,7 +13965,7 @@
         <v>908</v>
       </c>
     </row>
-    <row r="93" spans="1:338" x14ac:dyDescent="0.45">
+    <row r="93" spans="1:338" x14ac:dyDescent="0.25">
       <c r="A93" s="1" t="s">
         <v>46</v>
       </c>
@@ -13985,7 +13985,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="94" spans="1:338" x14ac:dyDescent="0.45">
+    <row r="94" spans="1:338" x14ac:dyDescent="0.25">
       <c r="A94" s="1" t="s">
         <v>45</v>
       </c>
@@ -14002,7 +14002,7 @@
         <v>1096</v>
       </c>
       <c r="LZ94" s="1" t="s">
-        <v>1130</v>
+        <v>1129</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Implemented changing value of condition with effects Improved avoiding duplicate conditions from Health circumstances Generally improved avoiding duplicate persistent conditions Fixed bug where Persistent Damage choice was not shown and not editable Fixed Conditions ending when changing choices when a choice was granting the endsWithCondition condition Tested and bugfixed some more complicated spell and condition combinations
</commit_message>
<xml_diff>
--- a/work assets/activities.xlsx
+++ b/work assets/activities.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/eb76e5660c890129/Personal/Projects/Design/PECS/PECS/work assets/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="619" documentId="13_ncr:40009_{E3EB266C-7612-416D-8781-7A2BED99FA57}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{4004FD57-9FFF-47DB-A752-68EC7A4EF4F2}"/>
+  <xr:revisionPtr revIDLastSave="621" documentId="13_ncr:40009_{E3EB266C-7612-416D-8781-7A2BED99FA57}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{51F91192-B6FE-4179-85BA-80308CB54093}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="77040" windowHeight="21240" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="24570" yWindow="1440" windowWidth="30780" windowHeight="15435" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="activities" sheetId="1" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5289" uniqueCount="1161">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2707" uniqueCount="1160">
   <si>
     <t>name</t>
   </si>
@@ -3540,9 +3540,6 @@
   </si>
   <si>
     <t>Nature Incarnate</t>
-  </si>
-  <si>
-    <t>Nature Incarnate (True Shapeshifter)</t>
   </si>
   <si>
     <t>The life-giving properties of the aeon orbs flourish within you. Small plants or fungi magically appear on all surfaces in a 60-foot emanation around you. This life withers after 1 day unless the environment can support it. You can choose one of the following options each time you use this feat.
@@ -4841,13 +4838,13 @@
     </row>
     <row r="2" spans="1:93" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>1138</v>
+        <v>1137</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>71</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>1141</v>
+        <v>1140</v>
       </c>
       <c r="D2" s="2" t="s">
         <v>696</v>
@@ -4861,7 +4858,7 @@
       <c r="I2" s="2"/>
       <c r="J2" s="2"/>
       <c r="K2" s="1" t="s">
-        <v>1140</v>
+        <v>1139</v>
       </c>
       <c r="L2" s="1" t="s">
         <v>697</v>
@@ -4875,7 +4872,7 @@
       <c r="S2" s="1"/>
       <c r="T2" s="1"/>
       <c r="U2" s="1" t="s">
-        <v>1139</v>
+        <v>1138</v>
       </c>
       <c r="V2" s="1"/>
       <c r="W2" s="3"/>
@@ -4952,13 +4949,13 @@
     </row>
     <row r="3" spans="1:93" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>1143</v>
+        <v>1142</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>51</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>1145</v>
+        <v>1144</v>
       </c>
       <c r="D3" s="2" t="s">
         <v>343</v>
@@ -4982,7 +4979,7 @@
       <c r="S3" s="1"/>
       <c r="T3" s="1"/>
       <c r="U3" s="1" t="s">
-        <v>1144</v>
+        <v>1143</v>
       </c>
       <c r="V3" s="1"/>
       <c r="W3" s="3"/>
@@ -5059,7 +5056,7 @@
     </row>
     <row r="4" spans="1:93" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>1146</v>
+        <v>1145</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>51</v>
@@ -5091,7 +5088,7 @@
       <c r="S4" s="1"/>
       <c r="T4" s="1"/>
       <c r="U4" s="1" t="s">
-        <v>1147</v>
+        <v>1146</v>
       </c>
       <c r="V4" s="1"/>
       <c r="W4" s="3"/>
@@ -5106,10 +5103,10 @@
         <v>1</v>
       </c>
       <c r="AF4" s="4" t="s">
-        <v>1146</v>
+        <v>1145</v>
       </c>
       <c r="AG4" s="4" t="s">
-        <v>1146</v>
+        <v>1145</v>
       </c>
       <c r="AH4" s="7"/>
       <c r="AI4" s="4"/>
@@ -5174,13 +5171,13 @@
     </row>
     <row r="5" spans="1:93" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>1148</v>
+        <v>1147</v>
       </c>
       <c r="B5" s="1" t="s">
         <v>130</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>1151</v>
+        <v>1150</v>
       </c>
       <c r="D5" s="2" t="s">
         <v>195</v>
@@ -5195,7 +5192,7 @@
       <c r="J5" s="2"/>
       <c r="K5" s="1"/>
       <c r="L5" s="1" t="s">
-        <v>1149</v>
+        <v>1148</v>
       </c>
       <c r="M5" s="1"/>
       <c r="N5" s="1"/>
@@ -5210,7 +5207,7 @@
       <c r="S5" s="1"/>
       <c r="T5" s="1"/>
       <c r="U5" s="1" t="s">
-        <v>1150</v>
+        <v>1149</v>
       </c>
       <c r="V5" s="1"/>
       <c r="W5" s="3"/>
@@ -5225,10 +5222,10 @@
         <v>1</v>
       </c>
       <c r="AF5" s="4" t="s">
-        <v>1146</v>
+        <v>1145</v>
       </c>
       <c r="AG5" s="4" t="s">
-        <v>1146</v>
+        <v>1145</v>
       </c>
       <c r="AH5" s="7"/>
       <c r="AI5" s="4"/>
@@ -5307,10 +5304,10 @@
   <dimension ref="A1:MG94"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="LM2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="LU2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="LY3" sqref="LY3"/>
+      <selection pane="bottomRight" activeCell="LZ32" sqref="LZ32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5988,7 +5985,7 @@
         <v>698</v>
       </c>
       <c r="HO1" t="s">
-        <v>1153</v>
+        <v>1152</v>
       </c>
       <c r="HP1" t="s">
         <v>701</v>
@@ -6339,22 +6336,22 @@
         <v>1125</v>
       </c>
       <c r="MB1" t="s">
-        <v>1134</v>
+        <v>1133</v>
       </c>
       <c r="MC1" t="s">
-        <v>1138</v>
+        <v>1137</v>
       </c>
       <c r="MD1" t="s">
-        <v>1143</v>
+        <v>1142</v>
       </c>
       <c r="ME1" t="s">
-        <v>1146</v>
+        <v>1145</v>
       </c>
       <c r="MF1" t="s">
-        <v>1148</v>
+        <v>1147</v>
       </c>
       <c r="MG1" t="s">
-        <v>1155</v>
+        <v>1154</v>
       </c>
     </row>
     <row r="2" spans="1:345" x14ac:dyDescent="0.25">
@@ -7531,7 +7528,7 @@
         <v>618</v>
       </c>
       <c r="HM3" s="1" t="s">
-        <v>1142</v>
+        <v>1141</v>
       </c>
       <c r="HQ3" s="1" t="s">
         <v>706</v>
@@ -7570,25 +7567,25 @@
         <v>1084</v>
       </c>
       <c r="LH3" s="1" t="s">
-        <v>1160</v>
+        <v>1159</v>
       </c>
       <c r="LM3" s="1" t="s">
         <v>1077</v>
       </c>
       <c r="LT3" s="1" t="s">
-        <v>1137</v>
+        <v>1136</v>
       </c>
       <c r="LY3" s="1" t="s">
-        <v>1132</v>
+        <v>1131</v>
       </c>
       <c r="MC3" s="1" t="s">
-        <v>1141</v>
+        <v>1140</v>
       </c>
       <c r="MD3" s="1" t="s">
-        <v>1145</v>
+        <v>1144</v>
       </c>
       <c r="MF3" s="1" t="s">
-        <v>1151</v>
+        <v>1150</v>
       </c>
     </row>
     <row r="4" spans="1:345" s="2" customFormat="1" x14ac:dyDescent="0.25">
@@ -10259,7 +10256,7 @@
         <v>683</v>
       </c>
       <c r="HO11" s="1" t="s">
-        <v>1154</v>
+        <v>1153</v>
       </c>
       <c r="HQ11" s="1" t="s">
         <v>705</v>
@@ -10340,7 +10337,7 @@
         <v>1117</v>
       </c>
       <c r="MC11" s="1" t="s">
-        <v>1140</v>
+        <v>1139</v>
       </c>
     </row>
     <row r="12" spans="1:345" x14ac:dyDescent="0.25">
@@ -10558,7 +10555,7 @@
         <v>697</v>
       </c>
       <c r="MF12" s="1" t="s">
-        <v>1149</v>
+        <v>1148</v>
       </c>
     </row>
     <row r="13" spans="1:345" x14ac:dyDescent="0.25">
@@ -11729,7 +11726,7 @@
         <v>699</v>
       </c>
       <c r="HO21" s="1" t="s">
-        <v>1152</v>
+        <v>1151</v>
       </c>
       <c r="HP21" s="1" t="s">
         <v>702</v>
@@ -12059,7 +12056,7 @@
         <v>1115</v>
       </c>
       <c r="LU21" s="1" t="s">
-        <v>1136</v>
+        <v>1135</v>
       </c>
       <c r="LV21" s="1" t="s">
         <v>1118</v>
@@ -12068,7 +12065,7 @@
         <v>1122</v>
       </c>
       <c r="LX21" s="1" t="s">
-        <v>1133</v>
+        <v>1132</v>
       </c>
       <c r="LY21" s="1" t="s">
         <v>1127</v>
@@ -12077,25 +12074,25 @@
         <v>1128</v>
       </c>
       <c r="MA21" s="1" t="s">
-        <v>1131</v>
+        <v>1130</v>
       </c>
       <c r="MB21" s="1" t="s">
-        <v>1135</v>
+        <v>1134</v>
       </c>
       <c r="MC21" s="1" t="s">
-        <v>1139</v>
+        <v>1138</v>
       </c>
       <c r="MD21" s="1" t="s">
-        <v>1144</v>
+        <v>1143</v>
       </c>
       <c r="ME21" s="1" t="s">
-        <v>1147</v>
+        <v>1146</v>
       </c>
       <c r="MF21" s="1" t="s">
-        <v>1150</v>
+        <v>1149</v>
       </c>
       <c r="MG21" s="1" t="s">
-        <v>1156</v>
+        <v>1155</v>
       </c>
     </row>
     <row r="22" spans="1:345" x14ac:dyDescent="0.25">
@@ -12918,7 +12915,7 @@
         <v>666</v>
       </c>
       <c r="HO32" s="4" t="s">
-        <v>1153</v>
+        <v>1152</v>
       </c>
       <c r="HQ32" s="4" t="s">
         <v>703</v>
@@ -13065,16 +13062,16 @@
         <v>1123</v>
       </c>
       <c r="LZ32" s="4" t="s">
-        <v>1130</v>
+        <v>1124</v>
       </c>
       <c r="MA32" s="4" t="s">
         <v>1125</v>
       </c>
       <c r="ME32" s="4" t="s">
-        <v>1146</v>
+        <v>1145</v>
       </c>
       <c r="MG32" s="4" t="s">
-        <v>1157</v>
+        <v>1156</v>
       </c>
     </row>
     <row r="33" spans="1:345" s="4" customFormat="1" x14ac:dyDescent="0.25">
@@ -13253,7 +13250,7 @@
         <v>666</v>
       </c>
       <c r="HO33" s="4" t="s">
-        <v>1153</v>
+        <v>1152</v>
       </c>
       <c r="HQ33" s="4" t="s">
         <v>703</v>
@@ -13406,15 +13403,15 @@
         <v>1125</v>
       </c>
       <c r="ME33" s="4" t="s">
-        <v>1146</v>
+        <v>1145</v>
       </c>
       <c r="MG33" s="4" t="s">
-        <v>1158</v>
+        <v>1157</v>
       </c>
     </row>
     <row r="34" spans="1:345" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A34" s="4" t="s">
-        <v>1159</v>
+        <v>1158</v>
       </c>
       <c r="MG34" s="4">
         <v>1</v>

</xml_diff>

<commit_message>
Tested activity condition choices determined by feat subtype Removed hideChoices from activity because it is implemented on conditionGain
</commit_message>
<xml_diff>
--- a/work assets/activities.xlsx
+++ b/work assets/activities.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/eb76e5660c890129/Personal/Projects/Design/PECS/PECS/work assets/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="621" documentId="13_ncr:40009_{E3EB266C-7612-416D-8781-7A2BED99FA57}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{51F91192-B6FE-4179-85BA-80308CB54093}"/>
+  <xr:revisionPtr revIDLastSave="641" documentId="13_ncr:40009_{E3EB266C-7612-416D-8781-7A2BED99FA57}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{9400059F-5AEE-499F-B9D2-3BD63C13A416}"/>
   <bookViews>
-    <workbookView xWindow="24570" yWindow="1440" windowWidth="30780" windowHeight="15435" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4920" yWindow="4530" windowWidth="10680" windowHeight="6240" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="activities" sheetId="1" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2707" uniqueCount="1160">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2640" uniqueCount="1145">
   <si>
     <t>name</t>
   </si>
@@ -3216,48 +3216,12 @@
     <t>You end your rage to stay at 1 Hit Point. You become wounded 2 (or increase your wounded condition by 2 if you are already wounded).</t>
   </si>
   <si>
-    <t>Ape</t>
-  </si>
-  <si>
-    <t>Bear</t>
-  </si>
-  <si>
-    <t>Bull</t>
-  </si>
-  <si>
-    <t>Canine</t>
-  </si>
-  <si>
-    <t>Cat</t>
-  </si>
-  <si>
-    <t>Deer</t>
-  </si>
-  <si>
-    <t>Frog</t>
-  </si>
-  <si>
-    <t>Shark</t>
-  </si>
-  <si>
-    <t>Snake</t>
-  </si>
-  <si>
     <t>gainConditions/0/choice</t>
   </si>
   <si>
     <t>gainConditions/1/choice</t>
   </si>
   <si>
-    <t>Has_Feat(Creature.type, 'Animal Instinct: Bull') ? 1 : 0</t>
-  </si>
-  <si>
-    <t>Has_Feat(Creature.type, 'Animal Instinct: Bear') ? 1 : 0</t>
-  </si>
-  <si>
-    <t>Has_Feat(Creature.type, 'Animal Instinct: Ape') ? 1 : 0</t>
-  </si>
-  <si>
     <t>gainConditions/2/choice</t>
   </si>
   <si>
@@ -3349,24 +3313,6 @@
   </si>
   <si>
     <t>gainConditions/8/source</t>
-  </si>
-  <si>
-    <t>Has_Feat(Creature.type, 'Animal Instinct: Cat') ? 1 : 0</t>
-  </si>
-  <si>
-    <t>Has_Feat(Creature.type, 'Animal Instinct: Deer') ? 1 : 0</t>
-  </si>
-  <si>
-    <t>Has_Feat(Creature.type, 'Animal Instinct: Frog') ? 1 : 0</t>
-  </si>
-  <si>
-    <t>Has_Feat(Creature.type, 'Animal Instinct: Shark') ? 1 : 0</t>
-  </si>
-  <si>
-    <t>Has_Feat(Creature.type, 'Animal Instinct: Snake') ? 1 : 0</t>
-  </si>
-  <si>
-    <t>Has_Feat(Creature.type, 'Animal Instinct: Wolf') ? 1 : 0</t>
   </si>
   <si>
     <t>Dragon Form Breath Weapon</t>
@@ -3640,6 +3586,15 @@
   </si>
   <si>
     <t>Roll 1d4 and choose the appropriate duration for the cooldown condition.</t>
+  </si>
+  <si>
+    <t>Animal Instinct</t>
+  </si>
+  <si>
+    <t>gainConditions/0/hideChoices</t>
+  </si>
+  <si>
+    <t>gainConditions/0/choiceBySubType</t>
   </si>
 </sst>
 </file>
@@ -4596,7 +4551,7 @@
         <v>5</v>
       </c>
       <c r="N1" s="1" t="s">
-        <v>1085</v>
+        <v>1067</v>
       </c>
       <c r="O1" s="1" t="s">
         <v>48</v>
@@ -4641,10 +4596,10 @@
         <v>22</v>
       </c>
       <c r="AC1" s="4" t="s">
-        <v>1034</v>
+        <v>1025</v>
       </c>
       <c r="AD1" s="4" t="s">
-        <v>1086</v>
+        <v>1068</v>
       </c>
       <c r="AE1" s="4" t="s">
         <v>7</v>
@@ -4659,10 +4614,10 @@
         <v>29</v>
       </c>
       <c r="AI1" s="4" t="s">
-        <v>1035</v>
+        <v>1026</v>
       </c>
       <c r="AJ1" s="4" t="s">
-        <v>1094</v>
+        <v>1076</v>
       </c>
       <c r="AK1" s="4" t="s">
         <v>26</v>
@@ -4680,10 +4635,10 @@
         <v>33</v>
       </c>
       <c r="AP1" s="4" t="s">
-        <v>1039</v>
+        <v>1027</v>
       </c>
       <c r="AQ1" s="4" t="s">
-        <v>1093</v>
+        <v>1075</v>
       </c>
       <c r="AR1" s="4" t="s">
         <v>30</v>
@@ -4695,112 +4650,112 @@
         <v>32</v>
       </c>
       <c r="AU1" s="7" t="s">
+        <v>1028</v>
+      </c>
+      <c r="AV1" s="4" t="s">
+        <v>1029</v>
+      </c>
+      <c r="AW1" s="4" t="s">
+        <v>1074</v>
+      </c>
+      <c r="AX1" s="4" t="s">
+        <v>1030</v>
+      </c>
+      <c r="AY1" s="4" t="s">
+        <v>1031</v>
+      </c>
+      <c r="AZ1" s="4" t="s">
+        <v>1032</v>
+      </c>
+      <c r="BA1" s="7" t="s">
+        <v>1033</v>
+      </c>
+      <c r="BB1" s="4" t="s">
+        <v>1034</v>
+      </c>
+      <c r="BC1" s="4" t="s">
+        <v>1073</v>
+      </c>
+      <c r="BD1" s="4" t="s">
+        <v>1035</v>
+      </c>
+      <c r="BE1" s="4" t="s">
+        <v>1036</v>
+      </c>
+      <c r="BF1" s="4" t="s">
+        <v>1037</v>
+      </c>
+      <c r="BG1" s="7" t="s">
+        <v>1038</v>
+      </c>
+      <c r="BH1" s="4" t="s">
+        <v>1039</v>
+      </c>
+      <c r="BI1" s="4" t="s">
+        <v>1072</v>
+      </c>
+      <c r="BJ1" s="4" t="s">
         <v>1040</v>
       </c>
-      <c r="AV1" s="4" t="s">
+      <c r="BK1" s="4" t="s">
         <v>1041</v>
       </c>
-      <c r="AW1" s="4" t="s">
-        <v>1092</v>
-      </c>
-      <c r="AX1" s="4" t="s">
+      <c r="BL1" s="4" t="s">
         <v>1042</v>
       </c>
-      <c r="AY1" s="4" t="s">
+      <c r="BM1" s="7" t="s">
         <v>1043</v>
       </c>
-      <c r="AZ1" s="4" t="s">
+      <c r="BN1" s="4" t="s">
         <v>1044</v>
       </c>
-      <c r="BA1" s="7" t="s">
+      <c r="BO1" s="4" t="s">
+        <v>1071</v>
+      </c>
+      <c r="BP1" s="4" t="s">
         <v>1045</v>
       </c>
-      <c r="BB1" s="4" t="s">
+      <c r="BQ1" s="4" t="s">
         <v>1046</v>
       </c>
-      <c r="BC1" s="4" t="s">
-        <v>1091</v>
-      </c>
-      <c r="BD1" s="4" t="s">
+      <c r="BR1" s="4" t="s">
         <v>1047</v>
       </c>
-      <c r="BE1" s="4" t="s">
+      <c r="BS1" s="7" t="s">
         <v>1048</v>
       </c>
-      <c r="BF1" s="4" t="s">
+      <c r="BT1" s="4" t="s">
         <v>1049</v>
       </c>
-      <c r="BG1" s="7" t="s">
+      <c r="BU1" s="4" t="s">
+        <v>1070</v>
+      </c>
+      <c r="BV1" s="4" t="s">
         <v>1050</v>
       </c>
-      <c r="BH1" s="4" t="s">
+      <c r="BW1" s="4" t="s">
         <v>1051</v>
       </c>
-      <c r="BI1" s="4" t="s">
-        <v>1090</v>
-      </c>
-      <c r="BJ1" s="4" t="s">
+      <c r="BX1" s="4" t="s">
         <v>1052</v>
       </c>
-      <c r="BK1" s="4" t="s">
+      <c r="BY1" s="7" t="s">
         <v>1053</v>
       </c>
-      <c r="BL1" s="4" t="s">
+      <c r="BZ1" s="4" t="s">
         <v>1054</v>
       </c>
-      <c r="BM1" s="7" t="s">
+      <c r="CA1" s="4" t="s">
+        <v>1069</v>
+      </c>
+      <c r="CB1" s="4" t="s">
         <v>1055</v>
       </c>
-      <c r="BN1" s="4" t="s">
+      <c r="CC1" s="4" t="s">
         <v>1056</v>
       </c>
-      <c r="BO1" s="4" t="s">
-        <v>1089</v>
-      </c>
-      <c r="BP1" s="4" t="s">
+      <c r="CD1" s="4" t="s">
         <v>1057</v>
-      </c>
-      <c r="BQ1" s="4" t="s">
-        <v>1058</v>
-      </c>
-      <c r="BR1" s="4" t="s">
-        <v>1059</v>
-      </c>
-      <c r="BS1" s="7" t="s">
-        <v>1060</v>
-      </c>
-      <c r="BT1" s="4" t="s">
-        <v>1061</v>
-      </c>
-      <c r="BU1" s="4" t="s">
-        <v>1088</v>
-      </c>
-      <c r="BV1" s="4" t="s">
-        <v>1062</v>
-      </c>
-      <c r="BW1" s="4" t="s">
-        <v>1063</v>
-      </c>
-      <c r="BX1" s="4" t="s">
-        <v>1064</v>
-      </c>
-      <c r="BY1" s="7" t="s">
-        <v>1065</v>
-      </c>
-      <c r="BZ1" s="4" t="s">
-        <v>1066</v>
-      </c>
-      <c r="CA1" s="4" t="s">
-        <v>1087</v>
-      </c>
-      <c r="CB1" s="4" t="s">
-        <v>1067</v>
-      </c>
-      <c r="CC1" s="4" t="s">
-        <v>1068</v>
-      </c>
-      <c r="CD1" s="4" t="s">
-        <v>1069</v>
       </c>
       <c r="CE1" s="5" t="s">
         <v>23</v>
@@ -4838,13 +4793,13 @@
     </row>
     <row r="2" spans="1:93" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>1137</v>
+        <v>1119</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>71</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>1140</v>
+        <v>1122</v>
       </c>
       <c r="D2" s="2" t="s">
         <v>696</v>
@@ -4858,7 +4813,7 @@
       <c r="I2" s="2"/>
       <c r="J2" s="2"/>
       <c r="K2" s="1" t="s">
-        <v>1139</v>
+        <v>1121</v>
       </c>
       <c r="L2" s="1" t="s">
         <v>697</v>
@@ -4872,7 +4827,7 @@
       <c r="S2" s="1"/>
       <c r="T2" s="1"/>
       <c r="U2" s="1" t="s">
-        <v>1138</v>
+        <v>1120</v>
       </c>
       <c r="V2" s="1"/>
       <c r="W2" s="3"/>
@@ -4949,13 +4904,13 @@
     </row>
     <row r="3" spans="1:93" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>1142</v>
+        <v>1124</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>51</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>1144</v>
+        <v>1126</v>
       </c>
       <c r="D3" s="2" t="s">
         <v>343</v>
@@ -4979,7 +4934,7 @@
       <c r="S3" s="1"/>
       <c r="T3" s="1"/>
       <c r="U3" s="1" t="s">
-        <v>1143</v>
+        <v>1125</v>
       </c>
       <c r="V3" s="1"/>
       <c r="W3" s="3"/>
@@ -5056,7 +5011,7 @@
     </row>
     <row r="4" spans="1:93" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>1145</v>
+        <v>1127</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>51</v>
@@ -5088,7 +5043,7 @@
       <c r="S4" s="1"/>
       <c r="T4" s="1"/>
       <c r="U4" s="1" t="s">
-        <v>1146</v>
+        <v>1128</v>
       </c>
       <c r="V4" s="1"/>
       <c r="W4" s="3"/>
@@ -5103,10 +5058,10 @@
         <v>1</v>
       </c>
       <c r="AF4" s="4" t="s">
-        <v>1145</v>
+        <v>1127</v>
       </c>
       <c r="AG4" s="4" t="s">
-        <v>1145</v>
+        <v>1127</v>
       </c>
       <c r="AH4" s="7"/>
       <c r="AI4" s="4"/>
@@ -5171,13 +5126,13 @@
     </row>
     <row r="5" spans="1:93" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>1147</v>
+        <v>1129</v>
       </c>
       <c r="B5" s="1" t="s">
         <v>130</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>1150</v>
+        <v>1132</v>
       </c>
       <c r="D5" s="2" t="s">
         <v>195</v>
@@ -5192,7 +5147,7 @@
       <c r="J5" s="2"/>
       <c r="K5" s="1"/>
       <c r="L5" s="1" t="s">
-        <v>1148</v>
+        <v>1130</v>
       </c>
       <c r="M5" s="1"/>
       <c r="N5" s="1"/>
@@ -5207,7 +5162,7 @@
       <c r="S5" s="1"/>
       <c r="T5" s="1"/>
       <c r="U5" s="1" t="s">
-        <v>1149</v>
+        <v>1131</v>
       </c>
       <c r="V5" s="1"/>
       <c r="W5" s="3"/>
@@ -5222,10 +5177,10 @@
         <v>1</v>
       </c>
       <c r="AF5" s="4" t="s">
-        <v>1145</v>
+        <v>1127</v>
       </c>
       <c r="AG5" s="4" t="s">
-        <v>1145</v>
+        <v>1127</v>
       </c>
       <c r="AH5" s="7"/>
       <c r="AI5" s="4"/>
@@ -5301,13 +5256,13 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:MG94"/>
+  <dimension ref="A1:MG60"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="LU2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="KO2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="LZ32" sqref="LZ32"/>
+      <selection pane="bottomRight" activeCell="KS33" sqref="KS33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5985,7 +5940,7 @@
         <v>698</v>
       </c>
       <c r="HO1" t="s">
-        <v>1152</v>
+        <v>1134</v>
       </c>
       <c r="HP1" t="s">
         <v>701</v>
@@ -6276,7 +6231,7 @@
         <v>959</v>
       </c>
       <c r="LH1" t="s">
-        <v>1076</v>
+        <v>1058</v>
       </c>
       <c r="LI1" t="s">
         <v>960</v>
@@ -6297,61 +6252,61 @@
         <v>965</v>
       </c>
       <c r="LO1" t="s">
-        <v>1099</v>
+        <v>1081</v>
       </c>
       <c r="LP1" t="s">
+        <v>1087</v>
+      </c>
+      <c r="LQ1" t="s">
+        <v>1084</v>
+      </c>
+      <c r="LR1" t="s">
+        <v>1086</v>
+      </c>
+      <c r="LS1" t="s">
+        <v>1094</v>
+      </c>
+      <c r="LT1" t="s">
+        <v>1096</v>
+      </c>
+      <c r="LU1" t="s">
+        <v>1098</v>
+      </c>
+      <c r="LV1" t="s">
+        <v>1102</v>
+      </c>
+      <c r="LW1" t="s">
+        <v>1103</v>
+      </c>
+      <c r="LX1" t="s">
         <v>1105</v>
       </c>
-      <c r="LQ1" t="s">
-        <v>1102</v>
-      </c>
-      <c r="LR1" t="s">
-        <v>1104</v>
-      </c>
-      <c r="LS1" t="s">
-        <v>1112</v>
-      </c>
-      <c r="LT1" t="s">
-        <v>1114</v>
-      </c>
-      <c r="LU1" t="s">
-        <v>1116</v>
-      </c>
-      <c r="LV1" t="s">
-        <v>1120</v>
-      </c>
-      <c r="LW1" t="s">
-        <v>1121</v>
-      </c>
-      <c r="LX1" t="s">
-        <v>1123</v>
-      </c>
       <c r="LY1" t="s">
+        <v>1106</v>
+      </c>
+      <c r="LZ1" t="s">
+        <v>1108</v>
+      </c>
+      <c r="MA1" t="s">
+        <v>1107</v>
+      </c>
+      <c r="MB1" t="s">
+        <v>1115</v>
+      </c>
+      <c r="MC1" t="s">
+        <v>1119</v>
+      </c>
+      <c r="MD1" t="s">
         <v>1124</v>
       </c>
-      <c r="LZ1" t="s">
-        <v>1126</v>
-      </c>
-      <c r="MA1" t="s">
-        <v>1125</v>
-      </c>
-      <c r="MB1" t="s">
-        <v>1133</v>
-      </c>
-      <c r="MC1" t="s">
-        <v>1137</v>
-      </c>
-      <c r="MD1" t="s">
-        <v>1142</v>
-      </c>
       <c r="ME1" t="s">
-        <v>1145</v>
+        <v>1127</v>
       </c>
       <c r="MF1" t="s">
-        <v>1147</v>
+        <v>1129</v>
       </c>
       <c r="MG1" t="s">
-        <v>1154</v>
+        <v>1136</v>
       </c>
     </row>
     <row r="2" spans="1:345" x14ac:dyDescent="0.25">
@@ -7495,7 +7450,7 @@
         <v>480</v>
       </c>
       <c r="EN3" s="1" t="s">
-        <v>1098</v>
+        <v>1080</v>
       </c>
       <c r="FK3" s="1" t="s">
         <v>562</v>
@@ -7528,7 +7483,7 @@
         <v>618</v>
       </c>
       <c r="HM3" s="1" t="s">
-        <v>1141</v>
+        <v>1123</v>
       </c>
       <c r="HQ3" s="1" t="s">
         <v>706</v>
@@ -7558,34 +7513,34 @@
         <v>932</v>
       </c>
       <c r="KK3" s="1" t="s">
-        <v>1081</v>
+        <v>1063</v>
       </c>
       <c r="KN3" s="1" t="s">
         <v>976</v>
       </c>
       <c r="KU3" s="1" t="s">
-        <v>1084</v>
+        <v>1066</v>
       </c>
       <c r="LH3" s="1" t="s">
-        <v>1159</v>
+        <v>1141</v>
       </c>
       <c r="LM3" s="1" t="s">
-        <v>1077</v>
+        <v>1059</v>
       </c>
       <c r="LT3" s="1" t="s">
-        <v>1136</v>
+        <v>1118</v>
       </c>
       <c r="LY3" s="1" t="s">
-        <v>1131</v>
+        <v>1113</v>
       </c>
       <c r="MC3" s="1" t="s">
-        <v>1140</v>
+        <v>1122</v>
       </c>
       <c r="MD3" s="1" t="s">
-        <v>1144</v>
+        <v>1126</v>
       </c>
       <c r="MF3" s="1" t="s">
-        <v>1150</v>
+        <v>1132</v>
       </c>
     </row>
     <row r="4" spans="1:345" s="2" customFormat="1" x14ac:dyDescent="0.25">
@@ -8520,7 +8475,7 @@
         <v>342</v>
       </c>
       <c r="LQ4" s="2" t="s">
-        <v>1103</v>
+        <v>1085</v>
       </c>
       <c r="LR4" s="2" t="s">
         <v>625</v>
@@ -10256,7 +10211,7 @@
         <v>683</v>
       </c>
       <c r="HO11" s="1" t="s">
-        <v>1153</v>
+        <v>1135</v>
       </c>
       <c r="HQ11" s="1" t="s">
         <v>705</v>
@@ -10325,19 +10280,19 @@
         <v>1006</v>
       </c>
       <c r="LF11" s="1" t="s">
-        <v>1079</v>
+        <v>1061</v>
       </c>
       <c r="LI11" s="1" t="s">
         <v>1014</v>
       </c>
       <c r="LP11" s="1" t="s">
-        <v>1107</v>
+        <v>1089</v>
       </c>
       <c r="LU11" s="1" t="s">
-        <v>1117</v>
+        <v>1099</v>
       </c>
       <c r="MC11" s="1" t="s">
-        <v>1139</v>
+        <v>1121</v>
       </c>
     </row>
     <row r="12" spans="1:345" x14ac:dyDescent="0.25">
@@ -10549,13 +10504,13 @@
         <v>1023</v>
       </c>
       <c r="LP12" s="1" t="s">
-        <v>1106</v>
+        <v>1088</v>
       </c>
       <c r="MC12" s="1" t="s">
         <v>697</v>
       </c>
       <c r="MF12" s="1" t="s">
-        <v>1148</v>
+        <v>1130</v>
       </c>
     </row>
     <row r="13" spans="1:345" x14ac:dyDescent="0.25">
@@ -10739,10 +10694,7 @@
     </row>
     <row r="14" spans="1:345" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
-        <v>1085</v>
-      </c>
-      <c r="KS14" s="1" t="b">
-        <v>1</v>
+        <v>1067</v>
       </c>
     </row>
     <row r="15" spans="1:345" x14ac:dyDescent="0.25">
@@ -11045,6 +10997,9 @@
       <c r="KM20" s="1">
         <v>1</v>
       </c>
+      <c r="KS20" s="1">
+        <v>100</v>
+      </c>
       <c r="LG20" s="1">
         <v>100</v>
       </c>
@@ -11726,7 +11681,7 @@
         <v>699</v>
       </c>
       <c r="HO21" s="1" t="s">
-        <v>1151</v>
+        <v>1133</v>
       </c>
       <c r="HP21" s="1" t="s">
         <v>702</v>
@@ -12011,13 +11966,13 @@
         <v>1011</v>
       </c>
       <c r="LF21" s="1" t="s">
-        <v>1080</v>
+        <v>1062</v>
       </c>
       <c r="LG21" s="1" t="s">
         <v>1013</v>
       </c>
       <c r="LH21" s="1" t="s">
-        <v>1101</v>
+        <v>1083</v>
       </c>
       <c r="LI21" s="1" t="s">
         <v>1016</v>
@@ -12038,61 +11993,61 @@
         <v>1021</v>
       </c>
       <c r="LO21" s="1" t="s">
+        <v>1082</v>
+      </c>
+      <c r="LP21" s="1" t="s">
+        <v>1090</v>
+      </c>
+      <c r="LQ21" s="1" t="s">
+        <v>1092</v>
+      </c>
+      <c r="LR21" s="1" t="s">
+        <v>1093</v>
+      </c>
+      <c r="LS21" s="1" t="s">
+        <v>1095</v>
+      </c>
+      <c r="LT21" s="1" t="s">
+        <v>1097</v>
+      </c>
+      <c r="LU21" s="1" t="s">
+        <v>1117</v>
+      </c>
+      <c r="LV21" s="1" t="s">
         <v>1100</v>
       </c>
-      <c r="LP21" s="1" t="s">
-        <v>1108</v>
-      </c>
-      <c r="LQ21" s="1" t="s">
+      <c r="LW21" s="1" t="s">
+        <v>1104</v>
+      </c>
+      <c r="LX21" s="1" t="s">
+        <v>1114</v>
+      </c>
+      <c r="LY21" s="1" t="s">
+        <v>1109</v>
+      </c>
+      <c r="LZ21" s="1" t="s">
         <v>1110</v>
       </c>
-      <c r="LR21" s="1" t="s">
-        <v>1111</v>
-      </c>
-      <c r="LS21" s="1" t="s">
-        <v>1113</v>
-      </c>
-      <c r="LT21" s="1" t="s">
-        <v>1115</v>
-      </c>
-      <c r="LU21" s="1" t="s">
-        <v>1135</v>
-      </c>
-      <c r="LV21" s="1" t="s">
-        <v>1118</v>
-      </c>
-      <c r="LW21" s="1" t="s">
-        <v>1122</v>
-      </c>
-      <c r="LX21" s="1" t="s">
-        <v>1132</v>
-      </c>
-      <c r="LY21" s="1" t="s">
-        <v>1127</v>
-      </c>
-      <c r="LZ21" s="1" t="s">
+      <c r="MA21" s="1" t="s">
+        <v>1112</v>
+      </c>
+      <c r="MB21" s="1" t="s">
+        <v>1116</v>
+      </c>
+      <c r="MC21" s="1" t="s">
+        <v>1120</v>
+      </c>
+      <c r="MD21" s="1" t="s">
+        <v>1125</v>
+      </c>
+      <c r="ME21" s="1" t="s">
         <v>1128</v>
       </c>
-      <c r="MA21" s="1" t="s">
-        <v>1130</v>
-      </c>
-      <c r="MB21" s="1" t="s">
-        <v>1134</v>
-      </c>
-      <c r="MC21" s="1" t="s">
-        <v>1138</v>
-      </c>
-      <c r="MD21" s="1" t="s">
-        <v>1143</v>
-      </c>
-      <c r="ME21" s="1" t="s">
-        <v>1146</v>
-      </c>
       <c r="MF21" s="1" t="s">
-        <v>1149</v>
+        <v>1131</v>
       </c>
       <c r="MG21" s="1" t="s">
-        <v>1155</v>
+        <v>1137</v>
       </c>
     </row>
     <row r="22" spans="1:345" x14ac:dyDescent="0.25">
@@ -12382,11 +12337,8 @@
       <c r="BB27" s="7" t="s">
         <v>241</v>
       </c>
-      <c r="KS27" s="7" t="s">
-        <v>1038</v>
-      </c>
       <c r="KU27" s="7" t="s">
-        <v>1082</v>
+        <v>1064</v>
       </c>
     </row>
     <row r="28" spans="1:345" s="4" customFormat="1" x14ac:dyDescent="0.25">
@@ -12402,1609 +12354,1322 @@
     </row>
     <row r="29" spans="1:345" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A29" s="4" t="s">
-        <v>1034</v>
-      </c>
-      <c r="KS29" s="4" t="s">
         <v>1025</v>
       </c>
     </row>
     <row r="30" spans="1:345" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A30" s="4" t="s">
-        <v>1086</v>
-      </c>
-      <c r="KS30" s="4" t="b">
-        <v>1</v>
+        <v>1144</v>
+      </c>
+      <c r="KS30" s="4" t="s">
+        <v>1142</v>
       </c>
     </row>
     <row r="31" spans="1:345" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A31" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="C31" s="4">
-        <v>-1</v>
-      </c>
-      <c r="D31" s="4">
-        <v>-1</v>
-      </c>
-      <c r="E31" s="4">
-        <v>-1</v>
-      </c>
-      <c r="F31" s="4">
-        <v>-1</v>
-      </c>
-      <c r="G31" s="4">
-        <v>-1</v>
-      </c>
-      <c r="H31" s="4">
-        <v>-1</v>
-      </c>
-      <c r="I31" s="4">
-        <v>1</v>
-      </c>
-      <c r="L31" s="4">
-        <v>1</v>
-      </c>
-      <c r="N31" s="4">
-        <v>10</v>
-      </c>
-      <c r="R31" s="4">
-        <v>-1</v>
-      </c>
-      <c r="T31" s="4">
-        <v>-1</v>
-      </c>
-      <c r="AA31" s="4">
-        <v>10</v>
-      </c>
-      <c r="AJ31" s="4">
-        <v>-2</v>
-      </c>
-      <c r="AN31" s="4">
-        <v>10</v>
-      </c>
-      <c r="AQ31" s="4">
-        <v>100</v>
-      </c>
-      <c r="AR31" s="4">
-        <v>200</v>
-      </c>
-      <c r="AS31" s="4">
-        <v>500</v>
-      </c>
-      <c r="BB31" s="4">
-        <v>1000</v>
-      </c>
-      <c r="BN31" s="4">
-        <v>-1</v>
-      </c>
-      <c r="BP31" s="4">
-        <v>1</v>
-      </c>
-      <c r="BR31" s="4">
-        <v>-1</v>
-      </c>
-      <c r="BU31" s="4">
-        <v>-1</v>
-      </c>
-      <c r="DH31" s="4">
-        <v>0</v>
-      </c>
-      <c r="DI31" s="4">
-        <v>0</v>
-      </c>
-      <c r="DJ31" s="4">
-        <v>0</v>
-      </c>
-      <c r="DK31" s="4">
-        <v>0</v>
-      </c>
-      <c r="DL31" s="4">
-        <v>0</v>
-      </c>
-      <c r="DM31" s="4">
-        <v>0</v>
-      </c>
-      <c r="DN31" s="4">
-        <v>0</v>
-      </c>
-      <c r="DO31" s="4">
-        <v>0</v>
-      </c>
-      <c r="DQ31" s="4">
-        <v>-1</v>
-      </c>
-      <c r="DS31" s="4">
-        <v>-1</v>
-      </c>
-      <c r="EB31" s="4">
-        <v>10</v>
-      </c>
-      <c r="EK31" s="4">
-        <v>10</v>
-      </c>
-      <c r="EM31" s="4">
-        <v>-1</v>
-      </c>
-      <c r="ES31" s="4">
-        <v>-1</v>
-      </c>
-      <c r="EU31" s="4">
-        <v>-1</v>
-      </c>
-      <c r="FA31" s="4">
-        <v>-1</v>
-      </c>
-      <c r="FE31" s="4">
-        <v>-1</v>
-      </c>
-      <c r="FG31" s="4">
-        <v>-1</v>
-      </c>
-      <c r="FH31" s="4">
-        <v>-1</v>
-      </c>
-      <c r="FP31" s="4">
-        <v>-1</v>
-      </c>
-      <c r="FQ31" s="4">
-        <v>-1</v>
-      </c>
-      <c r="FR31" s="4">
-        <v>-1</v>
-      </c>
-      <c r="FW31" s="4">
-        <v>-1</v>
-      </c>
-      <c r="FX31" s="4">
-        <v>-1</v>
-      </c>
-      <c r="FY31" s="4">
-        <v>-1</v>
-      </c>
-      <c r="FZ31" s="4">
-        <v>-1</v>
-      </c>
-      <c r="GA31" s="4">
-        <v>-1</v>
-      </c>
-      <c r="GB31" s="4">
-        <v>-1</v>
-      </c>
-      <c r="GC31" s="4">
-        <v>-1</v>
-      </c>
-      <c r="GD31" s="4">
-        <v>-1</v>
-      </c>
-      <c r="GE31" s="4">
-        <v>-1</v>
-      </c>
-      <c r="GN31" s="4">
-        <v>-1</v>
-      </c>
-      <c r="GV31" s="4">
-        <v>-1</v>
-      </c>
-      <c r="GW31" s="4">
-        <v>-1</v>
-      </c>
-      <c r="GX31" s="4">
-        <v>-1</v>
-      </c>
-      <c r="GZ31" s="4">
-        <v>-1</v>
-      </c>
-      <c r="HO31" s="4">
-        <v>5</v>
-      </c>
-      <c r="HQ31" s="4">
-        <v>15</v>
-      </c>
-      <c r="HT31" s="4">
-        <v>-1</v>
-      </c>
-      <c r="HW31" s="4">
-        <v>1</v>
-      </c>
-      <c r="IN31" s="4">
-        <v>10</v>
-      </c>
-      <c r="IP31" s="4">
-        <v>100</v>
-      </c>
-      <c r="IQ31" s="4">
-        <v>0</v>
-      </c>
-      <c r="IU31" s="4">
-        <v>100</v>
-      </c>
-      <c r="IV31" s="4">
-        <v>100</v>
-      </c>
-      <c r="JI31" s="4">
-        <v>100</v>
-      </c>
-      <c r="JN31" s="4">
-        <v>0</v>
-      </c>
-      <c r="JQ31" s="4">
-        <v>1</v>
-      </c>
-      <c r="JR31" s="4">
-        <v>-1</v>
-      </c>
-      <c r="JS31" s="4">
-        <v>1</v>
-      </c>
-      <c r="JT31" s="4">
-        <v>6000</v>
-      </c>
-      <c r="JU31" s="4">
-        <v>1</v>
-      </c>
-      <c r="JV31" s="4">
-        <v>15</v>
-      </c>
-      <c r="JX31" s="4">
-        <v>3000</v>
-      </c>
-      <c r="JY31" s="4">
-        <v>1</v>
-      </c>
-      <c r="KB31" s="4">
-        <v>15</v>
-      </c>
-      <c r="KC31" s="4">
-        <v>1008000</v>
-      </c>
-      <c r="KD31" s="4">
-        <v>100</v>
-      </c>
-      <c r="KE31" s="4">
-        <v>10</v>
-      </c>
-      <c r="KF31" s="4">
-        <v>100</v>
-      </c>
-      <c r="KH31" s="4">
-        <v>5</v>
-      </c>
-      <c r="KI31" s="4">
-        <v>1</v>
-      </c>
-      <c r="KL31" s="4">
-        <v>0</v>
-      </c>
-      <c r="KM31" s="4">
-        <v>1</v>
-      </c>
-      <c r="KP31" s="4">
-        <v>6000</v>
-      </c>
-      <c r="KQ31" s="4">
-        <v>-1</v>
-      </c>
-      <c r="KR31" s="4">
-        <v>-1</v>
-      </c>
-      <c r="KW31" s="4">
-        <v>-1</v>
-      </c>
-      <c r="LA31" s="4">
-        <v>-1</v>
-      </c>
-      <c r="LE31" s="4">
-        <v>-1</v>
-      </c>
-      <c r="LG31" s="4">
-        <v>100</v>
-      </c>
-      <c r="LH31" s="4">
-        <v>-5</v>
-      </c>
-      <c r="LI31" s="4">
-        <v>-1</v>
-      </c>
-      <c r="LJ31" s="4">
-        <v>1</v>
-      </c>
-      <c r="LO31" s="4">
-        <v>5</v>
-      </c>
-      <c r="LU31" s="4">
-        <v>-1</v>
-      </c>
-      <c r="LV31" s="4">
-        <v>48000</v>
-      </c>
-      <c r="LX31" s="4">
-        <v>1</v>
-      </c>
-      <c r="LZ31" s="4">
-        <v>100</v>
-      </c>
-      <c r="MA31" s="4">
-        <v>144000</v>
-      </c>
-      <c r="ME31" s="4">
-        <v>1</v>
-      </c>
-      <c r="MG31" s="4">
-        <v>5</v>
+        <v>1068</v>
       </c>
     </row>
     <row r="32" spans="1:345" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A32" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="C32" s="4" t="s">
-        <v>55</v>
-      </c>
-      <c r="D32" s="4" t="s">
-        <v>59</v>
-      </c>
-      <c r="E32" s="4" t="s">
-        <v>61</v>
-      </c>
-      <c r="F32" s="4" t="s">
-        <v>64</v>
-      </c>
-      <c r="G32" s="4" t="s">
-        <v>66</v>
-      </c>
-      <c r="H32" s="4" t="s">
-        <v>68</v>
-      </c>
-      <c r="I32" s="4" t="s">
-        <v>70</v>
-      </c>
-      <c r="L32" s="4" t="s">
-        <v>81</v>
-      </c>
-      <c r="N32" s="4" t="s">
-        <v>91</v>
-      </c>
-      <c r="R32" s="4" t="s">
-        <v>107</v>
-      </c>
-      <c r="T32" s="4" t="s">
-        <v>111</v>
-      </c>
-      <c r="AA32" s="4" t="s">
-        <v>133</v>
-      </c>
-      <c r="AJ32" s="4" t="s">
-        <v>164</v>
-      </c>
-      <c r="AM32" s="4" t="s">
-        <v>178</v>
-      </c>
-      <c r="AN32" s="4" t="s">
-        <v>1097</v>
-      </c>
-      <c r="AQ32" s="4" t="s">
-        <v>196</v>
-      </c>
-      <c r="AR32" s="4" t="s">
-        <v>196</v>
-      </c>
-      <c r="AS32" s="4" t="s">
-        <v>196</v>
-      </c>
-      <c r="BB32" s="4" t="s">
-        <v>239</v>
-      </c>
-      <c r="BN32" s="4" t="s">
-        <v>293</v>
-      </c>
-      <c r="BP32" s="4" t="s">
-        <v>299</v>
-      </c>
-      <c r="BR32" s="4" t="s">
-        <v>304</v>
-      </c>
-      <c r="BU32" s="4" t="s">
-        <v>315</v>
-      </c>
-      <c r="DH32" s="4" t="s">
-        <v>407</v>
-      </c>
-      <c r="DI32" s="4" t="s">
-        <v>407</v>
-      </c>
-      <c r="DJ32" s="4" t="s">
-        <v>407</v>
-      </c>
-      <c r="DK32" s="4" t="s">
-        <v>407</v>
-      </c>
-      <c r="DL32" s="4" t="s">
-        <v>407</v>
-      </c>
-      <c r="DM32" s="4" t="s">
-        <v>407</v>
-      </c>
-      <c r="DN32" s="4" t="s">
-        <v>407</v>
-      </c>
-      <c r="DO32" s="4" t="s">
-        <v>407</v>
-      </c>
-      <c r="DQ32" s="4" t="s">
-        <v>429</v>
-      </c>
-      <c r="DS32" s="4" t="s">
-        <v>437</v>
-      </c>
-      <c r="EB32" s="4" t="s">
-        <v>463</v>
-      </c>
-      <c r="EK32" s="4" t="s">
-        <v>488</v>
-      </c>
-      <c r="EM32" s="4" t="s">
-        <v>494</v>
-      </c>
-      <c r="ES32" s="4" t="s">
-        <v>512</v>
-      </c>
-      <c r="EU32" s="4" t="s">
-        <v>516</v>
-      </c>
-      <c r="FA32" s="4" t="s">
-        <v>532</v>
-      </c>
-      <c r="FE32" s="4" t="s">
-        <v>463</v>
-      </c>
-      <c r="FG32" s="4" t="s">
-        <v>549</v>
-      </c>
-      <c r="FH32" s="4" t="s">
-        <v>551</v>
-      </c>
-      <c r="FP32" s="4" t="s">
-        <v>573</v>
-      </c>
-      <c r="FQ32" s="4" t="s">
-        <v>575</v>
-      </c>
-      <c r="FR32" s="4" t="s">
-        <v>488</v>
-      </c>
-      <c r="FW32" s="4" t="s">
-        <v>592</v>
-      </c>
-      <c r="FX32" s="4" t="s">
-        <v>595</v>
-      </c>
-      <c r="FY32" s="4" t="s">
-        <v>598</v>
-      </c>
-      <c r="FZ32" s="4" t="s">
-        <v>601</v>
-      </c>
-      <c r="GA32" s="4" t="s">
-        <v>604</v>
-      </c>
-      <c r="GB32" s="4" t="s">
-        <v>607</v>
-      </c>
-      <c r="GC32" s="4" t="s">
-        <v>610</v>
-      </c>
-      <c r="GD32" s="4" t="s">
-        <v>613</v>
-      </c>
-      <c r="GE32" s="4" t="s">
-        <v>616</v>
-      </c>
-      <c r="GN32" s="4" t="s">
-        <v>639</v>
-      </c>
-      <c r="GV32" s="4" t="s">
-        <v>657</v>
-      </c>
-      <c r="GW32" s="4" t="s">
-        <v>659</v>
-      </c>
-      <c r="GX32" s="4" t="s">
-        <v>661</v>
-      </c>
-      <c r="GZ32" s="4" t="s">
-        <v>666</v>
-      </c>
-      <c r="HO32" s="4" t="s">
-        <v>1152</v>
-      </c>
-      <c r="HQ32" s="4" t="s">
-        <v>703</v>
-      </c>
-      <c r="HT32" s="4" t="s">
-        <v>712</v>
-      </c>
-      <c r="HW32" s="4" t="s">
-        <v>725</v>
-      </c>
-      <c r="IN32" s="4" t="s">
-        <v>785</v>
-      </c>
-      <c r="IP32" s="4" t="s">
-        <v>792</v>
-      </c>
-      <c r="IQ32" s="4" t="s">
-        <v>797</v>
-      </c>
-      <c r="IU32" s="4" t="s">
-        <v>810</v>
-      </c>
-      <c r="IV32" s="4" t="s">
-        <v>792</v>
-      </c>
-      <c r="JG32" s="4" t="s">
-        <v>850</v>
-      </c>
-      <c r="JI32" s="4" t="s">
-        <v>857</v>
-      </c>
-      <c r="JJ32" s="4" t="s">
-        <v>862</v>
-      </c>
-      <c r="JN32" s="4" t="s">
-        <v>873</v>
-      </c>
-      <c r="JQ32" s="4" t="s">
-        <v>881</v>
-      </c>
-      <c r="JR32" s="4" t="s">
-        <v>885</v>
-      </c>
-      <c r="JS32" s="4" t="s">
-        <v>887</v>
-      </c>
-      <c r="JT32" s="4" t="s">
-        <v>890</v>
-      </c>
-      <c r="JU32" s="4" t="s">
-        <v>894</v>
-      </c>
-      <c r="JV32" s="4" t="s">
-        <v>897</v>
-      </c>
-      <c r="JX32" s="4" t="s">
-        <v>905</v>
-      </c>
-      <c r="JY32" s="4" t="s">
-        <v>908</v>
-      </c>
-      <c r="KB32" s="4" t="s">
-        <v>916</v>
-      </c>
-      <c r="KC32" s="4" t="s">
-        <v>920</v>
-      </c>
-      <c r="KD32" s="4" t="s">
-        <v>924</v>
-      </c>
-      <c r="KE32" s="4" t="s">
-        <v>928</v>
-      </c>
-      <c r="KF32" s="4" t="s">
-        <v>930</v>
-      </c>
-      <c r="KH32" s="4" t="s">
-        <v>966</v>
-      </c>
-      <c r="KI32" s="4" t="s">
-        <v>936</v>
-      </c>
-      <c r="KK32" s="4" t="s">
-        <v>938</v>
-      </c>
-      <c r="KL32" s="4" t="s">
-        <v>939</v>
-      </c>
-      <c r="KM32" s="4" t="s">
-        <v>972</v>
-      </c>
-      <c r="KP32" s="4" t="s">
-        <v>979</v>
-      </c>
-      <c r="KQ32" s="4" t="s">
-        <v>943</v>
-      </c>
-      <c r="KR32" s="4" t="s">
-        <v>944</v>
-      </c>
-      <c r="KS32" s="4" t="s">
-        <v>945</v>
-      </c>
-      <c r="KU32" s="4" t="s">
-        <v>1083</v>
-      </c>
-      <c r="KW32" s="4" t="s">
-        <v>949</v>
-      </c>
-      <c r="LA32" s="4" t="s">
-        <v>1004</v>
-      </c>
-      <c r="LE32" s="4" t="s">
-        <v>957</v>
-      </c>
-      <c r="LG32" s="4" t="s">
-        <v>959</v>
-      </c>
-      <c r="LH32" s="4" t="s">
-        <v>1078</v>
-      </c>
-      <c r="LI32" s="4" t="s">
-        <v>960</v>
-      </c>
-      <c r="LJ32" s="4" t="s">
-        <v>961</v>
-      </c>
-      <c r="LM32" s="4" t="s">
-        <v>178</v>
-      </c>
-      <c r="LO32" s="4" t="s">
-        <v>1099</v>
-      </c>
-      <c r="LQ32" s="4" t="s">
-        <v>1102</v>
-      </c>
-      <c r="LU32" s="4" t="s">
-        <v>1116</v>
-      </c>
-      <c r="LV32" s="4" t="s">
-        <v>1119</v>
-      </c>
-      <c r="LX32" s="4" t="s">
-        <v>1123</v>
-      </c>
-      <c r="LZ32" s="4" t="s">
-        <v>1124</v>
-      </c>
-      <c r="MA32" s="4" t="s">
-        <v>1125</v>
-      </c>
-      <c r="ME32" s="4" t="s">
-        <v>1145</v>
-      </c>
-      <c r="MG32" s="4" t="s">
-        <v>1156</v>
+        <v>7</v>
+      </c>
+      <c r="C32" s="4">
+        <v>-1</v>
+      </c>
+      <c r="D32" s="4">
+        <v>-1</v>
+      </c>
+      <c r="E32" s="4">
+        <v>-1</v>
+      </c>
+      <c r="F32" s="4">
+        <v>-1</v>
+      </c>
+      <c r="G32" s="4">
+        <v>-1</v>
+      </c>
+      <c r="H32" s="4">
+        <v>-1</v>
+      </c>
+      <c r="I32" s="4">
+        <v>1</v>
+      </c>
+      <c r="L32" s="4">
+        <v>1</v>
+      </c>
+      <c r="N32" s="4">
+        <v>10</v>
+      </c>
+      <c r="R32" s="4">
+        <v>-1</v>
+      </c>
+      <c r="T32" s="4">
+        <v>-1</v>
+      </c>
+      <c r="AA32" s="4">
+        <v>10</v>
+      </c>
+      <c r="AJ32" s="4">
+        <v>-2</v>
+      </c>
+      <c r="AN32" s="4">
+        <v>10</v>
+      </c>
+      <c r="AQ32" s="4">
+        <v>100</v>
+      </c>
+      <c r="AR32" s="4">
+        <v>200</v>
+      </c>
+      <c r="AS32" s="4">
+        <v>500</v>
+      </c>
+      <c r="BB32" s="4">
+        <v>1000</v>
+      </c>
+      <c r="BN32" s="4">
+        <v>-1</v>
+      </c>
+      <c r="BP32" s="4">
+        <v>1</v>
+      </c>
+      <c r="BR32" s="4">
+        <v>-1</v>
+      </c>
+      <c r="BU32" s="4">
+        <v>-1</v>
+      </c>
+      <c r="DH32" s="4">
+        <v>0</v>
+      </c>
+      <c r="DI32" s="4">
+        <v>0</v>
+      </c>
+      <c r="DJ32" s="4">
+        <v>0</v>
+      </c>
+      <c r="DK32" s="4">
+        <v>0</v>
+      </c>
+      <c r="DL32" s="4">
+        <v>0</v>
+      </c>
+      <c r="DM32" s="4">
+        <v>0</v>
+      </c>
+      <c r="DN32" s="4">
+        <v>0</v>
+      </c>
+      <c r="DO32" s="4">
+        <v>0</v>
+      </c>
+      <c r="DQ32" s="4">
+        <v>-1</v>
+      </c>
+      <c r="DS32" s="4">
+        <v>-1</v>
+      </c>
+      <c r="EB32" s="4">
+        <v>10</v>
+      </c>
+      <c r="EK32" s="4">
+        <v>10</v>
+      </c>
+      <c r="EM32" s="4">
+        <v>-1</v>
+      </c>
+      <c r="ES32" s="4">
+        <v>-1</v>
+      </c>
+      <c r="EU32" s="4">
+        <v>-1</v>
+      </c>
+      <c r="FA32" s="4">
+        <v>-1</v>
+      </c>
+      <c r="FE32" s="4">
+        <v>-1</v>
+      </c>
+      <c r="FG32" s="4">
+        <v>-1</v>
+      </c>
+      <c r="FH32" s="4">
+        <v>-1</v>
+      </c>
+      <c r="FP32" s="4">
+        <v>-1</v>
+      </c>
+      <c r="FQ32" s="4">
+        <v>-1</v>
+      </c>
+      <c r="FR32" s="4">
+        <v>-1</v>
+      </c>
+      <c r="FW32" s="4">
+        <v>-1</v>
+      </c>
+      <c r="FX32" s="4">
+        <v>-1</v>
+      </c>
+      <c r="FY32" s="4">
+        <v>-1</v>
+      </c>
+      <c r="FZ32" s="4">
+        <v>-1</v>
+      </c>
+      <c r="GA32" s="4">
+        <v>-1</v>
+      </c>
+      <c r="GB32" s="4">
+        <v>-1</v>
+      </c>
+      <c r="GC32" s="4">
+        <v>-1</v>
+      </c>
+      <c r="GD32" s="4">
+        <v>-1</v>
+      </c>
+      <c r="GE32" s="4">
+        <v>-1</v>
+      </c>
+      <c r="GN32" s="4">
+        <v>-1</v>
+      </c>
+      <c r="GV32" s="4">
+        <v>-1</v>
+      </c>
+      <c r="GW32" s="4">
+        <v>-1</v>
+      </c>
+      <c r="GX32" s="4">
+        <v>-1</v>
+      </c>
+      <c r="GZ32" s="4">
+        <v>-1</v>
+      </c>
+      <c r="HO32" s="4">
+        <v>5</v>
+      </c>
+      <c r="HQ32" s="4">
+        <v>15</v>
+      </c>
+      <c r="HT32" s="4">
+        <v>-1</v>
+      </c>
+      <c r="HW32" s="4">
+        <v>1</v>
+      </c>
+      <c r="IN32" s="4">
+        <v>10</v>
+      </c>
+      <c r="IP32" s="4">
+        <v>100</v>
+      </c>
+      <c r="IQ32" s="4">
+        <v>0</v>
+      </c>
+      <c r="IU32" s="4">
+        <v>100</v>
+      </c>
+      <c r="IV32" s="4">
+        <v>100</v>
+      </c>
+      <c r="JI32" s="4">
+        <v>100</v>
+      </c>
+      <c r="JN32" s="4">
+        <v>0</v>
+      </c>
+      <c r="JQ32" s="4">
+        <v>1</v>
+      </c>
+      <c r="JR32" s="4">
+        <v>-1</v>
+      </c>
+      <c r="JS32" s="4">
+        <v>1</v>
+      </c>
+      <c r="JT32" s="4">
+        <v>6000</v>
+      </c>
+      <c r="JU32" s="4">
+        <v>1</v>
+      </c>
+      <c r="JV32" s="4">
+        <v>15</v>
+      </c>
+      <c r="JX32" s="4">
+        <v>3000</v>
+      </c>
+      <c r="JY32" s="4">
+        <v>1</v>
+      </c>
+      <c r="KB32" s="4">
+        <v>15</v>
+      </c>
+      <c r="KC32" s="4">
+        <v>1008000</v>
+      </c>
+      <c r="KD32" s="4">
+        <v>100</v>
+      </c>
+      <c r="KE32" s="4">
+        <v>10</v>
+      </c>
+      <c r="KF32" s="4">
+        <v>100</v>
+      </c>
+      <c r="KH32" s="4">
+        <v>5</v>
+      </c>
+      <c r="KI32" s="4">
+        <v>1</v>
+      </c>
+      <c r="KL32" s="4">
+        <v>0</v>
+      </c>
+      <c r="KM32" s="4">
+        <v>1</v>
+      </c>
+      <c r="KP32" s="4">
+        <v>6000</v>
+      </c>
+      <c r="KQ32" s="4">
+        <v>-1</v>
+      </c>
+      <c r="KR32" s="4">
+        <v>-1</v>
+      </c>
+      <c r="KS32" s="4">
+        <v>100</v>
+      </c>
+      <c r="KW32" s="4">
+        <v>-1</v>
+      </c>
+      <c r="LA32" s="4">
+        <v>-1</v>
+      </c>
+      <c r="LE32" s="4">
+        <v>-1</v>
+      </c>
+      <c r="LG32" s="4">
+        <v>100</v>
+      </c>
+      <c r="LH32" s="4">
+        <v>-5</v>
+      </c>
+      <c r="LI32" s="4">
+        <v>-1</v>
+      </c>
+      <c r="LJ32" s="4">
+        <v>1</v>
+      </c>
+      <c r="LO32" s="4">
+        <v>5</v>
+      </c>
+      <c r="LU32" s="4">
+        <v>-1</v>
+      </c>
+      <c r="LV32" s="4">
+        <v>48000</v>
+      </c>
+      <c r="LX32" s="4">
+        <v>1</v>
+      </c>
+      <c r="LZ32" s="4">
+        <v>100</v>
+      </c>
+      <c r="MA32" s="4">
+        <v>144000</v>
+      </c>
+      <c r="ME32" s="4">
+        <v>1</v>
+      </c>
+      <c r="MG32" s="4">
+        <v>5</v>
       </c>
     </row>
     <row r="33" spans="1:345" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A33" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="C33" s="4" t="s">
-        <v>55</v>
-      </c>
-      <c r="D33" s="4" t="s">
-        <v>59</v>
-      </c>
-      <c r="E33" s="4" t="s">
-        <v>61</v>
-      </c>
-      <c r="F33" s="4" t="s">
-        <v>64</v>
-      </c>
-      <c r="G33" s="4" t="s">
-        <v>66</v>
-      </c>
-      <c r="H33" s="4" t="s">
-        <v>68</v>
-      </c>
-      <c r="I33" s="4" t="s">
-        <v>70</v>
-      </c>
-      <c r="L33" s="4" t="s">
-        <v>81</v>
-      </c>
-      <c r="N33" s="4" t="s">
-        <v>91</v>
-      </c>
-      <c r="R33" s="4" t="s">
-        <v>107</v>
-      </c>
-      <c r="T33" s="4" t="s">
-        <v>111</v>
-      </c>
-      <c r="AA33" s="4" t="s">
-        <v>133</v>
-      </c>
-      <c r="AM33" s="4" t="s">
-        <v>175</v>
-      </c>
-      <c r="AN33" s="4" t="s">
-        <v>1097</v>
-      </c>
-      <c r="AQ33" s="4" t="s">
-        <v>196</v>
-      </c>
-      <c r="AR33" s="4" t="s">
-        <v>196</v>
-      </c>
-      <c r="AS33" s="4" t="s">
-        <v>196</v>
-      </c>
-      <c r="BN33" s="4" t="s">
-        <v>293</v>
-      </c>
-      <c r="BP33" s="4" t="s">
-        <v>299</v>
-      </c>
-      <c r="BR33" s="4" t="s">
-        <v>304</v>
-      </c>
-      <c r="BU33" s="4" t="s">
-        <v>315</v>
-      </c>
-      <c r="DH33" s="4" t="s">
-        <v>405</v>
-      </c>
-      <c r="DI33" s="4" t="s">
-        <v>410</v>
-      </c>
-      <c r="DJ33" s="4" t="s">
-        <v>413</v>
-      </c>
-      <c r="DK33" s="4" t="s">
-        <v>415</v>
-      </c>
-      <c r="DL33" s="4" t="s">
-        <v>417</v>
-      </c>
-      <c r="DM33" s="4" t="s">
-        <v>419</v>
-      </c>
-      <c r="DN33" s="4" t="s">
-        <v>421</v>
-      </c>
-      <c r="DO33" s="4" t="s">
-        <v>423</v>
-      </c>
-      <c r="DQ33" s="4" t="s">
-        <v>429</v>
-      </c>
-      <c r="DS33" s="4" t="s">
-        <v>437</v>
-      </c>
-      <c r="EB33" s="4" t="s">
-        <v>463</v>
-      </c>
-      <c r="EK33" s="4" t="s">
-        <v>488</v>
-      </c>
-      <c r="EM33" s="4" t="s">
-        <v>494</v>
-      </c>
-      <c r="ES33" s="4" t="s">
-        <v>512</v>
-      </c>
-      <c r="EU33" s="4" t="s">
-        <v>516</v>
-      </c>
-      <c r="FA33" s="4" t="s">
-        <v>532</v>
-      </c>
-      <c r="FE33" s="4" t="s">
-        <v>545</v>
-      </c>
-      <c r="FG33" s="4" t="s">
-        <v>549</v>
-      </c>
-      <c r="FH33" s="4" t="s">
-        <v>551</v>
-      </c>
-      <c r="FP33" s="4" t="s">
-        <v>573</v>
-      </c>
-      <c r="FQ33" s="4" t="s">
-        <v>575</v>
-      </c>
-      <c r="FR33" s="4" t="s">
-        <v>577</v>
-      </c>
-      <c r="FW33" s="4" t="s">
-        <v>592</v>
-      </c>
-      <c r="FX33" s="4" t="s">
-        <v>595</v>
-      </c>
-      <c r="FY33" s="4" t="s">
-        <v>598</v>
-      </c>
-      <c r="FZ33" s="4" t="s">
-        <v>601</v>
-      </c>
-      <c r="GA33" s="4" t="s">
-        <v>604</v>
-      </c>
-      <c r="GB33" s="4" t="s">
-        <v>607</v>
-      </c>
-      <c r="GC33" s="4" t="s">
-        <v>610</v>
-      </c>
-      <c r="GD33" s="4" t="s">
-        <v>613</v>
-      </c>
-      <c r="GE33" s="4" t="s">
-        <v>616</v>
-      </c>
-      <c r="GN33" s="4" t="s">
-        <v>639</v>
-      </c>
-      <c r="GV33" s="4" t="s">
-        <v>657</v>
-      </c>
-      <c r="GW33" s="4" t="s">
-        <v>659</v>
-      </c>
-      <c r="GX33" s="4" t="s">
-        <v>661</v>
-      </c>
-      <c r="GZ33" s="4" t="s">
-        <v>666</v>
-      </c>
-      <c r="HO33" s="4" t="s">
-        <v>1152</v>
-      </c>
-      <c r="HQ33" s="4" t="s">
-        <v>703</v>
-      </c>
-      <c r="HT33" s="4" t="s">
-        <v>712</v>
-      </c>
-      <c r="HW33" s="4" t="s">
-        <v>725</v>
-      </c>
-      <c r="IN33" s="4" t="s">
-        <v>785</v>
-      </c>
-      <c r="IP33" s="4" t="s">
-        <v>792</v>
-      </c>
-      <c r="IQ33" s="4" t="s">
-        <v>797</v>
-      </c>
-      <c r="IU33" s="4" t="s">
-        <v>810</v>
-      </c>
-      <c r="IV33" s="4" t="s">
-        <v>792</v>
-      </c>
-      <c r="JG33" s="4" t="s">
-        <v>850</v>
-      </c>
-      <c r="JI33" s="4" t="s">
-        <v>857</v>
-      </c>
-      <c r="JJ33" s="4" t="s">
-        <v>860</v>
-      </c>
-      <c r="JN33" s="4" t="s">
-        <v>873</v>
-      </c>
-      <c r="JQ33" s="4" t="s">
-        <v>881</v>
-      </c>
-      <c r="JR33" s="4" t="s">
-        <v>885</v>
-      </c>
-      <c r="JS33" s="4" t="s">
-        <v>887</v>
-      </c>
-      <c r="JT33" s="4" t="s">
-        <v>890</v>
-      </c>
-      <c r="JU33" s="4" t="s">
-        <v>894</v>
-      </c>
-      <c r="JV33" s="4" t="s">
-        <v>897</v>
-      </c>
-      <c r="JX33" s="4" t="s">
-        <v>905</v>
-      </c>
-      <c r="JY33" s="4" t="s">
-        <v>908</v>
-      </c>
-      <c r="KB33" s="4" t="s">
-        <v>916</v>
-      </c>
-      <c r="KC33" s="4" t="s">
-        <v>920</v>
-      </c>
-      <c r="KD33" s="4" t="s">
-        <v>924</v>
-      </c>
-      <c r="KE33" s="4" t="s">
-        <v>928</v>
-      </c>
-      <c r="KF33" s="4" t="s">
-        <v>930</v>
-      </c>
-      <c r="KH33" s="4" t="s">
-        <v>966</v>
-      </c>
-      <c r="KI33" s="4" t="s">
-        <v>936</v>
-      </c>
-      <c r="KK33" s="4" t="s">
-        <v>938</v>
-      </c>
-      <c r="KL33" s="4" t="s">
-        <v>939</v>
-      </c>
-      <c r="KM33" s="4" t="s">
-        <v>972</v>
-      </c>
-      <c r="KP33" s="4" t="s">
-        <v>942</v>
-      </c>
-      <c r="KQ33" s="4" t="s">
-        <v>943</v>
-      </c>
-      <c r="KR33" s="4" t="s">
-        <v>944</v>
-      </c>
-      <c r="KS33" s="4" t="s">
-        <v>945</v>
-      </c>
-      <c r="KU33" s="4" t="s">
-        <v>947</v>
-      </c>
-      <c r="KW33" s="4" t="s">
-        <v>949</v>
-      </c>
-      <c r="LA33" s="4" t="s">
-        <v>1004</v>
-      </c>
-      <c r="LE33" s="4" t="s">
-        <v>957</v>
-      </c>
-      <c r="LG33" s="4" t="s">
-        <v>959</v>
-      </c>
-      <c r="LH33" s="4" t="s">
-        <v>1076</v>
-      </c>
-      <c r="LI33" s="4" t="s">
-        <v>960</v>
-      </c>
-      <c r="LJ33" s="4" t="s">
-        <v>961</v>
-      </c>
-      <c r="LM33" s="4" t="s">
-        <v>964</v>
-      </c>
-      <c r="LO33" s="4" t="s">
-        <v>1099</v>
-      </c>
-      <c r="LQ33" s="4" t="s">
-        <v>1102</v>
-      </c>
-      <c r="LU33" s="4" t="s">
-        <v>1116</v>
-      </c>
-      <c r="LV33" s="4" t="s">
-        <v>1120</v>
-      </c>
-      <c r="LX33" s="4" t="s">
-        <v>1123</v>
-      </c>
-      <c r="LZ33" s="4" t="s">
-        <v>1124</v>
-      </c>
-      <c r="MA33" s="4" t="s">
-        <v>1125</v>
-      </c>
-      <c r="ME33" s="4" t="s">
-        <v>1145</v>
-      </c>
-      <c r="MG33" s="4" t="s">
-        <v>1157</v>
+        <v>1143</v>
+      </c>
+      <c r="KS33" s="4" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="34" spans="1:345" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A34" s="4" t="s">
-        <v>1158</v>
-      </c>
-      <c r="MG34" s="4">
-        <v>1</v>
+        <v>8</v>
+      </c>
+      <c r="C34" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="D34" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="E34" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="F34" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="G34" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="H34" s="4" t="s">
+        <v>68</v>
+      </c>
+      <c r="I34" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="L34" s="4" t="s">
+        <v>81</v>
+      </c>
+      <c r="N34" s="4" t="s">
+        <v>91</v>
+      </c>
+      <c r="R34" s="4" t="s">
+        <v>107</v>
+      </c>
+      <c r="T34" s="4" t="s">
+        <v>111</v>
+      </c>
+      <c r="AA34" s="4" t="s">
+        <v>133</v>
+      </c>
+      <c r="AJ34" s="4" t="s">
+        <v>164</v>
+      </c>
+      <c r="AM34" s="4" t="s">
+        <v>178</v>
+      </c>
+      <c r="AN34" s="4" t="s">
+        <v>1079</v>
+      </c>
+      <c r="AQ34" s="4" t="s">
+        <v>196</v>
+      </c>
+      <c r="AR34" s="4" t="s">
+        <v>196</v>
+      </c>
+      <c r="AS34" s="4" t="s">
+        <v>196</v>
+      </c>
+      <c r="BB34" s="4" t="s">
+        <v>239</v>
+      </c>
+      <c r="BN34" s="4" t="s">
+        <v>293</v>
+      </c>
+      <c r="BP34" s="4" t="s">
+        <v>299</v>
+      </c>
+      <c r="BR34" s="4" t="s">
+        <v>304</v>
+      </c>
+      <c r="BU34" s="4" t="s">
+        <v>315</v>
+      </c>
+      <c r="DH34" s="4" t="s">
+        <v>407</v>
+      </c>
+      <c r="DI34" s="4" t="s">
+        <v>407</v>
+      </c>
+      <c r="DJ34" s="4" t="s">
+        <v>407</v>
+      </c>
+      <c r="DK34" s="4" t="s">
+        <v>407</v>
+      </c>
+      <c r="DL34" s="4" t="s">
+        <v>407</v>
+      </c>
+      <c r="DM34" s="4" t="s">
+        <v>407</v>
+      </c>
+      <c r="DN34" s="4" t="s">
+        <v>407</v>
+      </c>
+      <c r="DO34" s="4" t="s">
+        <v>407</v>
+      </c>
+      <c r="DQ34" s="4" t="s">
+        <v>429</v>
+      </c>
+      <c r="DS34" s="4" t="s">
+        <v>437</v>
+      </c>
+      <c r="EB34" s="4" t="s">
+        <v>463</v>
+      </c>
+      <c r="EK34" s="4" t="s">
+        <v>488</v>
+      </c>
+      <c r="EM34" s="4" t="s">
+        <v>494</v>
+      </c>
+      <c r="ES34" s="4" t="s">
+        <v>512</v>
+      </c>
+      <c r="EU34" s="4" t="s">
+        <v>516</v>
+      </c>
+      <c r="FA34" s="4" t="s">
+        <v>532</v>
+      </c>
+      <c r="FE34" s="4" t="s">
+        <v>463</v>
+      </c>
+      <c r="FG34" s="4" t="s">
+        <v>549</v>
+      </c>
+      <c r="FH34" s="4" t="s">
+        <v>551</v>
+      </c>
+      <c r="FP34" s="4" t="s">
+        <v>573</v>
+      </c>
+      <c r="FQ34" s="4" t="s">
+        <v>575</v>
+      </c>
+      <c r="FR34" s="4" t="s">
+        <v>488</v>
+      </c>
+      <c r="FW34" s="4" t="s">
+        <v>592</v>
+      </c>
+      <c r="FX34" s="4" t="s">
+        <v>595</v>
+      </c>
+      <c r="FY34" s="4" t="s">
+        <v>598</v>
+      </c>
+      <c r="FZ34" s="4" t="s">
+        <v>601</v>
+      </c>
+      <c r="GA34" s="4" t="s">
+        <v>604</v>
+      </c>
+      <c r="GB34" s="4" t="s">
+        <v>607</v>
+      </c>
+      <c r="GC34" s="4" t="s">
+        <v>610</v>
+      </c>
+      <c r="GD34" s="4" t="s">
+        <v>613</v>
+      </c>
+      <c r="GE34" s="4" t="s">
+        <v>616</v>
+      </c>
+      <c r="GN34" s="4" t="s">
+        <v>639</v>
+      </c>
+      <c r="GV34" s="4" t="s">
+        <v>657</v>
+      </c>
+      <c r="GW34" s="4" t="s">
+        <v>659</v>
+      </c>
+      <c r="GX34" s="4" t="s">
+        <v>661</v>
+      </c>
+      <c r="GZ34" s="4" t="s">
+        <v>666</v>
+      </c>
+      <c r="HO34" s="4" t="s">
+        <v>1134</v>
+      </c>
+      <c r="HQ34" s="4" t="s">
+        <v>703</v>
+      </c>
+      <c r="HT34" s="4" t="s">
+        <v>712</v>
+      </c>
+      <c r="HW34" s="4" t="s">
+        <v>725</v>
+      </c>
+      <c r="IN34" s="4" t="s">
+        <v>785</v>
+      </c>
+      <c r="IP34" s="4" t="s">
+        <v>792</v>
+      </c>
+      <c r="IQ34" s="4" t="s">
+        <v>797</v>
+      </c>
+      <c r="IU34" s="4" t="s">
+        <v>810</v>
+      </c>
+      <c r="IV34" s="4" t="s">
+        <v>792</v>
+      </c>
+      <c r="JG34" s="4" t="s">
+        <v>850</v>
+      </c>
+      <c r="JI34" s="4" t="s">
+        <v>857</v>
+      </c>
+      <c r="JJ34" s="4" t="s">
+        <v>862</v>
+      </c>
+      <c r="JN34" s="4" t="s">
+        <v>873</v>
+      </c>
+      <c r="JQ34" s="4" t="s">
+        <v>881</v>
+      </c>
+      <c r="JR34" s="4" t="s">
+        <v>885</v>
+      </c>
+      <c r="JS34" s="4" t="s">
+        <v>887</v>
+      </c>
+      <c r="JT34" s="4" t="s">
+        <v>890</v>
+      </c>
+      <c r="JU34" s="4" t="s">
+        <v>894</v>
+      </c>
+      <c r="JV34" s="4" t="s">
+        <v>897</v>
+      </c>
+      <c r="JX34" s="4" t="s">
+        <v>905</v>
+      </c>
+      <c r="JY34" s="4" t="s">
+        <v>908</v>
+      </c>
+      <c r="KB34" s="4" t="s">
+        <v>916</v>
+      </c>
+      <c r="KC34" s="4" t="s">
+        <v>920</v>
+      </c>
+      <c r="KD34" s="4" t="s">
+        <v>924</v>
+      </c>
+      <c r="KE34" s="4" t="s">
+        <v>928</v>
+      </c>
+      <c r="KF34" s="4" t="s">
+        <v>930</v>
+      </c>
+      <c r="KH34" s="4" t="s">
+        <v>966</v>
+      </c>
+      <c r="KI34" s="4" t="s">
+        <v>936</v>
+      </c>
+      <c r="KK34" s="4" t="s">
+        <v>938</v>
+      </c>
+      <c r="KL34" s="4" t="s">
+        <v>939</v>
+      </c>
+      <c r="KM34" s="4" t="s">
+        <v>972</v>
+      </c>
+      <c r="KP34" s="4" t="s">
+        <v>979</v>
+      </c>
+      <c r="KQ34" s="4" t="s">
+        <v>943</v>
+      </c>
+      <c r="KR34" s="4" t="s">
+        <v>944</v>
+      </c>
+      <c r="KS34" s="4" t="s">
+        <v>945</v>
+      </c>
+      <c r="KU34" s="4" t="s">
+        <v>1065</v>
+      </c>
+      <c r="KW34" s="4" t="s">
+        <v>949</v>
+      </c>
+      <c r="LA34" s="4" t="s">
+        <v>1004</v>
+      </c>
+      <c r="LE34" s="4" t="s">
+        <v>957</v>
+      </c>
+      <c r="LG34" s="4" t="s">
+        <v>959</v>
+      </c>
+      <c r="LH34" s="4" t="s">
+        <v>1060</v>
+      </c>
+      <c r="LI34" s="4" t="s">
+        <v>960</v>
+      </c>
+      <c r="LJ34" s="4" t="s">
+        <v>961</v>
+      </c>
+      <c r="LM34" s="4" t="s">
+        <v>178</v>
+      </c>
+      <c r="LO34" s="4" t="s">
+        <v>1081</v>
+      </c>
+      <c r="LQ34" s="4" t="s">
+        <v>1084</v>
+      </c>
+      <c r="LU34" s="4" t="s">
+        <v>1098</v>
+      </c>
+      <c r="LV34" s="4" t="s">
+        <v>1101</v>
+      </c>
+      <c r="LX34" s="4" t="s">
+        <v>1105</v>
+      </c>
+      <c r="LZ34" s="4" t="s">
+        <v>1106</v>
+      </c>
+      <c r="MA34" s="4" t="s">
+        <v>1107</v>
+      </c>
+      <c r="ME34" s="4" t="s">
+        <v>1127</v>
+      </c>
+      <c r="MG34" s="4" t="s">
+        <v>1138</v>
       </c>
     </row>
-    <row r="35" spans="1:345" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A35" s="7" t="s">
-        <v>29</v>
-      </c>
-      <c r="AQ35" s="7" t="s">
-        <v>198</v>
-      </c>
-      <c r="KS35" s="7" t="s">
-        <v>1037</v>
+    <row r="35" spans="1:345" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A35" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="C35" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="D35" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="E35" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="F35" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="G35" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="H35" s="4" t="s">
+        <v>68</v>
+      </c>
+      <c r="I35" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="L35" s="4" t="s">
+        <v>81</v>
+      </c>
+      <c r="N35" s="4" t="s">
+        <v>91</v>
+      </c>
+      <c r="R35" s="4" t="s">
+        <v>107</v>
+      </c>
+      <c r="T35" s="4" t="s">
+        <v>111</v>
+      </c>
+      <c r="AA35" s="4" t="s">
+        <v>133</v>
+      </c>
+      <c r="AM35" s="4" t="s">
+        <v>175</v>
+      </c>
+      <c r="AN35" s="4" t="s">
+        <v>1079</v>
+      </c>
+      <c r="AQ35" s="4" t="s">
+        <v>196</v>
+      </c>
+      <c r="AR35" s="4" t="s">
+        <v>196</v>
+      </c>
+      <c r="AS35" s="4" t="s">
+        <v>196</v>
+      </c>
+      <c r="BN35" s="4" t="s">
+        <v>293</v>
+      </c>
+      <c r="BP35" s="4" t="s">
+        <v>299</v>
+      </c>
+      <c r="BR35" s="4" t="s">
+        <v>304</v>
+      </c>
+      <c r="BU35" s="4" t="s">
+        <v>315</v>
+      </c>
+      <c r="DH35" s="4" t="s">
+        <v>405</v>
+      </c>
+      <c r="DI35" s="4" t="s">
+        <v>410</v>
+      </c>
+      <c r="DJ35" s="4" t="s">
+        <v>413</v>
+      </c>
+      <c r="DK35" s="4" t="s">
+        <v>415</v>
+      </c>
+      <c r="DL35" s="4" t="s">
+        <v>417</v>
+      </c>
+      <c r="DM35" s="4" t="s">
+        <v>419</v>
+      </c>
+      <c r="DN35" s="4" t="s">
+        <v>421</v>
+      </c>
+      <c r="DO35" s="4" t="s">
+        <v>423</v>
+      </c>
+      <c r="DQ35" s="4" t="s">
+        <v>429</v>
+      </c>
+      <c r="DS35" s="4" t="s">
+        <v>437</v>
+      </c>
+      <c r="EB35" s="4" t="s">
+        <v>463</v>
+      </c>
+      <c r="EK35" s="4" t="s">
+        <v>488</v>
+      </c>
+      <c r="EM35" s="4" t="s">
+        <v>494</v>
+      </c>
+      <c r="ES35" s="4" t="s">
+        <v>512</v>
+      </c>
+      <c r="EU35" s="4" t="s">
+        <v>516</v>
+      </c>
+      <c r="FA35" s="4" t="s">
+        <v>532</v>
+      </c>
+      <c r="FE35" s="4" t="s">
+        <v>545</v>
+      </c>
+      <c r="FG35" s="4" t="s">
+        <v>549</v>
+      </c>
+      <c r="FH35" s="4" t="s">
+        <v>551</v>
+      </c>
+      <c r="FP35" s="4" t="s">
+        <v>573</v>
+      </c>
+      <c r="FQ35" s="4" t="s">
+        <v>575</v>
+      </c>
+      <c r="FR35" s="4" t="s">
+        <v>577</v>
+      </c>
+      <c r="FW35" s="4" t="s">
+        <v>592</v>
+      </c>
+      <c r="FX35" s="4" t="s">
+        <v>595</v>
+      </c>
+      <c r="FY35" s="4" t="s">
+        <v>598</v>
+      </c>
+      <c r="FZ35" s="4" t="s">
+        <v>601</v>
+      </c>
+      <c r="GA35" s="4" t="s">
+        <v>604</v>
+      </c>
+      <c r="GB35" s="4" t="s">
+        <v>607</v>
+      </c>
+      <c r="GC35" s="4" t="s">
+        <v>610</v>
+      </c>
+      <c r="GD35" s="4" t="s">
+        <v>613</v>
+      </c>
+      <c r="GE35" s="4" t="s">
+        <v>616</v>
+      </c>
+      <c r="GN35" s="4" t="s">
+        <v>639</v>
+      </c>
+      <c r="GV35" s="4" t="s">
+        <v>657</v>
+      </c>
+      <c r="GW35" s="4" t="s">
+        <v>659</v>
+      </c>
+      <c r="GX35" s="4" t="s">
+        <v>661</v>
+      </c>
+      <c r="GZ35" s="4" t="s">
+        <v>666</v>
+      </c>
+      <c r="HO35" s="4" t="s">
+        <v>1134</v>
+      </c>
+      <c r="HQ35" s="4" t="s">
+        <v>703</v>
+      </c>
+      <c r="HT35" s="4" t="s">
+        <v>712</v>
+      </c>
+      <c r="HW35" s="4" t="s">
+        <v>725</v>
+      </c>
+      <c r="IN35" s="4" t="s">
+        <v>785</v>
+      </c>
+      <c r="IP35" s="4" t="s">
+        <v>792</v>
+      </c>
+      <c r="IQ35" s="4" t="s">
+        <v>797</v>
+      </c>
+      <c r="IU35" s="4" t="s">
+        <v>810</v>
+      </c>
+      <c r="IV35" s="4" t="s">
+        <v>792</v>
+      </c>
+      <c r="JG35" s="4" t="s">
+        <v>850</v>
+      </c>
+      <c r="JI35" s="4" t="s">
+        <v>857</v>
+      </c>
+      <c r="JJ35" s="4" t="s">
+        <v>860</v>
+      </c>
+      <c r="JN35" s="4" t="s">
+        <v>873</v>
+      </c>
+      <c r="JQ35" s="4" t="s">
+        <v>881</v>
+      </c>
+      <c r="JR35" s="4" t="s">
+        <v>885</v>
+      </c>
+      <c r="JS35" s="4" t="s">
+        <v>887</v>
+      </c>
+      <c r="JT35" s="4" t="s">
+        <v>890</v>
+      </c>
+      <c r="JU35" s="4" t="s">
+        <v>894</v>
+      </c>
+      <c r="JV35" s="4" t="s">
+        <v>897</v>
+      </c>
+      <c r="JX35" s="4" t="s">
+        <v>905</v>
+      </c>
+      <c r="JY35" s="4" t="s">
+        <v>908</v>
+      </c>
+      <c r="KB35" s="4" t="s">
+        <v>916</v>
+      </c>
+      <c r="KC35" s="4" t="s">
+        <v>920</v>
+      </c>
+      <c r="KD35" s="4" t="s">
+        <v>924</v>
+      </c>
+      <c r="KE35" s="4" t="s">
+        <v>928</v>
+      </c>
+      <c r="KF35" s="4" t="s">
+        <v>930</v>
+      </c>
+      <c r="KH35" s="4" t="s">
+        <v>966</v>
+      </c>
+      <c r="KI35" s="4" t="s">
+        <v>936</v>
+      </c>
+      <c r="KK35" s="4" t="s">
+        <v>938</v>
+      </c>
+      <c r="KL35" s="4" t="s">
+        <v>939</v>
+      </c>
+      <c r="KM35" s="4" t="s">
+        <v>972</v>
+      </c>
+      <c r="KP35" s="4" t="s">
+        <v>942</v>
+      </c>
+      <c r="KQ35" s="4" t="s">
+        <v>943</v>
+      </c>
+      <c r="KR35" s="4" t="s">
+        <v>944</v>
+      </c>
+      <c r="KS35" s="4" t="s">
+        <v>945</v>
+      </c>
+      <c r="KU35" s="4" t="s">
+        <v>947</v>
+      </c>
+      <c r="KW35" s="4" t="s">
+        <v>949</v>
+      </c>
+      <c r="LA35" s="4" t="s">
+        <v>1004</v>
+      </c>
+      <c r="LE35" s="4" t="s">
+        <v>957</v>
+      </c>
+      <c r="LG35" s="4" t="s">
+        <v>959</v>
+      </c>
+      <c r="LH35" s="4" t="s">
+        <v>1058</v>
+      </c>
+      <c r="LI35" s="4" t="s">
+        <v>960</v>
+      </c>
+      <c r="LJ35" s="4" t="s">
+        <v>961</v>
+      </c>
+      <c r="LM35" s="4" t="s">
+        <v>964</v>
+      </c>
+      <c r="LO35" s="4" t="s">
+        <v>1081</v>
+      </c>
+      <c r="LQ35" s="4" t="s">
+        <v>1084</v>
+      </c>
+      <c r="LU35" s="4" t="s">
+        <v>1098</v>
+      </c>
+      <c r="LV35" s="4" t="s">
+        <v>1102</v>
+      </c>
+      <c r="LX35" s="4" t="s">
+        <v>1105</v>
+      </c>
+      <c r="LZ35" s="4" t="s">
+        <v>1106</v>
+      </c>
+      <c r="MA35" s="4" t="s">
+        <v>1107</v>
+      </c>
+      <c r="ME35" s="4" t="s">
+        <v>1127</v>
+      </c>
+      <c r="MG35" s="4" t="s">
+        <v>1139</v>
       </c>
     </row>
     <row r="36" spans="1:345" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A36" s="4" t="s">
-        <v>1035</v>
-      </c>
-      <c r="KS36" s="4" t="s">
-        <v>1026</v>
+        <v>1140</v>
+      </c>
+      <c r="MG36" s="4">
+        <v>1</v>
       </c>
     </row>
-    <row r="37" spans="1:345" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A37" s="4" t="s">
-        <v>1094</v>
-      </c>
-      <c r="KS37" s="4" t="b">
-        <v>1</v>
+    <row r="37" spans="1:345" s="7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A37" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="AQ37" s="7" t="s">
+        <v>198</v>
       </c>
     </row>
     <row r="38" spans="1:345" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A38" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="AQ38" s="4">
-        <v>200</v>
+        <v>1026</v>
       </c>
     </row>
     <row r="39" spans="1:345" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A39" s="4" t="s">
-        <v>27</v>
-      </c>
-      <c r="AQ39" s="4" t="s">
-        <v>196</v>
-      </c>
-      <c r="JJ39" s="4" t="s">
-        <v>864</v>
-      </c>
-      <c r="KP39" s="4" t="s">
-        <v>1095</v>
-      </c>
-      <c r="KS39" s="4" t="s">
-        <v>945</v>
+        <v>1076</v>
       </c>
     </row>
     <row r="40" spans="1:345" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A40" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="AQ40" s="4" t="s">
-        <v>196</v>
-      </c>
-      <c r="JJ40" s="4" t="s">
-        <v>860</v>
-      </c>
-      <c r="KP40" s="4" t="s">
-        <v>942</v>
-      </c>
-      <c r="KS40" s="4" t="s">
-        <v>945</v>
+        <v>26</v>
+      </c>
+      <c r="AQ40" s="4">
+        <v>200</v>
       </c>
     </row>
     <row r="41" spans="1:345" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A41" s="4" t="s">
-        <v>47</v>
-      </c>
-      <c r="JJ41" s="4">
-        <v>1</v>
+        <v>27</v>
+      </c>
+      <c r="AQ41" s="4" t="s">
+        <v>196</v>
+      </c>
+      <c r="JJ41" s="4" t="s">
+        <v>864</v>
+      </c>
+      <c r="KP41" s="4" t="s">
+        <v>1077</v>
       </c>
     </row>
-    <row r="42" spans="1:345" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A42" s="7" t="s">
-        <v>33</v>
-      </c>
-      <c r="AQ42" s="7" t="s">
-        <v>199</v>
-      </c>
-      <c r="KS42" s="7" t="s">
-        <v>1036</v>
+    <row r="42" spans="1:345" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A42" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="AQ42" s="4" t="s">
+        <v>196</v>
+      </c>
+      <c r="JJ42" s="4" t="s">
+        <v>860</v>
+      </c>
+      <c r="KP42" s="4" t="s">
+        <v>942</v>
       </c>
     </row>
     <row r="43" spans="1:345" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A43" s="4" t="s">
-        <v>1039</v>
-      </c>
-      <c r="KS43" s="4" t="s">
-        <v>1027</v>
+        <v>47</v>
+      </c>
+      <c r="JJ43" s="4">
+        <v>1</v>
       </c>
     </row>
-    <row r="44" spans="1:345" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A44" s="4" t="s">
-        <v>1093</v>
-      </c>
-      <c r="KS44" s="4" t="b">
-        <v>1</v>
+    <row r="44" spans="1:345" s="7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A44" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="AQ44" s="7" t="s">
+        <v>199</v>
       </c>
     </row>
     <row r="45" spans="1:345" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A45" s="4" t="s">
-        <v>30</v>
-      </c>
-      <c r="AQ45" s="4">
-        <v>500</v>
+        <v>1027</v>
       </c>
     </row>
     <row r="46" spans="1:345" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A46" s="4" t="s">
-        <v>31</v>
-      </c>
-      <c r="AQ46" s="4" t="s">
-        <v>196</v>
-      </c>
-      <c r="KS46" s="4" t="s">
-        <v>945</v>
+        <v>1075</v>
       </c>
     </row>
     <row r="47" spans="1:345" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A47" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="AQ47" s="4">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="48" spans="1:345" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A48" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="AQ48" s="4" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="49" spans="1:338" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A49" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="AQ47" s="4" t="s">
+      <c r="AQ49" s="4" t="s">
         <v>196</v>
       </c>
-      <c r="KS47" s="4" t="s">
-        <v>945</v>
-      </c>
     </row>
-    <row r="48" spans="1:345" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A48" s="7" t="s">
-        <v>1040</v>
-      </c>
-      <c r="KS48" s="7" t="s">
-        <v>1070</v>
+    <row r="50" spans="1:338" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A50" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="AM50" s="5" t="s">
+        <v>181</v>
+      </c>
+      <c r="BL50" s="5" t="s">
+        <v>289</v>
+      </c>
+      <c r="DU50" s="5" t="s">
+        <v>446</v>
+      </c>
+      <c r="FH50" s="5" t="s">
+        <v>446</v>
+      </c>
+      <c r="JW50" s="5" t="s">
+        <v>904</v>
+      </c>
+      <c r="KT50" s="5" t="s">
+        <v>987</v>
+      </c>
+      <c r="LM50" s="5" t="s">
+        <v>181</v>
+      </c>
+      <c r="LP50" s="5" t="s">
+        <v>289</v>
       </c>
     </row>
-    <row r="49" spans="1:305" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A49" s="4" t="s">
-        <v>1041</v>
-      </c>
-      <c r="KS49" s="4" t="s">
-        <v>1029</v>
+    <row r="51" spans="1:338" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A51" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="AM51" s="5" t="s">
+        <v>935</v>
+      </c>
+      <c r="BL51" s="5">
+        <v>1</v>
+      </c>
+      <c r="DU51" s="5">
+        <v>1</v>
+      </c>
+      <c r="FH51" s="5">
+        <v>1</v>
+      </c>
+      <c r="JW51" s="5">
+        <v>4</v>
+      </c>
+      <c r="KT51" s="5" t="s">
+        <v>988</v>
+      </c>
+      <c r="LM51" s="5" t="s">
+        <v>935</v>
+      </c>
+      <c r="LP51" s="5">
+        <v>-1</v>
       </c>
     </row>
-    <row r="50" spans="1:305" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A50" s="4" t="s">
-        <v>1092</v>
-      </c>
-      <c r="KS50" s="4" t="b">
+    <row r="52" spans="1:338" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A52" s="8" t="s">
+        <v>41</v>
+      </c>
+      <c r="HT52" s="8" t="s">
+        <v>718</v>
+      </c>
+      <c r="JX52" s="8" t="s">
+        <v>718</v>
+      </c>
+      <c r="LN52" s="8" t="s">
+        <v>718</v>
+      </c>
+      <c r="LP52" s="8" t="s">
+        <v>718</v>
+      </c>
+    </row>
+    <row r="53" spans="1:338" s="6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A53" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="HT53" s="6">
         <v>1</v>
       </c>
+      <c r="JX53" s="6">
+        <v>2</v>
+      </c>
+      <c r="LN53" s="6">
+        <v>8</v>
+      </c>
+      <c r="LP53" s="6">
+        <v>0</v>
+      </c>
     </row>
-    <row r="51" spans="1:305" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A51" s="4" t="s">
-        <v>1042</v>
+    <row r="54" spans="1:338" s="6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A54" s="6" t="s">
+        <v>39</v>
+      </c>
+      <c r="HT54" s="6" t="s">
+        <v>717</v>
+      </c>
+      <c r="JX54" s="6" t="s">
+        <v>907</v>
+      </c>
+      <c r="LN54" s="6" t="s">
+        <v>1022</v>
+      </c>
+      <c r="LP54" s="6" t="s">
+        <v>1091</v>
       </c>
     </row>
-    <row r="52" spans="1:305" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A52" s="4" t="s">
-        <v>1043</v>
-      </c>
-      <c r="KS52" s="4" t="s">
-        <v>945</v>
+    <row r="55" spans="1:338" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A55" s="8" t="s">
+        <v>44</v>
+      </c>
+      <c r="HT55" s="8" t="s">
+        <v>718</v>
       </c>
     </row>
-    <row r="53" spans="1:305" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A53" s="4" t="s">
-        <v>1044</v>
-      </c>
-      <c r="KS53" s="4" t="s">
-        <v>945</v>
+    <row r="56" spans="1:338" s="6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A56" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="HT56" s="6">
+        <v>3</v>
       </c>
     </row>
-    <row r="54" spans="1:305" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A54" s="7" t="s">
-        <v>1045</v>
-      </c>
-      <c r="KS54" s="7" t="s">
-        <v>1071</v>
+    <row r="57" spans="1:338" s="6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A57" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="HT57" s="6" t="s">
+        <v>717</v>
       </c>
     </row>
-    <row r="55" spans="1:305" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A55" s="4" t="s">
-        <v>1046</v>
-      </c>
-      <c r="KS55" s="4" t="s">
-        <v>1030</v>
+    <row r="58" spans="1:338" x14ac:dyDescent="0.25">
+      <c r="A58" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="JX58" s="1" t="s">
+        <v>908</v>
       </c>
     </row>
-    <row r="56" spans="1:305" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A56" s="4" t="s">
-        <v>1091</v>
-      </c>
-      <c r="KS56" s="4" t="b">
-        <v>1</v>
+    <row r="59" spans="1:338" x14ac:dyDescent="0.25">
+      <c r="A59" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="IP59" s="1">
+        <v>6</v>
+      </c>
+      <c r="JT59" s="1">
+        <v>5</v>
+      </c>
+      <c r="KS59" s="1">
+        <v>3</v>
+      </c>
+      <c r="LG59" s="1">
+        <v>6</v>
+      </c>
+      <c r="LZ59" s="1">
+        <v>10</v>
       </c>
     </row>
-    <row r="57" spans="1:305" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A57" s="4" t="s">
-        <v>1047</v>
-      </c>
-    </row>
-    <row r="58" spans="1:305" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A58" s="4" t="s">
-        <v>1048</v>
-      </c>
-      <c r="KS58" s="4" t="s">
-        <v>945</v>
-      </c>
-    </row>
-    <row r="59" spans="1:305" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A59" s="4" t="s">
-        <v>1049</v>
-      </c>
-      <c r="KS59" s="4" t="s">
-        <v>945</v>
-      </c>
-    </row>
-    <row r="60" spans="1:305" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A60" s="7" t="s">
-        <v>1050</v>
-      </c>
-      <c r="KS60" s="7" t="s">
-        <v>1072</v>
-      </c>
-    </row>
-    <row r="61" spans="1:305" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A61" s="4" t="s">
-        <v>1051</v>
-      </c>
-      <c r="KS61" s="4" t="s">
-        <v>1031</v>
-      </c>
-    </row>
-    <row r="62" spans="1:305" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A62" s="4" t="s">
-        <v>1090</v>
-      </c>
-      <c r="KS62" s="4" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="63" spans="1:305" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A63" s="4" t="s">
-        <v>1052</v>
-      </c>
-    </row>
-    <row r="64" spans="1:305" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A64" s="4" t="s">
-        <v>1053</v>
-      </c>
-      <c r="KS64" s="4" t="s">
-        <v>945</v>
-      </c>
-    </row>
-    <row r="65" spans="1:305" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A65" s="4" t="s">
-        <v>1054</v>
-      </c>
-      <c r="KS65" s="4" t="s">
-        <v>945</v>
-      </c>
-    </row>
-    <row r="66" spans="1:305" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A66" s="7" t="s">
-        <v>1055</v>
-      </c>
-      <c r="KS66" s="7" t="s">
-        <v>1073</v>
-      </c>
-    </row>
-    <row r="67" spans="1:305" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A67" s="4" t="s">
-        <v>1056</v>
-      </c>
-      <c r="KS67" s="4" t="s">
-        <v>1032</v>
-      </c>
-    </row>
-    <row r="68" spans="1:305" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A68" s="4" t="s">
-        <v>1089</v>
-      </c>
-      <c r="KS68" s="4" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="69" spans="1:305" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A69" s="4" t="s">
-        <v>1057</v>
-      </c>
-    </row>
-    <row r="70" spans="1:305" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A70" s="4" t="s">
-        <v>1058</v>
-      </c>
-      <c r="KS70" s="4" t="s">
-        <v>945</v>
-      </c>
-    </row>
-    <row r="71" spans="1:305" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A71" s="4" t="s">
-        <v>1059</v>
-      </c>
-      <c r="KS71" s="4" t="s">
-        <v>945</v>
-      </c>
-    </row>
-    <row r="72" spans="1:305" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A72" s="7" t="s">
-        <v>1060</v>
-      </c>
-      <c r="KS72" s="7" t="s">
-        <v>1074</v>
-      </c>
-    </row>
-    <row r="73" spans="1:305" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A73" s="4" t="s">
-        <v>1061</v>
-      </c>
-      <c r="KS73" s="4" t="s">
-        <v>1033</v>
-      </c>
-    </row>
-    <row r="74" spans="1:305" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A74" s="4" t="s">
-        <v>1088</v>
-      </c>
-      <c r="KS74" s="4" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="75" spans="1:305" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A75" s="4" t="s">
-        <v>1062</v>
-      </c>
-    </row>
-    <row r="76" spans="1:305" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A76" s="4" t="s">
-        <v>1063</v>
-      </c>
-      <c r="KS76" s="4" t="s">
-        <v>945</v>
-      </c>
-    </row>
-    <row r="77" spans="1:305" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A77" s="4" t="s">
-        <v>1064</v>
-      </c>
-      <c r="KS77" s="4" t="s">
-        <v>945</v>
-      </c>
-    </row>
-    <row r="78" spans="1:305" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A78" s="7" t="s">
-        <v>1065</v>
-      </c>
-      <c r="KS78" s="7" t="s">
-        <v>1075</v>
-      </c>
-    </row>
-    <row r="79" spans="1:305" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A79" s="4" t="s">
-        <v>1066</v>
-      </c>
-      <c r="KS79" s="4" t="s">
-        <v>1028</v>
-      </c>
-    </row>
-    <row r="80" spans="1:305" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A80" s="4" t="s">
-        <v>1087</v>
-      </c>
-      <c r="KS80" s="4" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="81" spans="1:338" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A81" s="4" t="s">
-        <v>1067</v>
-      </c>
-    </row>
-    <row r="82" spans="1:338" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A82" s="4" t="s">
-        <v>1068</v>
-      </c>
-      <c r="KS82" s="4" t="s">
-        <v>945</v>
-      </c>
-    </row>
-    <row r="83" spans="1:338" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A83" s="4" t="s">
-        <v>1069</v>
-      </c>
-      <c r="KS83" s="4" t="s">
-        <v>945</v>
-      </c>
-    </row>
-    <row r="84" spans="1:338" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A84" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="AM84" s="5" t="s">
-        <v>181</v>
-      </c>
-      <c r="BL84" s="5" t="s">
-        <v>289</v>
-      </c>
-      <c r="DU84" s="5" t="s">
-        <v>446</v>
-      </c>
-      <c r="FH84" s="5" t="s">
-        <v>446</v>
-      </c>
-      <c r="JW84" s="5" t="s">
-        <v>904</v>
-      </c>
-      <c r="KT84" s="5" t="s">
-        <v>987</v>
-      </c>
-      <c r="LM84" s="5" t="s">
-        <v>181</v>
-      </c>
-      <c r="LP84" s="5" t="s">
-        <v>289</v>
-      </c>
-    </row>
-    <row r="85" spans="1:338" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A85" s="5" t="s">
-        <v>24</v>
-      </c>
-      <c r="AM85" s="5" t="s">
-        <v>935</v>
-      </c>
-      <c r="BL85" s="5">
-        <v>1</v>
-      </c>
-      <c r="DU85" s="5">
-        <v>1</v>
-      </c>
-      <c r="FH85" s="5">
-        <v>1</v>
-      </c>
-      <c r="JW85" s="5">
-        <v>4</v>
-      </c>
-      <c r="KT85" s="5" t="s">
-        <v>988</v>
-      </c>
-      <c r="LM85" s="5" t="s">
-        <v>935</v>
-      </c>
-      <c r="LP85" s="5">
-        <v>-1</v>
-      </c>
-    </row>
-    <row r="86" spans="1:338" s="8" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A86" s="8" t="s">
-        <v>41</v>
-      </c>
-      <c r="HT86" s="8" t="s">
-        <v>718</v>
-      </c>
-      <c r="JX86" s="8" t="s">
-        <v>718</v>
-      </c>
-      <c r="LN86" s="8" t="s">
-        <v>718</v>
-      </c>
-      <c r="LP86" s="8" t="s">
-        <v>718</v>
-      </c>
-    </row>
-    <row r="87" spans="1:338" s="6" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A87" s="6" t="s">
-        <v>40</v>
-      </c>
-      <c r="HT87" s="6">
-        <v>1</v>
-      </c>
-      <c r="JX87" s="6">
-        <v>2</v>
-      </c>
-      <c r="LN87" s="6">
-        <v>8</v>
-      </c>
-      <c r="LP87" s="6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="88" spans="1:338" s="6" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A88" s="6" t="s">
-        <v>39</v>
-      </c>
-      <c r="HT88" s="6" t="s">
-        <v>717</v>
-      </c>
-      <c r="JX88" s="6" t="s">
-        <v>907</v>
-      </c>
-      <c r="LN88" s="6" t="s">
-        <v>1022</v>
-      </c>
-      <c r="LP88" s="6" t="s">
-        <v>1109</v>
-      </c>
-    </row>
-    <row r="89" spans="1:338" s="8" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A89" s="8" t="s">
-        <v>44</v>
-      </c>
-      <c r="HT89" s="8" t="s">
-        <v>718</v>
-      </c>
-    </row>
-    <row r="90" spans="1:338" s="6" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A90" s="6" t="s">
-        <v>43</v>
-      </c>
-      <c r="HT90" s="6">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="91" spans="1:338" s="6" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A91" s="6" t="s">
-        <v>42</v>
-      </c>
-      <c r="HT91" s="6" t="s">
-        <v>717</v>
-      </c>
-    </row>
-    <row r="92" spans="1:338" x14ac:dyDescent="0.25">
-      <c r="A92" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="JX92" s="1" t="s">
-        <v>908</v>
-      </c>
-    </row>
-    <row r="93" spans="1:338" x14ac:dyDescent="0.25">
-      <c r="A93" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="IP93" s="1">
-        <v>6</v>
-      </c>
-      <c r="JT93" s="1">
-        <v>5</v>
-      </c>
-      <c r="KS93" s="1">
-        <v>3</v>
-      </c>
-      <c r="LG93" s="1">
-        <v>6</v>
-      </c>
-      <c r="LZ93" s="1">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="94" spans="1:338" x14ac:dyDescent="0.25">
-      <c r="A94" s="1" t="s">
+    <row r="60" spans="1:338" x14ac:dyDescent="0.25">
+      <c r="A60" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="IP94" s="1" t="s">
+      <c r="IP60" s="1" t="s">
         <v>794</v>
       </c>
-      <c r="JT94" s="1" t="s">
+      <c r="JT60" s="1" t="s">
         <v>893</v>
       </c>
-      <c r="KS94" s="1" t="s">
+      <c r="KS60" s="1" t="s">
         <v>991</v>
       </c>
-      <c r="LG94" s="1" t="s">
-        <v>1096</v>
-      </c>
-      <c r="LZ94" s="1" t="s">
-        <v>1129</v>
+      <c r="LG60" s="1" t="s">
+        <v>1078</v>
+      </c>
+      <c r="LZ60" s="1" t="s">
+        <v>1111</v>
       </c>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A86:KG94">
-    <sortCondition ref="A86:A94"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A52:KG60">
+    <sortCondition ref="A52:A60"/>
   </sortState>
   <conditionalFormatting sqref="LT1:LW1 A1:LR1 MD1 MG1:XFD1">
     <cfRule type="duplicateValues" dxfId="3" priority="4"/>

</xml_diff>

<commit_message>
Added amount to consumable gridicons Some cleanup of constructor conditionals Started adding targets to activities
</commit_message>
<xml_diff>
--- a/work assets/activities.xlsx
+++ b/work assets/activities.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23901"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23929"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/eb76e5660c890129/Personal/Projects/Design/PECS/PECS/work assets/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="644" documentId="13_ncr:40009_{E3EB266C-7612-416D-8781-7A2BED99FA57}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{C9727751-91A3-44D6-B368-6CB358771C20}"/>
+  <xr:revisionPtr revIDLastSave="672" documentId="13_ncr:40009_{E3EB266C-7612-416D-8781-7A2BED99FA57}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{A9552DB2-A3AF-4F44-AF75-D2839D0CA2AC}"/>
   <bookViews>
-    <workbookView xWindow="4935" yWindow="2535" windowWidth="57600" windowHeight="15435" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="77040" windowHeight="21240" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="activities" sheetId="1" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2622" uniqueCount="1142">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2647" uniqueCount="1145">
   <si>
     <t>name</t>
   </si>
@@ -3586,6 +3586,15 @@
   </si>
   <si>
     <t>gainConditions/0/choiceBySubType</t>
+  </si>
+  <si>
+    <t>other</t>
+  </si>
+  <si>
+    <t>self</t>
+  </si>
+  <si>
+    <t>area</t>
   </si>
 </sst>
 </file>
@@ -5247,13 +5256,13 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:ME60"/>
+  <dimension ref="A1:ME61"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="AH2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="AQ1" sqref="AQ1:AQ1048576"/>
+      <selection pane="bottomRight" activeCell="AA21" sqref="AA21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -10963,2016 +10972,1758 @@
       </c>
     </row>
     <row r="21" spans="1:343" x14ac:dyDescent="0.25">
-      <c r="A21" s="1" t="s">
-        <v>2</v>
-      </c>
       <c r="B21" s="1" t="s">
-        <v>52</v>
+        <v>1142</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>56</v>
+        <v>1143</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>60</v>
+        <v>1143</v>
       </c>
       <c r="E21" s="1" t="s">
-        <v>62</v>
+        <v>1143</v>
       </c>
       <c r="F21" s="1" t="s">
-        <v>65</v>
+        <v>1143</v>
       </c>
       <c r="G21" s="1" t="s">
-        <v>67</v>
+        <v>1143</v>
       </c>
       <c r="H21" s="1" t="s">
-        <v>69</v>
+        <v>1143</v>
       </c>
       <c r="I21" s="1" t="s">
-        <v>72</v>
+        <v>1143</v>
       </c>
       <c r="J21" s="1" t="s">
-        <v>77</v>
+        <v>1142</v>
       </c>
       <c r="K21" s="1" t="s">
-        <v>79</v>
+        <v>1142</v>
       </c>
       <c r="L21" s="1" t="s">
-        <v>82</v>
+        <v>1143</v>
       </c>
       <c r="M21" s="1" t="s">
-        <v>85</v>
+        <v>1144</v>
       </c>
       <c r="N21" s="1" t="s">
-        <v>92</v>
+        <v>1143</v>
       </c>
       <c r="O21" s="1" t="s">
-        <v>95</v>
+        <v>1142</v>
       </c>
       <c r="P21" s="1" t="s">
-        <v>98</v>
+        <v>1142</v>
       </c>
       <c r="Q21" s="1" t="s">
-        <v>105</v>
+        <v>1142</v>
       </c>
       <c r="R21" s="1" t="s">
-        <v>108</v>
+        <v>1143</v>
       </c>
       <c r="S21" s="1" t="s">
-        <v>110</v>
+        <v>1142</v>
       </c>
       <c r="T21" s="1" t="s">
-        <v>112</v>
+        <v>1143</v>
       </c>
       <c r="U21" s="1" t="s">
-        <v>114</v>
+        <v>1143</v>
       </c>
       <c r="V21" s="1" t="s">
-        <v>116</v>
+        <v>1142</v>
       </c>
       <c r="W21" s="1" t="s">
-        <v>118</v>
+        <v>1142</v>
       </c>
       <c r="X21" s="1" t="s">
-        <v>124</v>
+        <v>1143</v>
       </c>
       <c r="Y21" s="1" t="s">
-        <v>127</v>
+        <v>1142</v>
       </c>
       <c r="Z21" s="1" t="s">
-        <v>131</v>
-      </c>
-      <c r="AA21" s="1" t="s">
-        <v>134</v>
-      </c>
-      <c r="AB21" s="1" t="s">
-        <v>137</v>
-      </c>
-      <c r="AC21" s="1" t="s">
-        <v>139</v>
-      </c>
-      <c r="AD21" s="1" t="s">
-        <v>142</v>
-      </c>
-      <c r="AE21" s="1" t="s">
-        <v>145</v>
-      </c>
-      <c r="AF21" s="1" t="s">
-        <v>147</v>
-      </c>
-      <c r="AG21" s="1" t="s">
-        <v>154</v>
-      </c>
-      <c r="AH21" s="1" t="s">
-        <v>158</v>
-      </c>
-      <c r="AI21" s="1" t="s">
-        <v>163</v>
-      </c>
-      <c r="AJ21" s="1" t="s">
-        <v>165</v>
-      </c>
-      <c r="AK21" s="1" t="s">
-        <v>168</v>
-      </c>
-      <c r="AL21" s="1" t="s">
-        <v>171</v>
-      </c>
-      <c r="AM21" s="1" t="s">
-        <v>176</v>
-      </c>
-      <c r="AN21" s="1" t="s">
-        <v>183</v>
-      </c>
-      <c r="AO21" s="1" t="s">
-        <v>186</v>
-      </c>
-      <c r="AP21" s="1" t="s">
-        <v>189</v>
-      </c>
-      <c r="AQ21" s="1" t="s">
-        <v>193</v>
-      </c>
-      <c r="AR21" s="1" t="s">
-        <v>200</v>
-      </c>
-      <c r="AS21" s="1" t="s">
-        <v>202</v>
-      </c>
-      <c r="AT21" s="1" t="s">
-        <v>205</v>
-      </c>
-      <c r="AU21" s="1" t="s">
-        <v>207</v>
-      </c>
-      <c r="AV21" s="1" t="s">
-        <v>215</v>
-      </c>
-      <c r="AW21" s="1" t="s">
-        <v>218</v>
-      </c>
-      <c r="AX21" s="1" t="s">
-        <v>226</v>
-      </c>
-      <c r="AY21" s="1" t="s">
-        <v>228</v>
-      </c>
-      <c r="AZ21" s="1" t="s">
-        <v>235</v>
-      </c>
-      <c r="BA21" s="1" t="s">
-        <v>241</v>
-      </c>
-      <c r="BB21" s="1" t="s">
-        <v>247</v>
-      </c>
-      <c r="BC21" s="1" t="s">
-        <v>252</v>
-      </c>
-      <c r="BD21" s="1" t="s">
-        <v>257</v>
-      </c>
-      <c r="BE21" s="1" t="s">
-        <v>257</v>
-      </c>
-      <c r="BF21" s="1" t="s">
-        <v>257</v>
-      </c>
-      <c r="BG21" s="1" t="s">
-        <v>257</v>
-      </c>
-      <c r="BH21" s="1" t="s">
-        <v>257</v>
-      </c>
-      <c r="BI21" s="1" t="s">
-        <v>279</v>
-      </c>
-      <c r="BJ21" s="1" t="s">
-        <v>285</v>
-      </c>
-      <c r="BK21" s="1" t="s">
-        <v>288</v>
-      </c>
-      <c r="BL21" s="1" t="s">
-        <v>291</v>
-      </c>
-      <c r="BM21" s="1" t="s">
-        <v>294</v>
-      </c>
-      <c r="BN21" s="1" t="s">
-        <v>297</v>
-      </c>
-      <c r="BO21" s="1" t="s">
-        <v>300</v>
-      </c>
-      <c r="BP21" s="1" t="s">
-        <v>302</v>
-      </c>
-      <c r="BQ21" s="1" t="s">
-        <v>304</v>
-      </c>
-      <c r="BR21" s="1" t="s">
-        <v>309</v>
-      </c>
-      <c r="BS21" s="1" t="s">
-        <v>313</v>
-      </c>
-      <c r="BT21" s="1" t="s">
-        <v>316</v>
-      </c>
-      <c r="BU21" s="1" t="s">
-        <v>319</v>
-      </c>
-      <c r="BV21" s="1" t="s">
-        <v>323</v>
-      </c>
-      <c r="BW21" s="1" t="s">
-        <v>329</v>
-      </c>
-      <c r="BX21" s="1" t="s">
-        <v>331</v>
-      </c>
-      <c r="BY21" s="1" t="s">
-        <v>335</v>
-      </c>
-      <c r="BZ21" s="1" t="s">
-        <v>338</v>
-      </c>
-      <c r="CA21" s="1" t="s">
-        <v>343</v>
-      </c>
-      <c r="CB21" s="1" t="s">
-        <v>347</v>
-      </c>
-      <c r="CC21" s="1" t="s">
-        <v>347</v>
-      </c>
-      <c r="CD21" s="1" t="s">
-        <v>355</v>
-      </c>
-      <c r="CE21" s="1" t="s">
-        <v>355</v>
-      </c>
-      <c r="CF21" s="1" t="s">
-        <v>359</v>
-      </c>
-      <c r="CG21" s="1" t="s">
-        <v>362</v>
-      </c>
-      <c r="CH21" s="1" t="s">
-        <v>365</v>
-      </c>
-      <c r="CI21" s="1" t="s">
-        <v>365</v>
-      </c>
-      <c r="CJ21" s="1" t="s">
-        <v>368</v>
-      </c>
-      <c r="CK21" s="1" t="s">
-        <v>368</v>
-      </c>
-      <c r="CL21" s="1" t="s">
-        <v>371</v>
-      </c>
-      <c r="CM21" s="1" t="s">
-        <v>371</v>
-      </c>
-      <c r="CN21" s="1" t="s">
-        <v>374</v>
-      </c>
-      <c r="CO21" s="1" t="s">
-        <v>374</v>
-      </c>
-      <c r="CP21" s="1" t="s">
-        <v>377</v>
-      </c>
-      <c r="CQ21" s="1" t="s">
-        <v>379</v>
-      </c>
-      <c r="CR21" s="1" t="s">
-        <v>381</v>
-      </c>
-      <c r="CS21" s="1" t="s">
-        <v>381</v>
-      </c>
-      <c r="CT21" s="1" t="s">
-        <v>384</v>
-      </c>
-      <c r="CU21" s="1" t="s">
-        <v>384</v>
-      </c>
-      <c r="CV21" s="1" t="s">
-        <v>387</v>
-      </c>
-      <c r="CW21" s="1" t="s">
-        <v>387</v>
-      </c>
-      <c r="CX21" s="1" t="s">
-        <v>390</v>
-      </c>
-      <c r="CY21" s="1" t="s">
-        <v>390</v>
-      </c>
-      <c r="CZ21" s="1" t="s">
-        <v>393</v>
-      </c>
-      <c r="DA21" s="1" t="s">
-        <v>395</v>
-      </c>
-      <c r="DB21" s="1" t="s">
-        <v>397</v>
-      </c>
-      <c r="DC21" s="1" t="s">
-        <v>397</v>
-      </c>
-      <c r="DD21" s="1" t="s">
-        <v>400</v>
-      </c>
-      <c r="DE21" s="1" t="s">
-        <v>400</v>
-      </c>
-      <c r="DF21" s="1" t="s">
-        <v>403</v>
-      </c>
-      <c r="DG21" s="1" t="s">
-        <v>408</v>
-      </c>
-      <c r="DH21" s="1" t="s">
-        <v>411</v>
-      </c>
-      <c r="DI21" s="1" t="s">
-        <v>413</v>
-      </c>
-      <c r="DJ21" s="1" t="s">
-        <v>415</v>
-      </c>
-      <c r="DK21" s="1" t="s">
-        <v>417</v>
-      </c>
-      <c r="DL21" s="1" t="s">
-        <v>419</v>
-      </c>
-      <c r="DM21" s="1" t="s">
-        <v>421</v>
-      </c>
-      <c r="DN21" s="1" t="s">
-        <v>423</v>
-      </c>
-      <c r="DO21" s="1" t="s">
-        <v>427</v>
-      </c>
-      <c r="DP21" s="1" t="s">
-        <v>431</v>
-      </c>
-      <c r="DQ21" s="1" t="s">
-        <v>435</v>
-      </c>
-      <c r="DR21" s="1" t="s">
-        <v>439</v>
-      </c>
-      <c r="DS21" s="1" t="s">
-        <v>441</v>
-      </c>
-      <c r="DT21" s="1" t="s">
-        <v>445</v>
-      </c>
-      <c r="DU21" s="1" t="s">
-        <v>448</v>
-      </c>
-      <c r="DV21" s="1" t="s">
-        <v>450</v>
-      </c>
-      <c r="DW21" s="1" t="s">
-        <v>453</v>
-      </c>
-      <c r="DX21" s="1" t="s">
-        <v>455</v>
-      </c>
-      <c r="DY21" s="1" t="s">
-        <v>459</v>
-      </c>
-      <c r="DZ21" s="1" t="s">
-        <v>461</v>
-      </c>
-      <c r="EA21" s="1" t="s">
-        <v>464</v>
-      </c>
-      <c r="EB21" s="1" t="s">
-        <v>466</v>
-      </c>
-      <c r="EC21" s="1" t="s">
-        <v>469</v>
-      </c>
-      <c r="ED21" s="1" t="s">
-        <v>472</v>
-      </c>
-      <c r="EE21" s="1" t="s">
-        <v>475</v>
-      </c>
-      <c r="EF21" s="1" t="s">
-        <v>479</v>
-      </c>
-      <c r="EG21" s="1" t="s">
-        <v>481</v>
-      </c>
-      <c r="EH21" s="1" t="s">
-        <v>484</v>
-      </c>
-      <c r="EI21" s="1" t="s">
-        <v>486</v>
-      </c>
-      <c r="EJ21" s="1" t="s">
-        <v>489</v>
-      </c>
-      <c r="EK21" s="1" t="s">
-        <v>492</v>
-      </c>
-      <c r="EL21" s="1" t="s">
-        <v>494</v>
-      </c>
-      <c r="EM21" s="1" t="s">
-        <v>498</v>
-      </c>
-      <c r="EN21" s="1" t="s">
-        <v>501</v>
-      </c>
-      <c r="EO21" s="1" t="s">
-        <v>504</v>
-      </c>
-      <c r="EP21" s="1" t="s">
-        <v>508</v>
-      </c>
-      <c r="EQ21" s="1" t="s">
-        <v>510</v>
-      </c>
-      <c r="ER21" s="1" t="s">
-        <v>512</v>
-      </c>
-      <c r="ES21" s="1" t="s">
-        <v>514</v>
-      </c>
-      <c r="ET21" s="1" t="s">
-        <v>516</v>
-      </c>
-      <c r="EU21" s="1" t="s">
-        <v>519</v>
-      </c>
-      <c r="EV21" s="1" t="s">
-        <v>522</v>
-      </c>
-      <c r="EW21" s="1" t="s">
-        <v>525</v>
-      </c>
-      <c r="EX21" s="1" t="s">
-        <v>527</v>
-      </c>
-      <c r="EY21" s="1" t="s">
-        <v>530</v>
-      </c>
-      <c r="EZ21" s="1" t="s">
-        <v>532</v>
-      </c>
-      <c r="FA21" s="1" t="s">
-        <v>536</v>
-      </c>
-      <c r="FB21" s="1" t="s">
-        <v>539</v>
-      </c>
-      <c r="FC21" s="1" t="s">
-        <v>543</v>
-      </c>
-      <c r="FD21" s="1" t="s">
-        <v>545</v>
-      </c>
-      <c r="FE21" s="1" t="s">
-        <v>547</v>
-      </c>
-      <c r="FF21" s="1" t="s">
-        <v>549</v>
-      </c>
-      <c r="FG21" s="1" t="s">
-        <v>551</v>
-      </c>
-      <c r="FH21" s="1" t="s">
-        <v>554</v>
-      </c>
-      <c r="FI21" s="1" t="s">
-        <v>558</v>
-      </c>
-      <c r="FJ21" s="1" t="s">
-        <v>561</v>
-      </c>
-      <c r="FK21" s="1" t="s">
-        <v>564</v>
-      </c>
-      <c r="FL21" s="1" t="s">
-        <v>566</v>
-      </c>
-      <c r="FM21" s="1" t="s">
-        <v>569</v>
-      </c>
-      <c r="FN21" s="1" t="s">
-        <v>571</v>
-      </c>
-      <c r="FO21" s="1" t="s">
-        <v>573</v>
-      </c>
-      <c r="FP21" s="1" t="s">
-        <v>575</v>
-      </c>
-      <c r="FQ21" s="1" t="s">
-        <v>577</v>
-      </c>
-      <c r="FR21" s="1" t="s">
-        <v>581</v>
-      </c>
-      <c r="FS21" s="1" t="s">
-        <v>586</v>
-      </c>
-      <c r="FT21" s="1" t="s">
-        <v>588</v>
-      </c>
-      <c r="FU21" s="1" t="s">
-        <v>590</v>
-      </c>
-      <c r="FV21" s="1" t="s">
-        <v>593</v>
-      </c>
-      <c r="FW21" s="1" t="s">
-        <v>596</v>
-      </c>
-      <c r="FX21" s="1" t="s">
-        <v>599</v>
-      </c>
-      <c r="FY21" s="1" t="s">
-        <v>602</v>
-      </c>
-      <c r="FZ21" s="1" t="s">
-        <v>605</v>
-      </c>
-      <c r="GA21" s="1" t="s">
-        <v>608</v>
-      </c>
-      <c r="GB21" s="1" t="s">
-        <v>611</v>
-      </c>
-      <c r="GC21" s="1" t="s">
-        <v>614</v>
-      </c>
-      <c r="GD21" s="1" t="s">
-        <v>617</v>
-      </c>
-      <c r="GE21" s="1" t="s">
-        <v>619</v>
-      </c>
-      <c r="GF21" s="1" t="s">
-        <v>621</v>
-      </c>
-      <c r="GG21" s="1" t="s">
-        <v>625</v>
-      </c>
-      <c r="GH21" s="1" t="s">
-        <v>628</v>
-      </c>
-      <c r="GI21" s="1" t="s">
-        <v>630</v>
-      </c>
-      <c r="GJ21" s="1" t="s">
-        <v>633</v>
-      </c>
-      <c r="GK21" s="1" t="s">
-        <v>635</v>
-      </c>
-      <c r="GL21" s="1" t="s">
-        <v>638</v>
-      </c>
-      <c r="GM21" s="1" t="s">
-        <v>640</v>
-      </c>
-      <c r="GN21" s="1" t="s">
-        <v>642</v>
-      </c>
-      <c r="GO21" s="1" t="s">
-        <v>644</v>
-      </c>
-      <c r="GP21" s="1" t="s">
-        <v>647</v>
-      </c>
-      <c r="GQ21" s="1" t="s">
-        <v>650</v>
-      </c>
-      <c r="GR21" s="1" t="s">
-        <v>652</v>
-      </c>
-      <c r="GS21" s="1" t="s">
-        <v>577</v>
-      </c>
-      <c r="GT21" s="1" t="s">
-        <v>655</v>
-      </c>
-      <c r="GU21" s="1" t="s">
-        <v>657</v>
-      </c>
-      <c r="GV21" s="1" t="s">
-        <v>659</v>
-      </c>
-      <c r="GW21" s="1" t="s">
-        <v>661</v>
-      </c>
-      <c r="GX21" s="1" t="s">
-        <v>664</v>
-      </c>
-      <c r="GY21" s="1" t="s">
-        <v>667</v>
-      </c>
-      <c r="GZ21" s="1" t="s">
-        <v>669</v>
-      </c>
-      <c r="HA21" s="1" t="s">
-        <v>174</v>
-      </c>
-      <c r="HB21" s="1" t="s">
-        <v>671</v>
-      </c>
-      <c r="HC21" s="1" t="s">
-        <v>673</v>
-      </c>
-      <c r="HD21" s="1" t="s">
-        <v>675</v>
-      </c>
-      <c r="HE21" s="1" t="s">
-        <v>677</v>
-      </c>
-      <c r="HF21" s="1" t="s">
-        <v>679</v>
-      </c>
-      <c r="HG21" s="1" t="s">
-        <v>682</v>
-      </c>
-      <c r="HH21" s="1" t="s">
-        <v>684</v>
-      </c>
-      <c r="HI21" s="1" t="s">
-        <v>687</v>
-      </c>
-      <c r="HJ21" s="1" t="s">
-        <v>690</v>
-      </c>
-      <c r="HK21" s="1" t="s">
-        <v>692</v>
-      </c>
-      <c r="HL21" s="1" t="s">
-        <v>696</v>
-      </c>
-      <c r="HM21" s="1" t="s">
-        <v>1130</v>
-      </c>
-      <c r="HN21" s="1" t="s">
-        <v>699</v>
-      </c>
-      <c r="HO21" s="1" t="s">
-        <v>701</v>
-      </c>
-      <c r="HP21" s="1" t="s">
-        <v>705</v>
-      </c>
-      <c r="HQ21" s="1" t="s">
-        <v>707</v>
-      </c>
-      <c r="HR21" s="1" t="s">
-        <v>710</v>
-      </c>
-      <c r="HS21" s="1" t="s">
-        <v>717</v>
-      </c>
-      <c r="HT21" s="1" t="s">
-        <v>720</v>
-      </c>
-      <c r="HU21" s="1" t="s">
-        <v>723</v>
-      </c>
-      <c r="HV21" s="1" t="s">
-        <v>727</v>
-      </c>
-      <c r="HW21" s="1" t="s">
-        <v>729</v>
-      </c>
-      <c r="HX21" s="1" t="s">
-        <v>732</v>
-      </c>
-      <c r="HY21" s="1" t="s">
-        <v>737</v>
-      </c>
-      <c r="HZ21" s="1" t="s">
-        <v>741</v>
-      </c>
-      <c r="IA21" s="1" t="s">
-        <v>744</v>
-      </c>
-      <c r="IB21" s="1" t="s">
-        <v>750</v>
-      </c>
-      <c r="IC21" s="1" t="s">
-        <v>753</v>
-      </c>
-      <c r="ID21" s="1" t="s">
-        <v>760</v>
-      </c>
-      <c r="IE21" s="1" t="s">
-        <v>763</v>
-      </c>
-      <c r="IF21" s="1" t="s">
-        <v>766</v>
-      </c>
-      <c r="IG21" s="1" t="s">
-        <v>768</v>
-      </c>
-      <c r="IH21" s="1" t="s">
-        <v>772</v>
-      </c>
-      <c r="II21" s="1" t="s">
-        <v>775</v>
-      </c>
-      <c r="IJ21" s="1" t="s">
-        <v>777</v>
-      </c>
-      <c r="IK21" s="1" t="s">
-        <v>781</v>
-      </c>
-      <c r="IL21" s="1" t="s">
-        <v>783</v>
-      </c>
-      <c r="IM21" s="1" t="s">
-        <v>788</v>
-      </c>
-      <c r="IN21" s="1" t="s">
-        <v>790</v>
-      </c>
-      <c r="IO21" s="1" t="s">
-        <v>793</v>
-      </c>
-      <c r="IP21" s="1" t="s">
-        <v>796</v>
-      </c>
-      <c r="IQ21" s="1" t="s">
-        <v>799</v>
-      </c>
-      <c r="IR21" s="1" t="s">
-        <v>804</v>
-      </c>
-      <c r="IS21" s="1" t="s">
-        <v>808</v>
-      </c>
-      <c r="IT21" s="1" t="s">
-        <v>811</v>
-      </c>
-      <c r="IU21" s="1" t="s">
-        <v>815</v>
-      </c>
-      <c r="IV21" s="1" t="s">
-        <v>817</v>
-      </c>
-      <c r="IW21" s="1" t="s">
-        <v>820</v>
-      </c>
-      <c r="IX21" s="1" t="s">
-        <v>822</v>
-      </c>
-      <c r="IY21" s="1" t="s">
-        <v>824</v>
-      </c>
-      <c r="IZ21" s="1" t="s">
-        <v>829</v>
-      </c>
-      <c r="JA21" s="1" t="s">
-        <v>834</v>
-      </c>
-      <c r="JB21" s="1" t="s">
-        <v>838</v>
-      </c>
-      <c r="JC21" s="1" t="s">
-        <v>843</v>
-      </c>
-      <c r="JD21" s="1" t="s">
-        <v>846</v>
-      </c>
-      <c r="JE21" s="1" t="s">
-        <v>848</v>
-      </c>
-      <c r="JF21" s="1" t="s">
-        <v>850</v>
-      </c>
-      <c r="JG21" s="1" t="s">
-        <v>855</v>
-      </c>
-      <c r="JH21" s="1" t="s">
-        <v>858</v>
-      </c>
-      <c r="JI21" s="1" t="s">
-        <v>863</v>
-      </c>
-      <c r="JJ21" s="1" t="s">
-        <v>866</v>
-      </c>
-      <c r="JK21" s="1" t="s">
-        <v>868</v>
-      </c>
-      <c r="JL21" s="1" t="s">
-        <v>871</v>
-      </c>
-      <c r="JM21" s="1" t="s">
-        <v>873</v>
-      </c>
-      <c r="JN21" s="1" t="s">
-        <v>876</v>
-      </c>
-      <c r="JO21" s="1" t="s">
-        <v>879</v>
-      </c>
-      <c r="JP21" s="1" t="s">
-        <v>883</v>
-      </c>
-      <c r="JQ21" s="1" t="s">
-        <v>885</v>
-      </c>
-      <c r="JR21" s="1" t="s">
-        <v>889</v>
-      </c>
-      <c r="JS21" s="1" t="s">
-        <v>892</v>
-      </c>
-      <c r="JT21" s="1" t="s">
-        <v>895</v>
-      </c>
-      <c r="JU21" s="1" t="s">
-        <v>898</v>
-      </c>
-      <c r="JV21" s="1" t="s">
-        <v>903</v>
-      </c>
-      <c r="JW21" s="1" t="s">
-        <v>906</v>
-      </c>
-      <c r="JX21" s="1" t="s">
-        <v>909</v>
-      </c>
-      <c r="JY21" s="1" t="s">
-        <v>911</v>
-      </c>
-      <c r="JZ21" s="1" t="s">
-        <v>914</v>
-      </c>
-      <c r="KA21" s="1" t="s">
-        <v>918</v>
-      </c>
-      <c r="KB21" s="1" t="s">
-        <v>922</v>
-      </c>
-      <c r="KC21" s="1" t="s">
-        <v>926</v>
-      </c>
-      <c r="KD21" s="1" t="s">
-        <v>928</v>
-      </c>
-      <c r="KE21" s="1" t="s">
-        <v>931</v>
-      </c>
-      <c r="KF21" s="1" t="s">
-        <v>966</v>
-      </c>
-      <c r="KG21" s="1" t="s">
-        <v>964</v>
-      </c>
-      <c r="KH21" s="1" t="s">
-        <v>967</v>
-      </c>
-      <c r="KI21" s="1" t="s">
-        <v>978</v>
-      </c>
-      <c r="KJ21" s="1" t="s">
-        <v>968</v>
-      </c>
-      <c r="KK21" s="1" t="s">
-        <v>971</v>
-      </c>
-      <c r="KL21" s="1" t="s">
-        <v>972</v>
-      </c>
-      <c r="KM21" s="1" t="s">
-        <v>975</v>
-      </c>
-      <c r="KN21" s="1" t="s">
-        <v>1012</v>
-      </c>
-      <c r="KO21" s="1" t="s">
-        <v>981</v>
-      </c>
-      <c r="KP21" s="1" t="s">
-        <v>982</v>
-      </c>
-      <c r="KQ21" s="1" t="s">
-        <v>987</v>
-      </c>
-      <c r="KR21" s="1" t="s">
-        <v>983</v>
-      </c>
-      <c r="KS21" s="1" t="s">
-        <v>986</v>
-      </c>
-      <c r="KT21" s="1" t="s">
-        <v>993</v>
-      </c>
-      <c r="KU21" s="1" t="s">
-        <v>994</v>
-      </c>
-      <c r="KV21" s="1" t="s">
-        <v>995</v>
-      </c>
-      <c r="KW21" s="1" t="s">
-        <v>997</v>
-      </c>
-      <c r="KX21" s="1" t="s">
-        <v>998</v>
-      </c>
-      <c r="KY21" s="1" t="s">
-        <v>999</v>
-      </c>
-      <c r="KZ21" s="1" t="s">
-        <v>1005</v>
-      </c>
-      <c r="LA21" s="1" t="s">
-        <v>1004</v>
-      </c>
-      <c r="LB21" s="1" t="s">
-        <v>1006</v>
-      </c>
-      <c r="LC21" s="1" t="s">
-        <v>1008</v>
-      </c>
-      <c r="LD21" s="1" t="s">
-        <v>1059</v>
-      </c>
-      <c r="LE21" s="1" t="s">
-        <v>1010</v>
-      </c>
-      <c r="LF21" s="1" t="s">
-        <v>1080</v>
-      </c>
-      <c r="LG21" s="1" t="s">
-        <v>1013</v>
-      </c>
-      <c r="LH21" s="1" t="s">
-        <v>1015</v>
-      </c>
-      <c r="LI21" s="1" t="s">
-        <v>1016</v>
-      </c>
-      <c r="LJ21" s="1" t="s">
-        <v>1017</v>
-      </c>
-      <c r="LK21" s="1" t="s">
-        <v>1021</v>
-      </c>
-      <c r="LL21" s="1" t="s">
-        <v>1018</v>
-      </c>
-      <c r="LM21" s="1" t="s">
-        <v>1079</v>
-      </c>
-      <c r="LN21" s="1" t="s">
-        <v>1087</v>
-      </c>
-      <c r="LO21" s="1" t="s">
-        <v>1089</v>
-      </c>
-      <c r="LP21" s="1" t="s">
-        <v>1090</v>
-      </c>
-      <c r="LQ21" s="1" t="s">
-        <v>1092</v>
-      </c>
-      <c r="LR21" s="1" t="s">
-        <v>1094</v>
-      </c>
-      <c r="LS21" s="1" t="s">
-        <v>1114</v>
-      </c>
-      <c r="LT21" s="1" t="s">
-        <v>1097</v>
-      </c>
-      <c r="LU21" s="1" t="s">
-        <v>1101</v>
-      </c>
-      <c r="LV21" s="1" t="s">
-        <v>1111</v>
-      </c>
-      <c r="LW21" s="1" t="s">
-        <v>1106</v>
-      </c>
-      <c r="LX21" s="1" t="s">
-        <v>1107</v>
-      </c>
-      <c r="LY21" s="1" t="s">
-        <v>1109</v>
-      </c>
-      <c r="LZ21" s="1" t="s">
-        <v>1113</v>
-      </c>
-      <c r="MA21" s="1" t="s">
-        <v>1117</v>
-      </c>
-      <c r="MB21" s="1" t="s">
-        <v>1122</v>
-      </c>
-      <c r="MC21" s="1" t="s">
-        <v>1125</v>
-      </c>
-      <c r="MD21" s="1" t="s">
-        <v>1128</v>
-      </c>
-      <c r="ME21" s="1" t="s">
-        <v>1134</v>
+        <v>1143</v>
       </c>
     </row>
     <row r="22" spans="1:343" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B22" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="C22" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="D22" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="E22" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="F22" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="G22" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="H22" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="I22" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="J22" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="K22" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="L22" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="M22" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="N22" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="O22" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="P22" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="Q22" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="R22" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="S22" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="T22" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="U22" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="V22" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="W22" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="X22" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="Y22" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="Z22" s="1" t="s">
+        <v>131</v>
+      </c>
+      <c r="AA22" s="1" t="s">
+        <v>134</v>
+      </c>
+      <c r="AB22" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="AC22" s="1" t="s">
+        <v>139</v>
+      </c>
+      <c r="AD22" s="1" t="s">
+        <v>142</v>
+      </c>
+      <c r="AE22" s="1" t="s">
+        <v>145</v>
+      </c>
+      <c r="AF22" s="1" t="s">
+        <v>147</v>
+      </c>
+      <c r="AG22" s="1" t="s">
+        <v>154</v>
+      </c>
+      <c r="AH22" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="AI22" s="1" t="s">
+        <v>163</v>
+      </c>
+      <c r="AJ22" s="1" t="s">
+        <v>165</v>
+      </c>
+      <c r="AK22" s="1" t="s">
+        <v>168</v>
+      </c>
+      <c r="AL22" s="1" t="s">
+        <v>171</v>
+      </c>
+      <c r="AM22" s="1" t="s">
+        <v>176</v>
+      </c>
+      <c r="AN22" s="1" t="s">
+        <v>183</v>
+      </c>
+      <c r="AO22" s="1" t="s">
+        <v>186</v>
+      </c>
+      <c r="AP22" s="1" t="s">
+        <v>189</v>
+      </c>
+      <c r="AQ22" s="1" t="s">
+        <v>193</v>
+      </c>
+      <c r="AR22" s="1" t="s">
+        <v>200</v>
+      </c>
+      <c r="AS22" s="1" t="s">
+        <v>202</v>
+      </c>
+      <c r="AT22" s="1" t="s">
+        <v>205</v>
+      </c>
+      <c r="AU22" s="1" t="s">
+        <v>207</v>
+      </c>
+      <c r="AV22" s="1" t="s">
+        <v>215</v>
+      </c>
+      <c r="AW22" s="1" t="s">
+        <v>218</v>
+      </c>
+      <c r="AX22" s="1" t="s">
+        <v>226</v>
+      </c>
+      <c r="AY22" s="1" t="s">
+        <v>228</v>
+      </c>
+      <c r="AZ22" s="1" t="s">
+        <v>235</v>
+      </c>
+      <c r="BA22" s="1" t="s">
+        <v>241</v>
+      </c>
+      <c r="BB22" s="1" t="s">
+        <v>247</v>
+      </c>
+      <c r="BC22" s="1" t="s">
+        <v>252</v>
+      </c>
+      <c r="BD22" s="1" t="s">
+        <v>257</v>
+      </c>
+      <c r="BE22" s="1" t="s">
+        <v>257</v>
+      </c>
+      <c r="BF22" s="1" t="s">
+        <v>257</v>
+      </c>
+      <c r="BG22" s="1" t="s">
+        <v>257</v>
+      </c>
+      <c r="BH22" s="1" t="s">
+        <v>257</v>
+      </c>
+      <c r="BI22" s="1" t="s">
+        <v>279</v>
+      </c>
+      <c r="BJ22" s="1" t="s">
+        <v>285</v>
+      </c>
+      <c r="BK22" s="1" t="s">
+        <v>288</v>
+      </c>
+      <c r="BL22" s="1" t="s">
+        <v>291</v>
+      </c>
+      <c r="BM22" s="1" t="s">
+        <v>294</v>
+      </c>
+      <c r="BN22" s="1" t="s">
+        <v>297</v>
+      </c>
+      <c r="BO22" s="1" t="s">
+        <v>300</v>
+      </c>
+      <c r="BP22" s="1" t="s">
+        <v>302</v>
+      </c>
+      <c r="BQ22" s="1" t="s">
+        <v>304</v>
+      </c>
+      <c r="BR22" s="1" t="s">
+        <v>309</v>
+      </c>
+      <c r="BS22" s="1" t="s">
+        <v>313</v>
+      </c>
+      <c r="BT22" s="1" t="s">
+        <v>316</v>
+      </c>
+      <c r="BU22" s="1" t="s">
+        <v>319</v>
+      </c>
+      <c r="BV22" s="1" t="s">
+        <v>323</v>
+      </c>
+      <c r="BW22" s="1" t="s">
+        <v>329</v>
+      </c>
+      <c r="BX22" s="1" t="s">
+        <v>331</v>
+      </c>
+      <c r="BY22" s="1" t="s">
+        <v>335</v>
+      </c>
+      <c r="BZ22" s="1" t="s">
+        <v>338</v>
+      </c>
+      <c r="CA22" s="1" t="s">
+        <v>343</v>
+      </c>
+      <c r="CB22" s="1" t="s">
+        <v>347</v>
+      </c>
+      <c r="CC22" s="1" t="s">
+        <v>347</v>
+      </c>
+      <c r="CD22" s="1" t="s">
+        <v>355</v>
+      </c>
+      <c r="CE22" s="1" t="s">
+        <v>355</v>
+      </c>
+      <c r="CF22" s="1" t="s">
+        <v>359</v>
+      </c>
+      <c r="CG22" s="1" t="s">
+        <v>362</v>
+      </c>
+      <c r="CH22" s="1" t="s">
+        <v>365</v>
+      </c>
+      <c r="CI22" s="1" t="s">
+        <v>365</v>
+      </c>
+      <c r="CJ22" s="1" t="s">
+        <v>368</v>
+      </c>
+      <c r="CK22" s="1" t="s">
+        <v>368</v>
+      </c>
+      <c r="CL22" s="1" t="s">
+        <v>371</v>
+      </c>
+      <c r="CM22" s="1" t="s">
+        <v>371</v>
+      </c>
+      <c r="CN22" s="1" t="s">
+        <v>374</v>
+      </c>
+      <c r="CO22" s="1" t="s">
+        <v>374</v>
+      </c>
+      <c r="CP22" s="1" t="s">
+        <v>377</v>
+      </c>
+      <c r="CQ22" s="1" t="s">
+        <v>379</v>
+      </c>
+      <c r="CR22" s="1" t="s">
+        <v>381</v>
+      </c>
+      <c r="CS22" s="1" t="s">
+        <v>381</v>
+      </c>
+      <c r="CT22" s="1" t="s">
+        <v>384</v>
+      </c>
+      <c r="CU22" s="1" t="s">
+        <v>384</v>
+      </c>
+      <c r="CV22" s="1" t="s">
+        <v>387</v>
+      </c>
+      <c r="CW22" s="1" t="s">
+        <v>387</v>
+      </c>
+      <c r="CX22" s="1" t="s">
+        <v>390</v>
+      </c>
+      <c r="CY22" s="1" t="s">
+        <v>390</v>
+      </c>
+      <c r="CZ22" s="1" t="s">
+        <v>393</v>
+      </c>
+      <c r="DA22" s="1" t="s">
+        <v>395</v>
+      </c>
+      <c r="DB22" s="1" t="s">
+        <v>397</v>
+      </c>
+      <c r="DC22" s="1" t="s">
+        <v>397</v>
+      </c>
+      <c r="DD22" s="1" t="s">
+        <v>400</v>
+      </c>
+      <c r="DE22" s="1" t="s">
+        <v>400</v>
+      </c>
+      <c r="DF22" s="1" t="s">
+        <v>403</v>
+      </c>
+      <c r="DG22" s="1" t="s">
+        <v>408</v>
+      </c>
+      <c r="DH22" s="1" t="s">
+        <v>411</v>
+      </c>
+      <c r="DI22" s="1" t="s">
+        <v>413</v>
+      </c>
+      <c r="DJ22" s="1" t="s">
+        <v>415</v>
+      </c>
+      <c r="DK22" s="1" t="s">
+        <v>417</v>
+      </c>
+      <c r="DL22" s="1" t="s">
+        <v>419</v>
+      </c>
+      <c r="DM22" s="1" t="s">
+        <v>421</v>
+      </c>
+      <c r="DN22" s="1" t="s">
+        <v>423</v>
+      </c>
+      <c r="DO22" s="1" t="s">
+        <v>427</v>
+      </c>
+      <c r="DP22" s="1" t="s">
+        <v>431</v>
+      </c>
+      <c r="DQ22" s="1" t="s">
+        <v>435</v>
+      </c>
+      <c r="DR22" s="1" t="s">
+        <v>439</v>
+      </c>
+      <c r="DS22" s="1" t="s">
+        <v>441</v>
+      </c>
+      <c r="DT22" s="1" t="s">
+        <v>445</v>
+      </c>
+      <c r="DU22" s="1" t="s">
+        <v>448</v>
+      </c>
+      <c r="DV22" s="1" t="s">
+        <v>450</v>
+      </c>
+      <c r="DW22" s="1" t="s">
+        <v>453</v>
+      </c>
+      <c r="DX22" s="1" t="s">
+        <v>455</v>
+      </c>
+      <c r="DY22" s="1" t="s">
+        <v>459</v>
+      </c>
+      <c r="DZ22" s="1" t="s">
+        <v>461</v>
+      </c>
+      <c r="EA22" s="1" t="s">
+        <v>464</v>
+      </c>
+      <c r="EB22" s="1" t="s">
+        <v>466</v>
+      </c>
+      <c r="EC22" s="1" t="s">
+        <v>469</v>
+      </c>
+      <c r="ED22" s="1" t="s">
+        <v>472</v>
+      </c>
+      <c r="EE22" s="1" t="s">
+        <v>475</v>
+      </c>
+      <c r="EF22" s="1" t="s">
+        <v>479</v>
+      </c>
+      <c r="EG22" s="1" t="s">
+        <v>481</v>
+      </c>
+      <c r="EH22" s="1" t="s">
+        <v>484</v>
+      </c>
+      <c r="EI22" s="1" t="s">
+        <v>486</v>
+      </c>
+      <c r="EJ22" s="1" t="s">
+        <v>489</v>
+      </c>
+      <c r="EK22" s="1" t="s">
+        <v>492</v>
+      </c>
+      <c r="EL22" s="1" t="s">
+        <v>494</v>
+      </c>
+      <c r="EM22" s="1" t="s">
+        <v>498</v>
+      </c>
+      <c r="EN22" s="1" t="s">
+        <v>501</v>
+      </c>
+      <c r="EO22" s="1" t="s">
+        <v>504</v>
+      </c>
+      <c r="EP22" s="1" t="s">
+        <v>508</v>
+      </c>
+      <c r="EQ22" s="1" t="s">
+        <v>510</v>
+      </c>
+      <c r="ER22" s="1" t="s">
+        <v>512</v>
+      </c>
+      <c r="ES22" s="1" t="s">
+        <v>514</v>
+      </c>
+      <c r="ET22" s="1" t="s">
+        <v>516</v>
+      </c>
+      <c r="EU22" s="1" t="s">
+        <v>519</v>
+      </c>
+      <c r="EV22" s="1" t="s">
+        <v>522</v>
+      </c>
+      <c r="EW22" s="1" t="s">
+        <v>525</v>
+      </c>
+      <c r="EX22" s="1" t="s">
+        <v>527</v>
+      </c>
+      <c r="EY22" s="1" t="s">
+        <v>530</v>
+      </c>
+      <c r="EZ22" s="1" t="s">
+        <v>532</v>
+      </c>
+      <c r="FA22" s="1" t="s">
+        <v>536</v>
+      </c>
+      <c r="FB22" s="1" t="s">
+        <v>539</v>
+      </c>
+      <c r="FC22" s="1" t="s">
+        <v>543</v>
+      </c>
+      <c r="FD22" s="1" t="s">
+        <v>545</v>
+      </c>
+      <c r="FE22" s="1" t="s">
+        <v>547</v>
+      </c>
+      <c r="FF22" s="1" t="s">
+        <v>549</v>
+      </c>
+      <c r="FG22" s="1" t="s">
+        <v>551</v>
+      </c>
+      <c r="FH22" s="1" t="s">
+        <v>554</v>
+      </c>
+      <c r="FI22" s="1" t="s">
+        <v>558</v>
+      </c>
+      <c r="FJ22" s="1" t="s">
+        <v>561</v>
+      </c>
+      <c r="FK22" s="1" t="s">
+        <v>564</v>
+      </c>
+      <c r="FL22" s="1" t="s">
+        <v>566</v>
+      </c>
+      <c r="FM22" s="1" t="s">
+        <v>569</v>
+      </c>
+      <c r="FN22" s="1" t="s">
+        <v>571</v>
+      </c>
+      <c r="FO22" s="1" t="s">
+        <v>573</v>
+      </c>
+      <c r="FP22" s="1" t="s">
+        <v>575</v>
+      </c>
+      <c r="FQ22" s="1" t="s">
+        <v>577</v>
+      </c>
+      <c r="FR22" s="1" t="s">
+        <v>581</v>
+      </c>
+      <c r="FS22" s="1" t="s">
+        <v>586</v>
+      </c>
+      <c r="FT22" s="1" t="s">
+        <v>588</v>
+      </c>
+      <c r="FU22" s="1" t="s">
+        <v>590</v>
+      </c>
+      <c r="FV22" s="1" t="s">
+        <v>593</v>
+      </c>
+      <c r="FW22" s="1" t="s">
+        <v>596</v>
+      </c>
+      <c r="FX22" s="1" t="s">
+        <v>599</v>
+      </c>
+      <c r="FY22" s="1" t="s">
+        <v>602</v>
+      </c>
+      <c r="FZ22" s="1" t="s">
+        <v>605</v>
+      </c>
+      <c r="GA22" s="1" t="s">
+        <v>608</v>
+      </c>
+      <c r="GB22" s="1" t="s">
+        <v>611</v>
+      </c>
+      <c r="GC22" s="1" t="s">
+        <v>614</v>
+      </c>
+      <c r="GD22" s="1" t="s">
+        <v>617</v>
+      </c>
+      <c r="GE22" s="1" t="s">
+        <v>619</v>
+      </c>
+      <c r="GF22" s="1" t="s">
+        <v>621</v>
+      </c>
+      <c r="GG22" s="1" t="s">
+        <v>625</v>
+      </c>
+      <c r="GH22" s="1" t="s">
+        <v>628</v>
+      </c>
+      <c r="GI22" s="1" t="s">
+        <v>630</v>
+      </c>
+      <c r="GJ22" s="1" t="s">
+        <v>633</v>
+      </c>
+      <c r="GK22" s="1" t="s">
+        <v>635</v>
+      </c>
+      <c r="GL22" s="1" t="s">
+        <v>638</v>
+      </c>
+      <c r="GM22" s="1" t="s">
+        <v>640</v>
+      </c>
+      <c r="GN22" s="1" t="s">
+        <v>642</v>
+      </c>
+      <c r="GO22" s="1" t="s">
+        <v>644</v>
+      </c>
+      <c r="GP22" s="1" t="s">
+        <v>647</v>
+      </c>
+      <c r="GQ22" s="1" t="s">
+        <v>650</v>
+      </c>
+      <c r="GR22" s="1" t="s">
+        <v>652</v>
+      </c>
+      <c r="GS22" s="1" t="s">
+        <v>577</v>
+      </c>
+      <c r="GT22" s="1" t="s">
+        <v>655</v>
+      </c>
+      <c r="GU22" s="1" t="s">
+        <v>657</v>
+      </c>
+      <c r="GV22" s="1" t="s">
+        <v>659</v>
+      </c>
+      <c r="GW22" s="1" t="s">
+        <v>661</v>
+      </c>
+      <c r="GX22" s="1" t="s">
+        <v>664</v>
+      </c>
+      <c r="GY22" s="1" t="s">
+        <v>667</v>
+      </c>
+      <c r="GZ22" s="1" t="s">
+        <v>669</v>
+      </c>
+      <c r="HA22" s="1" t="s">
+        <v>174</v>
+      </c>
+      <c r="HB22" s="1" t="s">
+        <v>671</v>
+      </c>
+      <c r="HC22" s="1" t="s">
+        <v>673</v>
+      </c>
+      <c r="HD22" s="1" t="s">
+        <v>675</v>
+      </c>
+      <c r="HE22" s="1" t="s">
+        <v>677</v>
+      </c>
+      <c r="HF22" s="1" t="s">
+        <v>679</v>
+      </c>
+      <c r="HG22" s="1" t="s">
+        <v>682</v>
+      </c>
+      <c r="HH22" s="1" t="s">
+        <v>684</v>
+      </c>
+      <c r="HI22" s="1" t="s">
+        <v>687</v>
+      </c>
+      <c r="HJ22" s="1" t="s">
+        <v>690</v>
+      </c>
+      <c r="HK22" s="1" t="s">
+        <v>692</v>
+      </c>
+      <c r="HL22" s="1" t="s">
+        <v>696</v>
+      </c>
+      <c r="HM22" s="1" t="s">
+        <v>1130</v>
+      </c>
+      <c r="HN22" s="1" t="s">
+        <v>699</v>
+      </c>
+      <c r="HO22" s="1" t="s">
+        <v>701</v>
+      </c>
+      <c r="HP22" s="1" t="s">
+        <v>705</v>
+      </c>
+      <c r="HQ22" s="1" t="s">
+        <v>707</v>
+      </c>
+      <c r="HR22" s="1" t="s">
+        <v>710</v>
+      </c>
+      <c r="HS22" s="1" t="s">
+        <v>717</v>
+      </c>
+      <c r="HT22" s="1" t="s">
+        <v>720</v>
+      </c>
+      <c r="HU22" s="1" t="s">
+        <v>723</v>
+      </c>
+      <c r="HV22" s="1" t="s">
+        <v>727</v>
+      </c>
+      <c r="HW22" s="1" t="s">
+        <v>729</v>
+      </c>
+      <c r="HX22" s="1" t="s">
+        <v>732</v>
+      </c>
+      <c r="HY22" s="1" t="s">
+        <v>737</v>
+      </c>
+      <c r="HZ22" s="1" t="s">
+        <v>741</v>
+      </c>
+      <c r="IA22" s="1" t="s">
+        <v>744</v>
+      </c>
+      <c r="IB22" s="1" t="s">
+        <v>750</v>
+      </c>
+      <c r="IC22" s="1" t="s">
+        <v>753</v>
+      </c>
+      <c r="ID22" s="1" t="s">
+        <v>760</v>
+      </c>
+      <c r="IE22" s="1" t="s">
+        <v>763</v>
+      </c>
+      <c r="IF22" s="1" t="s">
+        <v>766</v>
+      </c>
+      <c r="IG22" s="1" t="s">
+        <v>768</v>
+      </c>
+      <c r="IH22" s="1" t="s">
+        <v>772</v>
+      </c>
+      <c r="II22" s="1" t="s">
+        <v>775</v>
+      </c>
+      <c r="IJ22" s="1" t="s">
+        <v>777</v>
+      </c>
+      <c r="IK22" s="1" t="s">
+        <v>781</v>
+      </c>
+      <c r="IL22" s="1" t="s">
+        <v>783</v>
+      </c>
+      <c r="IM22" s="1" t="s">
+        <v>788</v>
+      </c>
+      <c r="IN22" s="1" t="s">
+        <v>790</v>
+      </c>
+      <c r="IO22" s="1" t="s">
+        <v>793</v>
+      </c>
+      <c r="IP22" s="1" t="s">
+        <v>796</v>
+      </c>
+      <c r="IQ22" s="1" t="s">
+        <v>799</v>
+      </c>
+      <c r="IR22" s="1" t="s">
+        <v>804</v>
+      </c>
+      <c r="IS22" s="1" t="s">
+        <v>808</v>
+      </c>
+      <c r="IT22" s="1" t="s">
+        <v>811</v>
+      </c>
+      <c r="IU22" s="1" t="s">
+        <v>815</v>
+      </c>
+      <c r="IV22" s="1" t="s">
+        <v>817</v>
+      </c>
+      <c r="IW22" s="1" t="s">
+        <v>820</v>
+      </c>
+      <c r="IX22" s="1" t="s">
+        <v>822</v>
+      </c>
+      <c r="IY22" s="1" t="s">
+        <v>824</v>
+      </c>
+      <c r="IZ22" s="1" t="s">
+        <v>829</v>
+      </c>
+      <c r="JA22" s="1" t="s">
+        <v>834</v>
+      </c>
+      <c r="JB22" s="1" t="s">
+        <v>838</v>
+      </c>
+      <c r="JC22" s="1" t="s">
+        <v>843</v>
+      </c>
+      <c r="JD22" s="1" t="s">
+        <v>846</v>
+      </c>
+      <c r="JE22" s="1" t="s">
+        <v>848</v>
+      </c>
+      <c r="JF22" s="1" t="s">
+        <v>850</v>
+      </c>
+      <c r="JG22" s="1" t="s">
+        <v>855</v>
+      </c>
+      <c r="JH22" s="1" t="s">
+        <v>858</v>
+      </c>
+      <c r="JI22" s="1" t="s">
+        <v>863</v>
+      </c>
+      <c r="JJ22" s="1" t="s">
+        <v>866</v>
+      </c>
+      <c r="JK22" s="1" t="s">
+        <v>868</v>
+      </c>
+      <c r="JL22" s="1" t="s">
+        <v>871</v>
+      </c>
+      <c r="JM22" s="1" t="s">
+        <v>873</v>
+      </c>
+      <c r="JN22" s="1" t="s">
+        <v>876</v>
+      </c>
+      <c r="JO22" s="1" t="s">
+        <v>879</v>
+      </c>
+      <c r="JP22" s="1" t="s">
+        <v>883</v>
+      </c>
+      <c r="JQ22" s="1" t="s">
+        <v>885</v>
+      </c>
+      <c r="JR22" s="1" t="s">
+        <v>889</v>
+      </c>
+      <c r="JS22" s="1" t="s">
+        <v>892</v>
+      </c>
+      <c r="JT22" s="1" t="s">
+        <v>895</v>
+      </c>
+      <c r="JU22" s="1" t="s">
+        <v>898</v>
+      </c>
+      <c r="JV22" s="1" t="s">
+        <v>903</v>
+      </c>
+      <c r="JW22" s="1" t="s">
+        <v>906</v>
+      </c>
+      <c r="JX22" s="1" t="s">
+        <v>909</v>
+      </c>
+      <c r="JY22" s="1" t="s">
+        <v>911</v>
+      </c>
+      <c r="JZ22" s="1" t="s">
+        <v>914</v>
+      </c>
+      <c r="KA22" s="1" t="s">
+        <v>918</v>
+      </c>
+      <c r="KB22" s="1" t="s">
+        <v>922</v>
+      </c>
+      <c r="KC22" s="1" t="s">
+        <v>926</v>
+      </c>
+      <c r="KD22" s="1" t="s">
+        <v>928</v>
+      </c>
+      <c r="KE22" s="1" t="s">
+        <v>931</v>
+      </c>
+      <c r="KF22" s="1" t="s">
+        <v>966</v>
+      </c>
+      <c r="KG22" s="1" t="s">
+        <v>964</v>
+      </c>
+      <c r="KH22" s="1" t="s">
+        <v>967</v>
+      </c>
+      <c r="KI22" s="1" t="s">
+        <v>978</v>
+      </c>
+      <c r="KJ22" s="1" t="s">
+        <v>968</v>
+      </c>
+      <c r="KK22" s="1" t="s">
+        <v>971</v>
+      </c>
+      <c r="KL22" s="1" t="s">
+        <v>972</v>
+      </c>
+      <c r="KM22" s="1" t="s">
+        <v>975</v>
+      </c>
+      <c r="KN22" s="1" t="s">
+        <v>1012</v>
+      </c>
+      <c r="KO22" s="1" t="s">
+        <v>981</v>
+      </c>
+      <c r="KP22" s="1" t="s">
+        <v>982</v>
+      </c>
+      <c r="KQ22" s="1" t="s">
+        <v>987</v>
+      </c>
+      <c r="KR22" s="1" t="s">
+        <v>983</v>
+      </c>
+      <c r="KS22" s="1" t="s">
+        <v>986</v>
+      </c>
+      <c r="KT22" s="1" t="s">
+        <v>993</v>
+      </c>
+      <c r="KU22" s="1" t="s">
+        <v>994</v>
+      </c>
+      <c r="KV22" s="1" t="s">
+        <v>995</v>
+      </c>
+      <c r="KW22" s="1" t="s">
+        <v>997</v>
+      </c>
+      <c r="KX22" s="1" t="s">
+        <v>998</v>
+      </c>
+      <c r="KY22" s="1" t="s">
+        <v>999</v>
+      </c>
+      <c r="KZ22" s="1" t="s">
+        <v>1005</v>
+      </c>
+      <c r="LA22" s="1" t="s">
+        <v>1004</v>
+      </c>
+      <c r="LB22" s="1" t="s">
+        <v>1006</v>
+      </c>
+      <c r="LC22" s="1" t="s">
+        <v>1008</v>
+      </c>
+      <c r="LD22" s="1" t="s">
+        <v>1059</v>
+      </c>
+      <c r="LE22" s="1" t="s">
+        <v>1010</v>
+      </c>
+      <c r="LF22" s="1" t="s">
+        <v>1080</v>
+      </c>
+      <c r="LG22" s="1" t="s">
+        <v>1013</v>
+      </c>
+      <c r="LH22" s="1" t="s">
+        <v>1015</v>
+      </c>
+      <c r="LI22" s="1" t="s">
+        <v>1016</v>
+      </c>
+      <c r="LJ22" s="1" t="s">
+        <v>1017</v>
+      </c>
+      <c r="LK22" s="1" t="s">
+        <v>1021</v>
+      </c>
+      <c r="LL22" s="1" t="s">
+        <v>1018</v>
+      </c>
+      <c r="LM22" s="1" t="s">
+        <v>1079</v>
+      </c>
+      <c r="LN22" s="1" t="s">
+        <v>1087</v>
+      </c>
+      <c r="LO22" s="1" t="s">
+        <v>1089</v>
+      </c>
+      <c r="LP22" s="1" t="s">
+        <v>1090</v>
+      </c>
+      <c r="LQ22" s="1" t="s">
+        <v>1092</v>
+      </c>
+      <c r="LR22" s="1" t="s">
+        <v>1094</v>
+      </c>
+      <c r="LS22" s="1" t="s">
+        <v>1114</v>
+      </c>
+      <c r="LT22" s="1" t="s">
+        <v>1097</v>
+      </c>
+      <c r="LU22" s="1" t="s">
+        <v>1101</v>
+      </c>
+      <c r="LV22" s="1" t="s">
+        <v>1111</v>
+      </c>
+      <c r="LW22" s="1" t="s">
+        <v>1106</v>
+      </c>
+      <c r="LX22" s="1" t="s">
+        <v>1107</v>
+      </c>
+      <c r="LY22" s="1" t="s">
+        <v>1109</v>
+      </c>
+      <c r="LZ22" s="1" t="s">
+        <v>1113</v>
+      </c>
+      <c r="MA22" s="1" t="s">
+        <v>1117</v>
+      </c>
+      <c r="MB22" s="1" t="s">
+        <v>1122</v>
+      </c>
+      <c r="MC22" s="1" t="s">
+        <v>1125</v>
+      </c>
+      <c r="MD22" s="1" t="s">
+        <v>1128</v>
+      </c>
+      <c r="ME22" s="1" t="s">
+        <v>1134</v>
+      </c>
+    </row>
+    <row r="23" spans="1:343" x14ac:dyDescent="0.25">
+      <c r="A23" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="EU22" s="1" t="s">
+      <c r="EU23" s="1" t="s">
         <v>520</v>
       </c>
-      <c r="FQ22" s="1" t="s">
+      <c r="FQ23" s="1" t="s">
         <v>579</v>
       </c>
-      <c r="HQ22" s="1" t="s">
+      <c r="HQ23" s="1" t="s">
         <v>708</v>
       </c>
-      <c r="IL22" s="1" t="s">
+      <c r="IL23" s="1" t="s">
         <v>786</v>
-      </c>
-    </row>
-    <row r="23" spans="1:343" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="P23" s="3" t="s">
-        <v>100</v>
-      </c>
-      <c r="W23" s="3" t="s">
-        <v>121</v>
-      </c>
-      <c r="AU23" s="3" t="s">
-        <v>210</v>
-      </c>
-      <c r="AW23" s="3" t="s">
-        <v>220</v>
-      </c>
-      <c r="AY23" s="3" t="s">
-        <v>230</v>
-      </c>
-      <c r="BA23" s="3" t="s">
-        <v>242</v>
-      </c>
-      <c r="BD23" s="3" t="s">
-        <v>258</v>
-      </c>
-      <c r="BE23" s="3" t="s">
-        <v>264</v>
-      </c>
-      <c r="BF23" s="3" t="s">
-        <v>268</v>
-      </c>
-      <c r="BG23" s="3" t="s">
-        <v>272</v>
-      </c>
-      <c r="BH23" s="3" t="s">
-        <v>276</v>
-      </c>
-      <c r="BI23" s="3" t="s">
-        <v>281</v>
-      </c>
-      <c r="FR23" s="3" t="s">
-        <v>233</v>
-      </c>
-      <c r="HX23" s="3" t="s">
-        <v>733</v>
-      </c>
-      <c r="IA23" s="3" t="s">
-        <v>746</v>
-      </c>
-      <c r="IC23" s="3" t="s">
-        <v>755</v>
-      </c>
-      <c r="JB23" s="3" t="s">
-        <v>839</v>
-      </c>
-      <c r="JF23" s="3" t="s">
-        <v>851</v>
       </c>
     </row>
     <row r="24" spans="1:343" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A24" s="3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="P24" s="3" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="W24" s="3" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="AU24" s="3" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="AW24" s="3" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="AY24" s="3" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="BA24" s="3" t="s">
-        <v>243</v>
-      </c>
-      <c r="BB24" s="3" t="s">
-        <v>249</v>
-      </c>
-      <c r="BC24" s="3" t="s">
-        <v>253</v>
+        <v>242</v>
       </c>
       <c r="BD24" s="3" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="BE24" s="3" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="BF24" s="3" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="BG24" s="3" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="BH24" s="3" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="BI24" s="3" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="FR24" s="3" t="s">
-        <v>582</v>
+        <v>233</v>
       </c>
       <c r="HX24" s="3" t="s">
-        <v>734</v>
+        <v>733</v>
       </c>
       <c r="IA24" s="3" t="s">
-        <v>747</v>
+        <v>746</v>
       </c>
       <c r="IC24" s="3" t="s">
-        <v>756</v>
-      </c>
-      <c r="IG24" s="3" t="s">
-        <v>233</v>
+        <v>755</v>
       </c>
       <c r="JB24" s="3" t="s">
-        <v>840</v>
+        <v>839</v>
       </c>
       <c r="JF24" s="3" t="s">
-        <v>852</v>
+        <v>851</v>
       </c>
     </row>
     <row r="25" spans="1:343" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A25" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="P25" s="3" t="s">
-        <v>102</v>
+        <v>101</v>
+      </c>
+      <c r="W25" s="3" t="s">
+        <v>122</v>
       </c>
       <c r="AU25" s="3" t="s">
-        <v>212</v>
+        <v>211</v>
+      </c>
+      <c r="AW25" s="3" t="s">
+        <v>221</v>
       </c>
       <c r="AY25" s="3" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="BA25" s="3" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="BB25" s="3" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="BC25" s="3" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="BD25" s="3" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="BE25" s="3" t="s">
-        <v>260</v>
+        <v>265</v>
       </c>
       <c r="BF25" s="3" t="s">
-        <v>260</v>
+        <v>269</v>
       </c>
       <c r="BG25" s="3" t="s">
-        <v>260</v>
+        <v>273</v>
       </c>
       <c r="BH25" s="3" t="s">
-        <v>260</v>
+        <v>277</v>
       </c>
       <c r="BI25" s="3" t="s">
+        <v>282</v>
+      </c>
+      <c r="FR25" s="3" t="s">
+        <v>582</v>
+      </c>
+      <c r="HX25" s="3" t="s">
+        <v>734</v>
+      </c>
+      <c r="IA25" s="3" t="s">
+        <v>747</v>
+      </c>
+      <c r="IC25" s="3" t="s">
+        <v>756</v>
+      </c>
+      <c r="IG25" s="3" t="s">
         <v>233</v>
       </c>
-      <c r="DP25" s="3" t="s">
-        <v>433</v>
-      </c>
-      <c r="DX25" s="3" t="s">
-        <v>457</v>
-      </c>
-      <c r="EJ25" s="3" t="s">
-        <v>490</v>
-      </c>
-      <c r="EV25" s="3" t="s">
-        <v>523</v>
-      </c>
-      <c r="EX25" s="3" t="s">
-        <v>528</v>
-      </c>
-      <c r="FB25" s="3" t="s">
-        <v>541</v>
-      </c>
-      <c r="FJ25" s="3" t="s">
-        <v>562</v>
-      </c>
-      <c r="FR25" s="3" t="s">
-        <v>583</v>
-      </c>
-      <c r="GO25" s="3" t="s">
-        <v>645</v>
-      </c>
-      <c r="IC25" s="3" t="s">
-        <v>757</v>
-      </c>
-      <c r="IG25" s="3" t="s">
-        <v>769</v>
+      <c r="JB25" s="3" t="s">
+        <v>840</v>
+      </c>
+      <c r="JF25" s="3" t="s">
+        <v>852</v>
       </c>
     </row>
     <row r="26" spans="1:343" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A26" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="P26" s="3" t="s">
+        <v>102</v>
+      </c>
+      <c r="AU26" s="3" t="s">
+        <v>212</v>
+      </c>
+      <c r="AY26" s="3" t="s">
+        <v>232</v>
+      </c>
+      <c r="BA26" s="3" t="s">
+        <v>244</v>
+      </c>
+      <c r="BB26" s="3" t="s">
+        <v>250</v>
+      </c>
+      <c r="BC26" s="3" t="s">
+        <v>254</v>
+      </c>
+      <c r="BD26" s="3" t="s">
+        <v>260</v>
+      </c>
+      <c r="BE26" s="3" t="s">
+        <v>260</v>
+      </c>
+      <c r="BF26" s="3" t="s">
+        <v>260</v>
+      </c>
+      <c r="BG26" s="3" t="s">
+        <v>260</v>
+      </c>
+      <c r="BH26" s="3" t="s">
+        <v>260</v>
+      </c>
+      <c r="BI26" s="3" t="s">
+        <v>233</v>
+      </c>
+      <c r="DP26" s="3" t="s">
+        <v>433</v>
+      </c>
+      <c r="DX26" s="3" t="s">
+        <v>457</v>
+      </c>
+      <c r="EJ26" s="3" t="s">
+        <v>490</v>
+      </c>
+      <c r="EV26" s="3" t="s">
+        <v>523</v>
+      </c>
+      <c r="EX26" s="3" t="s">
+        <v>528</v>
+      </c>
+      <c r="FB26" s="3" t="s">
+        <v>541</v>
+      </c>
+      <c r="FJ26" s="3" t="s">
+        <v>562</v>
+      </c>
+      <c r="FR26" s="3" t="s">
+        <v>583</v>
+      </c>
+      <c r="GO26" s="3" t="s">
+        <v>645</v>
+      </c>
+      <c r="IC26" s="3" t="s">
+        <v>757</v>
+      </c>
+      <c r="IG26" s="3" t="s">
+        <v>769</v>
+      </c>
+    </row>
+    <row r="27" spans="1:343" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A27" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="P26" s="3" t="s">
+      <c r="P27" s="3" t="s">
         <v>103</v>
       </c>
-      <c r="AU26" s="3" t="s">
+      <c r="AU27" s="3" t="s">
         <v>213</v>
       </c>
-      <c r="AW26" s="3" t="s">
+      <c r="AW27" s="3" t="s">
         <v>222</v>
       </c>
-      <c r="AY26" s="3" t="s">
+      <c r="AY27" s="3" t="s">
         <v>233</v>
       </c>
-      <c r="BA26" s="3" t="s">
+      <c r="BA27" s="3" t="s">
         <v>245</v>
       </c>
-      <c r="BC26" s="3" t="s">
+      <c r="BC27" s="3" t="s">
         <v>255</v>
       </c>
-      <c r="BD26" s="3" t="s">
+      <c r="BD27" s="3" t="s">
         <v>261</v>
       </c>
-      <c r="BE26" s="3" t="s">
+      <c r="BE27" s="3" t="s">
         <v>261</v>
       </c>
-      <c r="BF26" s="3" t="s">
+      <c r="BF27" s="3" t="s">
         <v>261</v>
       </c>
-      <c r="BG26" s="3" t="s">
+      <c r="BG27" s="3" t="s">
         <v>261</v>
       </c>
-      <c r="BH26" s="3" t="s">
+      <c r="BH27" s="3" t="s">
         <v>261</v>
       </c>
-      <c r="FR26" s="3" t="s">
+      <c r="FR27" s="3" t="s">
         <v>584</v>
       </c>
-      <c r="HX26" s="3" t="s">
+      <c r="HX27" s="3" t="s">
         <v>735</v>
       </c>
-      <c r="IA26" s="3" t="s">
+      <c r="IA27" s="3" t="s">
         <v>748</v>
       </c>
-      <c r="IC26" s="3" t="s">
+      <c r="IC27" s="3" t="s">
         <v>758</v>
       </c>
-      <c r="IG26" s="3" t="s">
+      <c r="IG27" s="3" t="s">
         <v>770</v>
       </c>
-      <c r="JB26" s="3" t="s">
+      <c r="JB27" s="3" t="s">
         <v>841</v>
       </c>
-      <c r="JF26" s="3" t="s">
+      <c r="JF27" s="3" t="s">
         <v>853</v>
       </c>
     </row>
-    <row r="27" spans="1:343" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="7" t="s">
+    <row r="28" spans="1:343" s="7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A28" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="AQ27" s="7" t="s">
+      <c r="AQ28" s="7" t="s">
         <v>196</v>
       </c>
-      <c r="AZ27" s="7" t="s">
+      <c r="AZ28" s="7" t="s">
         <v>238</v>
       </c>
-      <c r="KS27" s="7" t="s">
+      <c r="KS28" s="7" t="s">
         <v>1061</v>
-      </c>
-    </row>
-    <row r="28" spans="1:343" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="AM28" s="4">
-        <v>1</v>
-      </c>
-      <c r="LK28" s="4">
-        <v>2</v>
       </c>
     </row>
     <row r="29" spans="1:343" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A29" s="4" t="s">
-        <v>1022</v>
+        <v>22</v>
+      </c>
+      <c r="AM29" s="4">
+        <v>1</v>
+      </c>
+      <c r="LK29" s="4">
+        <v>2</v>
       </c>
     </row>
     <row r="30" spans="1:343" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A30" s="4" t="s">
-        <v>1141</v>
-      </c>
-      <c r="KQ30" s="4" t="s">
-        <v>1139</v>
+        <v>1022</v>
       </c>
     </row>
     <row r="31" spans="1:343" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A31" s="4" t="s">
-        <v>1065</v>
+        <v>1141</v>
+      </c>
+      <c r="KQ31" s="4" t="s">
+        <v>1139</v>
       </c>
     </row>
     <row r="32" spans="1:343" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A32" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="C32" s="4">
-        <v>-1</v>
-      </c>
-      <c r="D32" s="4">
-        <v>-1</v>
-      </c>
-      <c r="E32" s="4">
-        <v>-1</v>
-      </c>
-      <c r="F32" s="4">
-        <v>-1</v>
-      </c>
-      <c r="G32" s="4">
-        <v>-1</v>
-      </c>
-      <c r="H32" s="4">
-        <v>-1</v>
-      </c>
-      <c r="I32" s="4">
-        <v>1</v>
-      </c>
-      <c r="L32" s="4">
-        <v>1</v>
-      </c>
-      <c r="N32" s="4">
-        <v>10</v>
-      </c>
-      <c r="R32" s="4">
-        <v>-1</v>
-      </c>
-      <c r="T32" s="4">
-        <v>-1</v>
-      </c>
-      <c r="AA32" s="4">
-        <v>10</v>
-      </c>
-      <c r="AJ32" s="4">
-        <v>-2</v>
-      </c>
-      <c r="AN32" s="4">
-        <v>10</v>
-      </c>
-      <c r="AQ32" s="4">
-        <v>100</v>
-      </c>
-      <c r="AZ32" s="4">
-        <v>1000</v>
-      </c>
-      <c r="BL32" s="4">
-        <v>-1</v>
-      </c>
-      <c r="BN32" s="4">
-        <v>1</v>
-      </c>
-      <c r="BP32" s="4">
-        <v>-1</v>
-      </c>
-      <c r="BS32" s="4">
-        <v>-1</v>
-      </c>
-      <c r="DF32" s="4">
-        <v>0</v>
-      </c>
-      <c r="DG32" s="4">
-        <v>0</v>
-      </c>
-      <c r="DH32" s="4">
-        <v>0</v>
-      </c>
-      <c r="DI32" s="4">
-        <v>0</v>
-      </c>
-      <c r="DJ32" s="4">
-        <v>0</v>
-      </c>
-      <c r="DK32" s="4">
-        <v>0</v>
-      </c>
-      <c r="DL32" s="4">
-        <v>0</v>
-      </c>
-      <c r="DM32" s="4">
-        <v>0</v>
-      </c>
-      <c r="DO32" s="4">
-        <v>-1</v>
-      </c>
-      <c r="DQ32" s="4">
-        <v>-1</v>
-      </c>
-      <c r="DZ32" s="4">
-        <v>10</v>
-      </c>
-      <c r="EI32" s="4">
-        <v>10</v>
-      </c>
-      <c r="EK32" s="4">
-        <v>-1</v>
-      </c>
-      <c r="EQ32" s="4">
-        <v>-1</v>
-      </c>
-      <c r="ES32" s="4">
-        <v>-1</v>
-      </c>
-      <c r="EY32" s="4">
-        <v>-1</v>
-      </c>
-      <c r="FC32" s="4">
-        <v>-1</v>
-      </c>
-      <c r="FE32" s="4">
-        <v>-1</v>
-      </c>
-      <c r="FF32" s="4">
-        <v>-1</v>
-      </c>
-      <c r="FN32" s="4">
-        <v>-1</v>
-      </c>
-      <c r="FO32" s="4">
-        <v>-1</v>
-      </c>
-      <c r="FP32" s="4">
-        <v>-1</v>
-      </c>
-      <c r="FU32" s="4">
-        <v>-1</v>
-      </c>
-      <c r="FV32" s="4">
-        <v>-1</v>
-      </c>
-      <c r="FW32" s="4">
-        <v>-1</v>
-      </c>
-      <c r="FX32" s="4">
-        <v>-1</v>
-      </c>
-      <c r="FY32" s="4">
-        <v>-1</v>
-      </c>
-      <c r="FZ32" s="4">
-        <v>-1</v>
-      </c>
-      <c r="GA32" s="4">
-        <v>-1</v>
-      </c>
-      <c r="GB32" s="4">
-        <v>-1</v>
-      </c>
-      <c r="GC32" s="4">
-        <v>-1</v>
-      </c>
-      <c r="GL32" s="4">
-        <v>-1</v>
-      </c>
-      <c r="GT32" s="4">
-        <v>-1</v>
-      </c>
-      <c r="GU32" s="4">
-        <v>-1</v>
-      </c>
-      <c r="GV32" s="4">
-        <v>-1</v>
-      </c>
-      <c r="GX32" s="4">
-        <v>-1</v>
-      </c>
-      <c r="HM32" s="4">
-        <v>5</v>
-      </c>
-      <c r="HO32" s="4">
-        <v>15</v>
-      </c>
-      <c r="HR32" s="4">
-        <v>-1</v>
-      </c>
-      <c r="HU32" s="4">
-        <v>1</v>
-      </c>
-      <c r="IL32" s="4">
-        <v>10</v>
-      </c>
-      <c r="IN32" s="4">
-        <v>100</v>
-      </c>
-      <c r="IO32" s="4">
-        <v>0</v>
-      </c>
-      <c r="IS32" s="4">
-        <v>100</v>
-      </c>
-      <c r="IT32" s="4">
-        <v>100</v>
-      </c>
-      <c r="JG32" s="4">
-        <v>100</v>
-      </c>
-      <c r="JL32" s="4">
-        <v>0</v>
-      </c>
-      <c r="JO32" s="4">
-        <v>1</v>
-      </c>
-      <c r="JP32" s="4">
-        <v>-1</v>
-      </c>
-      <c r="JQ32" s="4">
-        <v>1</v>
-      </c>
-      <c r="JR32" s="4">
-        <v>6000</v>
-      </c>
-      <c r="JS32" s="4">
-        <v>1</v>
-      </c>
-      <c r="JT32" s="4">
-        <v>15</v>
-      </c>
-      <c r="JV32" s="4">
-        <v>3000</v>
-      </c>
-      <c r="JW32" s="4">
-        <v>1</v>
-      </c>
-      <c r="JZ32" s="4">
-        <v>15</v>
-      </c>
-      <c r="KA32" s="4">
-        <v>1008000</v>
-      </c>
-      <c r="KB32" s="4">
-        <v>100</v>
-      </c>
-      <c r="KC32" s="4">
-        <v>10</v>
-      </c>
-      <c r="KD32" s="4">
-        <v>100</v>
-      </c>
-      <c r="KF32" s="4">
-        <v>5</v>
-      </c>
-      <c r="KG32" s="4">
-        <v>1</v>
-      </c>
-      <c r="KJ32" s="4">
-        <v>0</v>
-      </c>
-      <c r="KK32" s="4">
-        <v>1</v>
-      </c>
-      <c r="KN32" s="4">
-        <v>6000</v>
-      </c>
-      <c r="KO32" s="4">
-        <v>-1</v>
-      </c>
-      <c r="KP32" s="4">
-        <v>-1</v>
-      </c>
-      <c r="KQ32" s="4">
-        <v>100</v>
-      </c>
-      <c r="KU32" s="4">
-        <v>-1</v>
-      </c>
-      <c r="KY32" s="4">
-        <v>-1</v>
-      </c>
-      <c r="LC32" s="4">
-        <v>-1</v>
-      </c>
-      <c r="LE32" s="4">
-        <v>100</v>
-      </c>
-      <c r="LF32" s="4">
-        <v>-5</v>
-      </c>
-      <c r="LG32" s="4">
-        <v>-1</v>
-      </c>
-      <c r="LH32" s="4">
-        <v>1</v>
-      </c>
-      <c r="LM32" s="4">
-        <v>5</v>
-      </c>
-      <c r="LS32" s="4">
-        <v>-1</v>
-      </c>
-      <c r="LT32" s="4">
-        <v>48000</v>
-      </c>
-      <c r="LV32" s="4">
-        <v>1</v>
-      </c>
-      <c r="LX32" s="4">
-        <v>0</v>
-      </c>
-      <c r="LY32" s="4">
-        <v>144000</v>
-      </c>
-      <c r="MC32" s="4">
-        <v>1</v>
-      </c>
-      <c r="ME32" s="4">
-        <v>5</v>
+        <v>1065</v>
       </c>
     </row>
     <row r="33" spans="1:343" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A33" s="4" t="s">
-        <v>1140</v>
-      </c>
-      <c r="KQ33" s="4" t="b">
+        <v>7</v>
+      </c>
+      <c r="C33" s="4">
+        <v>-1</v>
+      </c>
+      <c r="D33" s="4">
+        <v>-1</v>
+      </c>
+      <c r="E33" s="4">
+        <v>-1</v>
+      </c>
+      <c r="F33" s="4">
+        <v>-1</v>
+      </c>
+      <c r="G33" s="4">
+        <v>-1</v>
+      </c>
+      <c r="H33" s="4">
+        <v>-1</v>
+      </c>
+      <c r="I33" s="4">
         <v>1</v>
+      </c>
+      <c r="L33" s="4">
+        <v>1</v>
+      </c>
+      <c r="N33" s="4">
+        <v>10</v>
+      </c>
+      <c r="R33" s="4">
+        <v>-1</v>
+      </c>
+      <c r="T33" s="4">
+        <v>-1</v>
+      </c>
+      <c r="AA33" s="4">
+        <v>10</v>
+      </c>
+      <c r="AJ33" s="4">
+        <v>-2</v>
+      </c>
+      <c r="AN33" s="4">
+        <v>10</v>
+      </c>
+      <c r="AQ33" s="4">
+        <v>100</v>
+      </c>
+      <c r="AZ33" s="4">
+        <v>1000</v>
+      </c>
+      <c r="BL33" s="4">
+        <v>-1</v>
+      </c>
+      <c r="BN33" s="4">
+        <v>1</v>
+      </c>
+      <c r="BP33" s="4">
+        <v>-1</v>
+      </c>
+      <c r="BS33" s="4">
+        <v>-1</v>
+      </c>
+      <c r="DF33" s="4">
+        <v>0</v>
+      </c>
+      <c r="DG33" s="4">
+        <v>0</v>
+      </c>
+      <c r="DH33" s="4">
+        <v>0</v>
+      </c>
+      <c r="DI33" s="4">
+        <v>0</v>
+      </c>
+      <c r="DJ33" s="4">
+        <v>0</v>
+      </c>
+      <c r="DK33" s="4">
+        <v>0</v>
+      </c>
+      <c r="DL33" s="4">
+        <v>0</v>
+      </c>
+      <c r="DM33" s="4">
+        <v>0</v>
+      </c>
+      <c r="DO33" s="4">
+        <v>-1</v>
+      </c>
+      <c r="DQ33" s="4">
+        <v>-1</v>
+      </c>
+      <c r="DZ33" s="4">
+        <v>10</v>
+      </c>
+      <c r="EI33" s="4">
+        <v>10</v>
+      </c>
+      <c r="EK33" s="4">
+        <v>-1</v>
+      </c>
+      <c r="EQ33" s="4">
+        <v>-1</v>
+      </c>
+      <c r="ES33" s="4">
+        <v>-1</v>
+      </c>
+      <c r="EY33" s="4">
+        <v>-1</v>
+      </c>
+      <c r="FC33" s="4">
+        <v>-1</v>
+      </c>
+      <c r="FE33" s="4">
+        <v>-1</v>
+      </c>
+      <c r="FF33" s="4">
+        <v>-1</v>
+      </c>
+      <c r="FN33" s="4">
+        <v>-1</v>
+      </c>
+      <c r="FO33" s="4">
+        <v>-1</v>
+      </c>
+      <c r="FP33" s="4">
+        <v>-1</v>
+      </c>
+      <c r="FU33" s="4">
+        <v>-1</v>
+      </c>
+      <c r="FV33" s="4">
+        <v>-1</v>
+      </c>
+      <c r="FW33" s="4">
+        <v>-1</v>
+      </c>
+      <c r="FX33" s="4">
+        <v>-1</v>
+      </c>
+      <c r="FY33" s="4">
+        <v>-1</v>
+      </c>
+      <c r="FZ33" s="4">
+        <v>-1</v>
+      </c>
+      <c r="GA33" s="4">
+        <v>-1</v>
+      </c>
+      <c r="GB33" s="4">
+        <v>-1</v>
+      </c>
+      <c r="GC33" s="4">
+        <v>-1</v>
+      </c>
+      <c r="GL33" s="4">
+        <v>-1</v>
+      </c>
+      <c r="GT33" s="4">
+        <v>-1</v>
+      </c>
+      <c r="GU33" s="4">
+        <v>-1</v>
+      </c>
+      <c r="GV33" s="4">
+        <v>-1</v>
+      </c>
+      <c r="GX33" s="4">
+        <v>-1</v>
+      </c>
+      <c r="HM33" s="4">
+        <v>5</v>
+      </c>
+      <c r="HO33" s="4">
+        <v>15</v>
+      </c>
+      <c r="HR33" s="4">
+        <v>-1</v>
+      </c>
+      <c r="HU33" s="4">
+        <v>1</v>
+      </c>
+      <c r="IL33" s="4">
+        <v>10</v>
+      </c>
+      <c r="IN33" s="4">
+        <v>100</v>
+      </c>
+      <c r="IO33" s="4">
+        <v>0</v>
+      </c>
+      <c r="IS33" s="4">
+        <v>100</v>
+      </c>
+      <c r="IT33" s="4">
+        <v>100</v>
+      </c>
+      <c r="JG33" s="4">
+        <v>100</v>
+      </c>
+      <c r="JL33" s="4">
+        <v>0</v>
+      </c>
+      <c r="JO33" s="4">
+        <v>1</v>
+      </c>
+      <c r="JP33" s="4">
+        <v>-1</v>
+      </c>
+      <c r="JQ33" s="4">
+        <v>1</v>
+      </c>
+      <c r="JR33" s="4">
+        <v>6000</v>
+      </c>
+      <c r="JS33" s="4">
+        <v>1</v>
+      </c>
+      <c r="JT33" s="4">
+        <v>15</v>
+      </c>
+      <c r="JV33" s="4">
+        <v>3000</v>
+      </c>
+      <c r="JW33" s="4">
+        <v>1</v>
+      </c>
+      <c r="JZ33" s="4">
+        <v>15</v>
+      </c>
+      <c r="KA33" s="4">
+        <v>1008000</v>
+      </c>
+      <c r="KB33" s="4">
+        <v>100</v>
+      </c>
+      <c r="KC33" s="4">
+        <v>10</v>
+      </c>
+      <c r="KD33" s="4">
+        <v>100</v>
+      </c>
+      <c r="KF33" s="4">
+        <v>5</v>
+      </c>
+      <c r="KG33" s="4">
+        <v>1</v>
+      </c>
+      <c r="KJ33" s="4">
+        <v>0</v>
+      </c>
+      <c r="KK33" s="4">
+        <v>1</v>
+      </c>
+      <c r="KN33" s="4">
+        <v>6000</v>
+      </c>
+      <c r="KO33" s="4">
+        <v>-1</v>
+      </c>
+      <c r="KP33" s="4">
+        <v>-1</v>
+      </c>
+      <c r="KQ33" s="4">
+        <v>100</v>
+      </c>
+      <c r="KU33" s="4">
+        <v>-1</v>
+      </c>
+      <c r="KY33" s="4">
+        <v>-1</v>
+      </c>
+      <c r="LC33" s="4">
+        <v>-1</v>
+      </c>
+      <c r="LE33" s="4">
+        <v>100</v>
+      </c>
+      <c r="LF33" s="4">
+        <v>-5</v>
+      </c>
+      <c r="LG33" s="4">
+        <v>-1</v>
+      </c>
+      <c r="LH33" s="4">
+        <v>1</v>
+      </c>
+      <c r="LM33" s="4">
+        <v>5</v>
+      </c>
+      <c r="LS33" s="4">
+        <v>-1</v>
+      </c>
+      <c r="LT33" s="4">
+        <v>48000</v>
+      </c>
+      <c r="LV33" s="4">
+        <v>1</v>
+      </c>
+      <c r="LX33" s="4">
+        <v>0</v>
+      </c>
+      <c r="LY33" s="4">
+        <v>144000</v>
+      </c>
+      <c r="MC33" s="4">
+        <v>1</v>
+      </c>
+      <c r="ME33" s="4">
+        <v>5</v>
       </c>
     </row>
     <row r="34" spans="1:343" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A34" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="C34" s="4" t="s">
-        <v>55</v>
-      </c>
-      <c r="D34" s="4" t="s">
-        <v>59</v>
-      </c>
-      <c r="E34" s="4" t="s">
-        <v>61</v>
-      </c>
-      <c r="F34" s="4" t="s">
-        <v>64</v>
-      </c>
-      <c r="G34" s="4" t="s">
-        <v>66</v>
-      </c>
-      <c r="H34" s="4" t="s">
-        <v>68</v>
-      </c>
-      <c r="I34" s="4" t="s">
-        <v>70</v>
-      </c>
-      <c r="L34" s="4" t="s">
-        <v>81</v>
-      </c>
-      <c r="N34" s="4" t="s">
-        <v>91</v>
-      </c>
-      <c r="R34" s="4" t="s">
-        <v>107</v>
-      </c>
-      <c r="T34" s="4" t="s">
-        <v>111</v>
-      </c>
-      <c r="AA34" s="4" t="s">
-        <v>133</v>
-      </c>
-      <c r="AJ34" s="4" t="s">
-        <v>164</v>
-      </c>
-      <c r="AM34" s="4" t="s">
-        <v>178</v>
-      </c>
-      <c r="AN34" s="4" t="s">
-        <v>1076</v>
-      </c>
-      <c r="AQ34" s="4" t="s">
-        <v>195</v>
-      </c>
-      <c r="AZ34" s="4" t="s">
-        <v>236</v>
-      </c>
-      <c r="BL34" s="4" t="s">
-        <v>290</v>
-      </c>
-      <c r="BN34" s="4" t="s">
-        <v>296</v>
-      </c>
-      <c r="BP34" s="4" t="s">
-        <v>301</v>
-      </c>
-      <c r="BS34" s="4" t="s">
-        <v>312</v>
-      </c>
-      <c r="DF34" s="4" t="s">
-        <v>404</v>
-      </c>
-      <c r="DG34" s="4" t="s">
-        <v>404</v>
-      </c>
-      <c r="DH34" s="4" t="s">
-        <v>404</v>
-      </c>
-      <c r="DI34" s="4" t="s">
-        <v>404</v>
-      </c>
-      <c r="DJ34" s="4" t="s">
-        <v>404</v>
-      </c>
-      <c r="DK34" s="4" t="s">
-        <v>404</v>
-      </c>
-      <c r="DL34" s="4" t="s">
-        <v>404</v>
-      </c>
-      <c r="DM34" s="4" t="s">
-        <v>404</v>
-      </c>
-      <c r="DO34" s="4" t="s">
-        <v>426</v>
-      </c>
-      <c r="DQ34" s="4" t="s">
-        <v>434</v>
-      </c>
-      <c r="DZ34" s="4" t="s">
-        <v>460</v>
-      </c>
-      <c r="EI34" s="4" t="s">
-        <v>485</v>
-      </c>
-      <c r="EK34" s="4" t="s">
-        <v>491</v>
-      </c>
-      <c r="EQ34" s="4" t="s">
-        <v>509</v>
-      </c>
-      <c r="ES34" s="4" t="s">
-        <v>513</v>
-      </c>
-      <c r="EY34" s="4" t="s">
-        <v>529</v>
-      </c>
-      <c r="FC34" s="4" t="s">
-        <v>460</v>
-      </c>
-      <c r="FE34" s="4" t="s">
-        <v>546</v>
-      </c>
-      <c r="FF34" s="4" t="s">
-        <v>548</v>
-      </c>
-      <c r="FN34" s="4" t="s">
-        <v>570</v>
-      </c>
-      <c r="FO34" s="4" t="s">
-        <v>572</v>
-      </c>
-      <c r="FP34" s="4" t="s">
-        <v>485</v>
-      </c>
-      <c r="FU34" s="4" t="s">
-        <v>589</v>
-      </c>
-      <c r="FV34" s="4" t="s">
-        <v>592</v>
-      </c>
-      <c r="FW34" s="4" t="s">
-        <v>595</v>
-      </c>
-      <c r="FX34" s="4" t="s">
-        <v>598</v>
-      </c>
-      <c r="FY34" s="4" t="s">
-        <v>601</v>
-      </c>
-      <c r="FZ34" s="4" t="s">
-        <v>604</v>
-      </c>
-      <c r="GA34" s="4" t="s">
-        <v>607</v>
-      </c>
-      <c r="GB34" s="4" t="s">
-        <v>610</v>
-      </c>
-      <c r="GC34" s="4" t="s">
-        <v>613</v>
-      </c>
-      <c r="GL34" s="4" t="s">
-        <v>636</v>
-      </c>
-      <c r="GT34" s="4" t="s">
-        <v>654</v>
-      </c>
-      <c r="GU34" s="4" t="s">
-        <v>656</v>
-      </c>
-      <c r="GV34" s="4" t="s">
-        <v>658</v>
-      </c>
-      <c r="GX34" s="4" t="s">
-        <v>663</v>
-      </c>
-      <c r="HM34" s="4" t="s">
-        <v>1131</v>
-      </c>
-      <c r="HO34" s="4" t="s">
-        <v>700</v>
-      </c>
-      <c r="HR34" s="4" t="s">
-        <v>709</v>
-      </c>
-      <c r="HU34" s="4" t="s">
-        <v>722</v>
-      </c>
-      <c r="IL34" s="4" t="s">
-        <v>782</v>
-      </c>
-      <c r="IN34" s="4" t="s">
-        <v>789</v>
-      </c>
-      <c r="IO34" s="4" t="s">
-        <v>794</v>
-      </c>
-      <c r="IS34" s="4" t="s">
-        <v>807</v>
-      </c>
-      <c r="IT34" s="4" t="s">
-        <v>789</v>
-      </c>
-      <c r="JE34" s="4" t="s">
-        <v>847</v>
-      </c>
-      <c r="JG34" s="4" t="s">
-        <v>854</v>
-      </c>
-      <c r="JH34" s="4" t="s">
-        <v>859</v>
-      </c>
-      <c r="JL34" s="4" t="s">
-        <v>870</v>
-      </c>
-      <c r="JO34" s="4" t="s">
-        <v>878</v>
-      </c>
-      <c r="JP34" s="4" t="s">
-        <v>882</v>
-      </c>
-      <c r="JQ34" s="4" t="s">
-        <v>884</v>
-      </c>
-      <c r="JR34" s="4" t="s">
-        <v>887</v>
-      </c>
-      <c r="JS34" s="4" t="s">
-        <v>891</v>
-      </c>
-      <c r="JT34" s="4" t="s">
-        <v>894</v>
-      </c>
-      <c r="JV34" s="4" t="s">
-        <v>902</v>
-      </c>
-      <c r="JW34" s="4" t="s">
-        <v>905</v>
-      </c>
-      <c r="JZ34" s="4" t="s">
-        <v>913</v>
-      </c>
-      <c r="KA34" s="4" t="s">
-        <v>917</v>
-      </c>
-      <c r="KB34" s="4" t="s">
-        <v>921</v>
-      </c>
-      <c r="KC34" s="4" t="s">
-        <v>925</v>
-      </c>
-      <c r="KD34" s="4" t="s">
-        <v>927</v>
-      </c>
-      <c r="KF34" s="4" t="s">
-        <v>963</v>
-      </c>
-      <c r="KG34" s="4" t="s">
-        <v>933</v>
-      </c>
-      <c r="KI34" s="4" t="s">
-        <v>935</v>
-      </c>
-      <c r="KJ34" s="4" t="s">
-        <v>936</v>
-      </c>
-      <c r="KK34" s="4" t="s">
-        <v>969</v>
-      </c>
-      <c r="KN34" s="4" t="s">
-        <v>976</v>
-      </c>
-      <c r="KO34" s="4" t="s">
-        <v>940</v>
-      </c>
-      <c r="KP34" s="4" t="s">
-        <v>941</v>
-      </c>
-      <c r="KQ34" s="4" t="s">
-        <v>942</v>
-      </c>
-      <c r="KS34" s="4" t="s">
-        <v>1062</v>
-      </c>
-      <c r="KU34" s="4" t="s">
-        <v>946</v>
-      </c>
-      <c r="KY34" s="4" t="s">
-        <v>1001</v>
-      </c>
-      <c r="LC34" s="4" t="s">
-        <v>954</v>
-      </c>
-      <c r="LE34" s="4" t="s">
-        <v>956</v>
-      </c>
-      <c r="LF34" s="4" t="s">
-        <v>1057</v>
-      </c>
-      <c r="LG34" s="4" t="s">
-        <v>957</v>
-      </c>
-      <c r="LH34" s="4" t="s">
-        <v>958</v>
-      </c>
-      <c r="LK34" s="4" t="s">
-        <v>178</v>
-      </c>
-      <c r="LM34" s="4" t="s">
-        <v>1078</v>
-      </c>
-      <c r="LO34" s="4" t="s">
-        <v>1081</v>
-      </c>
-      <c r="LS34" s="4" t="s">
-        <v>1095</v>
-      </c>
-      <c r="LT34" s="4" t="s">
-        <v>1098</v>
-      </c>
-      <c r="LV34" s="4" t="s">
-        <v>1102</v>
-      </c>
-      <c r="LX34" s="4" t="s">
-        <v>1103</v>
-      </c>
-      <c r="LY34" s="4" t="s">
-        <v>1104</v>
-      </c>
-      <c r="MC34" s="4" t="s">
-        <v>1124</v>
-      </c>
-      <c r="ME34" s="4" t="s">
-        <v>1135</v>
+        <v>1140</v>
+      </c>
+      <c r="KQ34" s="4" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="35" spans="1:343" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A35" s="4" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C35" s="4" t="s">
         <v>55</v>
@@ -13010,8 +12761,11 @@
       <c r="AA35" s="4" t="s">
         <v>133</v>
       </c>
+      <c r="AJ35" s="4" t="s">
+        <v>164</v>
+      </c>
       <c r="AM35" s="4" t="s">
-        <v>175</v>
+        <v>178</v>
       </c>
       <c r="AN35" s="4" t="s">
         <v>1076</v>
@@ -13019,6 +12773,9 @@
       <c r="AQ35" s="4" t="s">
         <v>195</v>
       </c>
+      <c r="AZ35" s="4" t="s">
+        <v>236</v>
+      </c>
       <c r="BL35" s="4" t="s">
         <v>290</v>
       </c>
@@ -13032,28 +12789,28 @@
         <v>312</v>
       </c>
       <c r="DF35" s="4" t="s">
-        <v>402</v>
+        <v>404</v>
       </c>
       <c r="DG35" s="4" t="s">
-        <v>407</v>
+        <v>404</v>
       </c>
       <c r="DH35" s="4" t="s">
-        <v>410</v>
+        <v>404</v>
       </c>
       <c r="DI35" s="4" t="s">
-        <v>412</v>
+        <v>404</v>
       </c>
       <c r="DJ35" s="4" t="s">
-        <v>414</v>
+        <v>404</v>
       </c>
       <c r="DK35" s="4" t="s">
-        <v>416</v>
+        <v>404</v>
       </c>
       <c r="DL35" s="4" t="s">
-        <v>418</v>
+        <v>404</v>
       </c>
       <c r="DM35" s="4" t="s">
-        <v>420</v>
+        <v>404</v>
       </c>
       <c r="DO35" s="4" t="s">
         <v>426</v>
@@ -13080,7 +12837,7 @@
         <v>529</v>
       </c>
       <c r="FC35" s="4" t="s">
-        <v>542</v>
+        <v>460</v>
       </c>
       <c r="FE35" s="4" t="s">
         <v>546</v>
@@ -13095,7 +12852,7 @@
         <v>572</v>
       </c>
       <c r="FP35" s="4" t="s">
-        <v>574</v>
+        <v>485</v>
       </c>
       <c r="FU35" s="4" t="s">
         <v>589</v>
@@ -13173,7 +12930,7 @@
         <v>854</v>
       </c>
       <c r="JH35" s="4" t="s">
-        <v>857</v>
+        <v>859</v>
       </c>
       <c r="JL35" s="4" t="s">
         <v>870</v>
@@ -13233,7 +12990,7 @@
         <v>969</v>
       </c>
       <c r="KN35" s="4" t="s">
-        <v>939</v>
+        <v>976</v>
       </c>
       <c r="KO35" s="4" t="s">
         <v>940</v>
@@ -13245,7 +13002,7 @@
         <v>942</v>
       </c>
       <c r="KS35" s="4" t="s">
-        <v>944</v>
+        <v>1062</v>
       </c>
       <c r="KU35" s="4" t="s">
         <v>946</v>
@@ -13260,7 +13017,7 @@
         <v>956</v>
       </c>
       <c r="LF35" s="4" t="s">
-        <v>1055</v>
+        <v>1057</v>
       </c>
       <c r="LG35" s="4" t="s">
         <v>957</v>
@@ -13269,7 +13026,7 @@
         <v>958</v>
       </c>
       <c r="LK35" s="4" t="s">
-        <v>961</v>
+        <v>178</v>
       </c>
       <c r="LM35" s="4" t="s">
         <v>1078</v>
@@ -13281,7 +13038,7 @@
         <v>1095</v>
       </c>
       <c r="LT35" s="4" t="s">
-        <v>1099</v>
+        <v>1098</v>
       </c>
       <c r="LV35" s="4" t="s">
         <v>1102</v>
@@ -13296,305 +13053,634 @@
         <v>1124</v>
       </c>
       <c r="ME35" s="4" t="s">
-        <v>1136</v>
+        <v>1135</v>
       </c>
     </row>
     <row r="36" spans="1:343" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A36" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="C36" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="D36" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="E36" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="F36" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="G36" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="H36" s="4" t="s">
+        <v>68</v>
+      </c>
+      <c r="I36" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="L36" s="4" t="s">
+        <v>81</v>
+      </c>
+      <c r="N36" s="4" t="s">
+        <v>91</v>
+      </c>
+      <c r="R36" s="4" t="s">
+        <v>107</v>
+      </c>
+      <c r="T36" s="4" t="s">
+        <v>111</v>
+      </c>
+      <c r="AA36" s="4" t="s">
+        <v>133</v>
+      </c>
+      <c r="AM36" s="4" t="s">
+        <v>175</v>
+      </c>
+      <c r="AN36" s="4" t="s">
+        <v>1076</v>
+      </c>
+      <c r="AQ36" s="4" t="s">
+        <v>195</v>
+      </c>
+      <c r="BL36" s="4" t="s">
+        <v>290</v>
+      </c>
+      <c r="BN36" s="4" t="s">
+        <v>296</v>
+      </c>
+      <c r="BP36" s="4" t="s">
+        <v>301</v>
+      </c>
+      <c r="BS36" s="4" t="s">
+        <v>312</v>
+      </c>
+      <c r="DF36" s="4" t="s">
+        <v>402</v>
+      </c>
+      <c r="DG36" s="4" t="s">
+        <v>407</v>
+      </c>
+      <c r="DH36" s="4" t="s">
+        <v>410</v>
+      </c>
+      <c r="DI36" s="4" t="s">
+        <v>412</v>
+      </c>
+      <c r="DJ36" s="4" t="s">
+        <v>414</v>
+      </c>
+      <c r="DK36" s="4" t="s">
+        <v>416</v>
+      </c>
+      <c r="DL36" s="4" t="s">
+        <v>418</v>
+      </c>
+      <c r="DM36" s="4" t="s">
+        <v>420</v>
+      </c>
+      <c r="DO36" s="4" t="s">
+        <v>426</v>
+      </c>
+      <c r="DQ36" s="4" t="s">
+        <v>434</v>
+      </c>
+      <c r="DZ36" s="4" t="s">
+        <v>460</v>
+      </c>
+      <c r="EI36" s="4" t="s">
+        <v>485</v>
+      </c>
+      <c r="EK36" s="4" t="s">
+        <v>491</v>
+      </c>
+      <c r="EQ36" s="4" t="s">
+        <v>509</v>
+      </c>
+      <c r="ES36" s="4" t="s">
+        <v>513</v>
+      </c>
+      <c r="EY36" s="4" t="s">
+        <v>529</v>
+      </c>
+      <c r="FC36" s="4" t="s">
+        <v>542</v>
+      </c>
+      <c r="FE36" s="4" t="s">
+        <v>546</v>
+      </c>
+      <c r="FF36" s="4" t="s">
+        <v>548</v>
+      </c>
+      <c r="FN36" s="4" t="s">
+        <v>570</v>
+      </c>
+      <c r="FO36" s="4" t="s">
+        <v>572</v>
+      </c>
+      <c r="FP36" s="4" t="s">
+        <v>574</v>
+      </c>
+      <c r="FU36" s="4" t="s">
+        <v>589</v>
+      </c>
+      <c r="FV36" s="4" t="s">
+        <v>592</v>
+      </c>
+      <c r="FW36" s="4" t="s">
+        <v>595</v>
+      </c>
+      <c r="FX36" s="4" t="s">
+        <v>598</v>
+      </c>
+      <c r="FY36" s="4" t="s">
+        <v>601</v>
+      </c>
+      <c r="FZ36" s="4" t="s">
+        <v>604</v>
+      </c>
+      <c r="GA36" s="4" t="s">
+        <v>607</v>
+      </c>
+      <c r="GB36" s="4" t="s">
+        <v>610</v>
+      </c>
+      <c r="GC36" s="4" t="s">
+        <v>613</v>
+      </c>
+      <c r="GL36" s="4" t="s">
+        <v>636</v>
+      </c>
+      <c r="GT36" s="4" t="s">
+        <v>654</v>
+      </c>
+      <c r="GU36" s="4" t="s">
+        <v>656</v>
+      </c>
+      <c r="GV36" s="4" t="s">
+        <v>658</v>
+      </c>
+      <c r="GX36" s="4" t="s">
+        <v>663</v>
+      </c>
+      <c r="HM36" s="4" t="s">
+        <v>1131</v>
+      </c>
+      <c r="HO36" s="4" t="s">
+        <v>700</v>
+      </c>
+      <c r="HR36" s="4" t="s">
+        <v>709</v>
+      </c>
+      <c r="HU36" s="4" t="s">
+        <v>722</v>
+      </c>
+      <c r="IL36" s="4" t="s">
+        <v>782</v>
+      </c>
+      <c r="IN36" s="4" t="s">
+        <v>789</v>
+      </c>
+      <c r="IO36" s="4" t="s">
+        <v>794</v>
+      </c>
+      <c r="IS36" s="4" t="s">
+        <v>807</v>
+      </c>
+      <c r="IT36" s="4" t="s">
+        <v>789</v>
+      </c>
+      <c r="JE36" s="4" t="s">
+        <v>847</v>
+      </c>
+      <c r="JG36" s="4" t="s">
+        <v>854</v>
+      </c>
+      <c r="JH36" s="4" t="s">
+        <v>857</v>
+      </c>
+      <c r="JL36" s="4" t="s">
+        <v>870</v>
+      </c>
+      <c r="JO36" s="4" t="s">
+        <v>878</v>
+      </c>
+      <c r="JP36" s="4" t="s">
+        <v>882</v>
+      </c>
+      <c r="JQ36" s="4" t="s">
+        <v>884</v>
+      </c>
+      <c r="JR36" s="4" t="s">
+        <v>887</v>
+      </c>
+      <c r="JS36" s="4" t="s">
+        <v>891</v>
+      </c>
+      <c r="JT36" s="4" t="s">
+        <v>894</v>
+      </c>
+      <c r="JV36" s="4" t="s">
+        <v>902</v>
+      </c>
+      <c r="JW36" s="4" t="s">
+        <v>905</v>
+      </c>
+      <c r="JZ36" s="4" t="s">
+        <v>913</v>
+      </c>
+      <c r="KA36" s="4" t="s">
+        <v>917</v>
+      </c>
+      <c r="KB36" s="4" t="s">
+        <v>921</v>
+      </c>
+      <c r="KC36" s="4" t="s">
+        <v>925</v>
+      </c>
+      <c r="KD36" s="4" t="s">
+        <v>927</v>
+      </c>
+      <c r="KF36" s="4" t="s">
+        <v>963</v>
+      </c>
+      <c r="KG36" s="4" t="s">
+        <v>933</v>
+      </c>
+      <c r="KI36" s="4" t="s">
+        <v>935</v>
+      </c>
+      <c r="KJ36" s="4" t="s">
+        <v>936</v>
+      </c>
+      <c r="KK36" s="4" t="s">
+        <v>969</v>
+      </c>
+      <c r="KN36" s="4" t="s">
+        <v>939</v>
+      </c>
+      <c r="KO36" s="4" t="s">
+        <v>940</v>
+      </c>
+      <c r="KP36" s="4" t="s">
+        <v>941</v>
+      </c>
+      <c r="KQ36" s="4" t="s">
+        <v>942</v>
+      </c>
+      <c r="KS36" s="4" t="s">
+        <v>944</v>
+      </c>
+      <c r="KU36" s="4" t="s">
+        <v>946</v>
+      </c>
+      <c r="KY36" s="4" t="s">
+        <v>1001</v>
+      </c>
+      <c r="LC36" s="4" t="s">
+        <v>954</v>
+      </c>
+      <c r="LE36" s="4" t="s">
+        <v>956</v>
+      </c>
+      <c r="LF36" s="4" t="s">
+        <v>1055</v>
+      </c>
+      <c r="LG36" s="4" t="s">
+        <v>957</v>
+      </c>
+      <c r="LH36" s="4" t="s">
+        <v>958</v>
+      </c>
+      <c r="LK36" s="4" t="s">
+        <v>961</v>
+      </c>
+      <c r="LM36" s="4" t="s">
+        <v>1078</v>
+      </c>
+      <c r="LO36" s="4" t="s">
+        <v>1081</v>
+      </c>
+      <c r="LS36" s="4" t="s">
+        <v>1095</v>
+      </c>
+      <c r="LT36" s="4" t="s">
+        <v>1099</v>
+      </c>
+      <c r="LV36" s="4" t="s">
+        <v>1102</v>
+      </c>
+      <c r="LX36" s="4" t="s">
+        <v>1103</v>
+      </c>
+      <c r="LY36" s="4" t="s">
+        <v>1104</v>
+      </c>
+      <c r="MC36" s="4" t="s">
+        <v>1124</v>
+      </c>
+      <c r="ME36" s="4" t="s">
+        <v>1136</v>
+      </c>
+    </row>
+    <row r="37" spans="1:343" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A37" s="4" t="s">
         <v>1137</v>
       </c>
-      <c r="ME36" s="4">
+      <c r="ME37" s="4">
         <v>1</v>
       </c>
     </row>
-    <row r="37" spans="1:343" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A37" s="7" t="s">
+    <row r="38" spans="1:343" s="7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A38" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="AQ37" s="7" t="s">
+      <c r="AQ38" s="7" t="s">
         <v>197</v>
-      </c>
-    </row>
-    <row r="38" spans="1:343" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A38" s="4" t="s">
-        <v>1023</v>
       </c>
     </row>
     <row r="39" spans="1:343" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A39" s="4" t="s">
-        <v>1073</v>
+        <v>1023</v>
       </c>
     </row>
     <row r="40" spans="1:343" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A40" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="AQ40" s="4">
-        <v>200</v>
+        <v>1073</v>
       </c>
     </row>
     <row r="41" spans="1:343" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A41" s="4" t="s">
-        <v>27</v>
-      </c>
-      <c r="AQ41" s="4" t="s">
-        <v>195</v>
-      </c>
-      <c r="JH41" s="4" t="s">
-        <v>861</v>
-      </c>
-      <c r="KN41" s="4" t="s">
-        <v>1074</v>
+        <v>26</v>
+      </c>
+      <c r="AQ41" s="4">
+        <v>200</v>
       </c>
     </row>
     <row r="42" spans="1:343" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A42" s="4" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="AQ42" s="4" t="s">
         <v>195</v>
       </c>
       <c r="JH42" s="4" t="s">
-        <v>857</v>
+        <v>861</v>
       </c>
       <c r="KN42" s="4" t="s">
-        <v>939</v>
+        <v>1074</v>
       </c>
     </row>
     <row r="43" spans="1:343" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A43" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="AQ43" s="4" t="s">
+        <v>195</v>
+      </c>
+      <c r="JH43" s="4" t="s">
+        <v>857</v>
+      </c>
+      <c r="KN43" s="4" t="s">
+        <v>939</v>
+      </c>
+    </row>
+    <row r="44" spans="1:343" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A44" s="4" t="s">
         <v>47</v>
       </c>
-      <c r="JH43" s="4">
+      <c r="JH44" s="4">
         <v>1</v>
       </c>
     </row>
-    <row r="44" spans="1:343" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A44" s="7" t="s">
+    <row r="45" spans="1:343" s="7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A45" s="7" t="s">
         <v>33</v>
       </c>
-      <c r="AQ44" s="7" t="s">
+      <c r="AQ45" s="7" t="s">
         <v>198</v>
-      </c>
-    </row>
-    <row r="45" spans="1:343" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A45" s="4" t="s">
-        <v>1024</v>
       </c>
     </row>
     <row r="46" spans="1:343" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A46" s="4" t="s">
-        <v>1072</v>
+        <v>1024</v>
       </c>
     </row>
     <row r="47" spans="1:343" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A47" s="4" t="s">
-        <v>30</v>
-      </c>
-      <c r="AQ47" s="4">
-        <v>500</v>
+        <v>1072</v>
       </c>
     </row>
     <row r="48" spans="1:343" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A48" s="4" t="s">
-        <v>31</v>
-      </c>
-      <c r="AQ48" s="4" t="s">
-        <v>195</v>
+        <v>30</v>
+      </c>
+      <c r="AQ48" s="4">
+        <v>500</v>
       </c>
     </row>
     <row r="49" spans="1:336" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A49" s="4" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="AQ49" s="4" t="s">
         <v>195</v>
       </c>
     </row>
-    <row r="50" spans="1:336" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A50" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="AM50" s="5" t="s">
-        <v>181</v>
-      </c>
-      <c r="BJ50" s="5" t="s">
-        <v>286</v>
-      </c>
-      <c r="DS50" s="5" t="s">
-        <v>443</v>
-      </c>
-      <c r="FF50" s="5" t="s">
-        <v>443</v>
-      </c>
-      <c r="JU50" s="5" t="s">
-        <v>901</v>
-      </c>
-      <c r="KR50" s="5" t="s">
-        <v>984</v>
-      </c>
-      <c r="LK50" s="5" t="s">
-        <v>181</v>
-      </c>
-      <c r="LN50" s="5" t="s">
-        <v>286</v>
+    <row r="50" spans="1:336" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A50" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="AQ50" s="4" t="s">
+        <v>195</v>
       </c>
     </row>
     <row r="51" spans="1:336" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A51" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="AM51" s="5" t="s">
+        <v>181</v>
+      </c>
+      <c r="BJ51" s="5" t="s">
+        <v>286</v>
+      </c>
+      <c r="DS51" s="5" t="s">
+        <v>443</v>
+      </c>
+      <c r="FF51" s="5" t="s">
+        <v>443</v>
+      </c>
+      <c r="JU51" s="5" t="s">
+        <v>901</v>
+      </c>
+      <c r="KR51" s="5" t="s">
+        <v>984</v>
+      </c>
+      <c r="LK51" s="5" t="s">
+        <v>181</v>
+      </c>
+      <c r="LN51" s="5" t="s">
+        <v>286</v>
+      </c>
+    </row>
+    <row r="52" spans="1:336" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A52" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="AM51" s="5" t="s">
+      <c r="AM52" s="5" t="s">
         <v>932</v>
       </c>
-      <c r="BJ51" s="5">
+      <c r="BJ52" s="5">
         <v>1</v>
       </c>
-      <c r="DS51" s="5">
+      <c r="DS52" s="5">
         <v>1</v>
       </c>
-      <c r="FF51" s="5">
+      <c r="FF52" s="5">
         <v>1</v>
       </c>
-      <c r="JU51" s="5">
+      <c r="JU52" s="5">
         <v>4</v>
       </c>
-      <c r="KR51" s="5" t="s">
+      <c r="KR52" s="5" t="s">
         <v>985</v>
       </c>
-      <c r="LK51" s="5" t="s">
+      <c r="LK52" s="5" t="s">
         <v>932</v>
       </c>
-      <c r="LN51" s="5">
+      <c r="LN52" s="5">
         <v>-1</v>
       </c>
     </row>
-    <row r="52" spans="1:336" s="8" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A52" s="8" t="s">
+    <row r="53" spans="1:336" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A53" s="8" t="s">
         <v>41</v>
       </c>
-      <c r="HR52" s="8" t="s">
+      <c r="HR53" s="8" t="s">
         <v>715</v>
       </c>
-      <c r="JV52" s="8" t="s">
+      <c r="JV53" s="8" t="s">
         <v>715</v>
       </c>
-      <c r="LL52" s="8" t="s">
+      <c r="LL53" s="8" t="s">
         <v>715</v>
       </c>
-      <c r="LN52" s="8" t="s">
+      <c r="LN53" s="8" t="s">
         <v>715</v>
-      </c>
-    </row>
-    <row r="53" spans="1:336" s="6" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A53" s="6" t="s">
-        <v>40</v>
-      </c>
-      <c r="HR53" s="6">
-        <v>1</v>
-      </c>
-      <c r="JV53" s="6">
-        <v>2</v>
-      </c>
-      <c r="LL53" s="6">
-        <v>8</v>
-      </c>
-      <c r="LN53" s="6">
-        <v>0</v>
       </c>
     </row>
     <row r="54" spans="1:336" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A54" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="HR54" s="6">
+        <v>1</v>
+      </c>
+      <c r="JV54" s="6">
+        <v>2</v>
+      </c>
+      <c r="LL54" s="6">
+        <v>8</v>
+      </c>
+      <c r="LN54" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="55" spans="1:336" s="6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A55" s="6" t="s">
         <v>39</v>
       </c>
-      <c r="HR54" s="6" t="s">
+      <c r="HR55" s="6" t="s">
         <v>714</v>
       </c>
-      <c r="JV54" s="6" t="s">
+      <c r="JV55" s="6" t="s">
         <v>904</v>
       </c>
-      <c r="LL54" s="6" t="s">
+      <c r="LL55" s="6" t="s">
         <v>1019</v>
       </c>
-      <c r="LN54" s="6" t="s">
+      <c r="LN55" s="6" t="s">
         <v>1088</v>
       </c>
     </row>
-    <row r="55" spans="1:336" s="8" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A55" s="8" t="s">
+    <row r="56" spans="1:336" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A56" s="8" t="s">
         <v>44</v>
       </c>
-      <c r="HR55" s="8" t="s">
+      <c r="HR56" s="8" t="s">
         <v>715</v>
-      </c>
-    </row>
-    <row r="56" spans="1:336" s="6" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A56" s="6" t="s">
-        <v>43</v>
-      </c>
-      <c r="HR56" s="6">
-        <v>3</v>
       </c>
     </row>
     <row r="57" spans="1:336" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A57" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="HR57" s="6">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="58" spans="1:336" s="6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A58" s="6" t="s">
         <v>42</v>
       </c>
-      <c r="HR57" s="6" t="s">
+      <c r="HR58" s="6" t="s">
         <v>714</v>
-      </c>
-    </row>
-    <row r="58" spans="1:336" x14ac:dyDescent="0.25">
-      <c r="A58" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="JV58" s="1" t="s">
-        <v>905</v>
       </c>
     </row>
     <row r="59" spans="1:336" x14ac:dyDescent="0.25">
       <c r="A59" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="IN59" s="1">
-        <v>6</v>
-      </c>
-      <c r="JR59" s="1">
-        <v>5</v>
-      </c>
-      <c r="KQ59" s="1">
-        <v>3</v>
-      </c>
-      <c r="LE59" s="1">
-        <v>6</v>
-      </c>
-      <c r="LX59" s="1">
-        <v>10</v>
+        <v>49</v>
+      </c>
+      <c r="JV59" s="1" t="s">
+        <v>905</v>
       </c>
     </row>
     <row r="60" spans="1:336" x14ac:dyDescent="0.25">
       <c r="A60" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="IN60" s="1">
+        <v>6</v>
+      </c>
+      <c r="JR60" s="1">
+        <v>5</v>
+      </c>
+      <c r="KQ60" s="1">
+        <v>3</v>
+      </c>
+      <c r="LE60" s="1">
+        <v>6</v>
+      </c>
+      <c r="LX60" s="1">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="61" spans="1:336" x14ac:dyDescent="0.25">
+      <c r="A61" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="IN60" s="1" t="s">
+      <c r="IN61" s="1" t="s">
         <v>791</v>
       </c>
-      <c r="JR60" s="1" t="s">
+      <c r="JR61" s="1" t="s">
         <v>890</v>
       </c>
-      <c r="KQ60" s="1" t="s">
+      <c r="KQ61" s="1" t="s">
         <v>988</v>
       </c>
-      <c r="LE60" s="1" t="s">
+      <c r="LE61" s="1" t="s">
         <v>1075</v>
       </c>
-      <c r="LX60" s="1" t="s">
+      <c r="LX61" s="1" t="s">
         <v>1108</v>
       </c>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A52:KE60">
-    <sortCondition ref="A52:A60"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A53:KE61">
+    <sortCondition ref="A53:A61"/>
   </sortState>
   <conditionalFormatting sqref="LR1:LU1 A1:LP1 MB1 ME1:XFD1">
     <cfRule type="duplicateValues" dxfId="3" priority="4"/>

</xml_diff>

<commit_message>
Implemented tile mode for activities Cleaned up various title headers
</commit_message>
<xml_diff>
--- a/work assets/activities.xlsx
+++ b/work assets/activities.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/eb76e5660c890129/Personal/Projects/Design/PECS/PECS/work assets/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1180" documentId="13_ncr:40009_{E3EB266C-7612-416D-8781-7A2BED99FA57}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{27A8C996-46DA-4284-B539-260B2D65E417}"/>
+  <xr:revisionPtr revIDLastSave="1181" documentId="13_ncr:40009_{E3EB266C-7612-416D-8781-7A2BED99FA57}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{3E953F48-5C1A-4069-B154-F503ECEB9D59}"/>
   <bookViews>
-    <workbookView xWindow="3510" yWindow="3510" windowWidth="57600" windowHeight="15435" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="11970" yWindow="1695" windowWidth="57600" windowHeight="15435" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="activities" sheetId="1" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5737" uniqueCount="1132">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5737" uniqueCount="1133">
   <si>
     <t>name</t>
   </si>
@@ -3556,6 +3556,9 @@
   </si>
   <si>
     <t>cannotTargetCaster</t>
+  </si>
+  <si>
+    <t>minion</t>
   </si>
 </sst>
 </file>
@@ -34908,10 +34911,10 @@
   <dimension ref="A1:LR69"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="FP2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="AS2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="FQ1" sqref="FQ1"/>
+      <selection pane="bottomRight" activeCell="BB22" sqref="BB22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -40609,7 +40612,7 @@
         <v>1097</v>
       </c>
       <c r="BB22" s="1" t="s">
-        <v>1097</v>
+        <v>1132</v>
       </c>
       <c r="BC22" s="1" t="s">
         <v>1101</v>

</xml_diff>